<commit_message>
DB, Share에 UI 추가
</commit_message>
<xml_diff>
--- a/Documents/Aphelios_Database.xlsx
+++ b/Documents/Aphelios_Database.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03ad4a8e8f7310f3/project/GangsterHamster/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{01041995-EAED-4FCF-B70E-09E89BBA756B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C4BAE14-1AB6-4CF4-A923-C49C93A3B76B}"/>
+  <xr:revisionPtr revIDLastSave="322" documentId="13_ncr:1_{01041995-EAED-4FCF-B70E-09E89BBA756B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06F8C97F-E452-4707-95CC-1C685BF874B7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="3" r:id="rId1"/>
     <sheet name="history" sheetId="2" r:id="rId2"/>
     <sheet name="obj" sheetId="1" r:id="rId3"/>
     <sheet name="stage" sheetId="4" r:id="rId4"/>
+    <sheet name="UI" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="222">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1067,53 +1068,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4m x 1m x 4m</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사물이나 생물을 밑에서 
-받쳐주는 바닥</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기본 바닥
-(Floor_Inter_Noraml_01)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1m x 1m x 1m</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구멍이 뚫려 있어 이동이 가능하며
-빛을 낸다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구멍 뚫린 조명
-(Floor_Inter_Normal_02)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">직사각형 조명
-(Floor_Inter_Normal_03)
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>직사각형의 조명으로 밝은 빛을 낸다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>원형 조명
-(Floor_Inter_Normal_04)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>원형의 조명으로 밝은 빛을 낸다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>우주정거장에서 보이는 지구로, 
 플레이어가 있는 곳이 우주라는 것을
 알려주기 위한 장치다.</t>
@@ -1989,6 +1943,302 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ref. UI배치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Title UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나머지 요소를 담는 패널</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 누른 버튼의 기능을 
+플레이어에게 알려주는 텍스트</t>
+  </si>
+  <si>
+    <t>현재 누른 버튼의 기능을 
+플레이어에게 알려주는 텍스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Game UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Choose Chapter UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택 가능한 스테이지의 정보를
+담은 패널</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클릭 시, 활성화된 현재  
+패널을 비활성화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나머지 요소를 담은 패널</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테이지명을 넣을 텍스트박스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테이지의 광경을 
+넣을 이미지박스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테이지에서 진행될 시나리오
+초반 부분을 넣을 텍스트박스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어두운 회색은 남은 스크롤바
+밝은 회색은 스크롤로 
+스크롤은 스크롤바 안에서만 
+상 하로 움직일 수 있으며
+스크롤이 내려가면 다른 
+스테이지들을 볼 수 있음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임의 전체적인 분위기나 컨셉을
+넣을 백그라운드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임의 전체적인 분위기를 로고로
+표현한 이미지박스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클릭 시, "New Game UI"를 
+활성화 시키는 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클릭 시, "Choose Chapter UI"를 
+활성화 시키는 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클릭 시, 게임을 종료하는 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클릭 시, "Option UI"를 활성화 
+시키는 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Option UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>명칭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백그라운드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타이틀로고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>옵션 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>챕터선택 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨티뉴 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뉴 게임 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임 종료 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>텍스트 박스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비활성화 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수락 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상급 패널</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중급 패널</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우측에 있는 스크롤의 기능을 명시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상하스크롤&amp;바</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>좌우스크롤바</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>버튼에 텍스트도 넣어 주세요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+좌 : 클릭 시, 풀스크린모드 전환
+우 : 클릭 시, 창모드 전환</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>버튼에 텍스트도 넣어 주세요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+좌 : 클릭 시, 1920x1080 해상도로 전환
+우 : 클릭 시, 2560x1080 해상도로 전환</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에임포인트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무기아이콘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 사용중인 무기를 나타내는
+무기를 직관적으로 표현한 아이콘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에임포인트가 있는 위치로
+무기가 발사됨.
+A타입 오브젝트에 포인트가
+올라갈 때, 색이 변함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In Game UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클릭 시, 기존의 저장 데이터를
+모두 삭제 후, 게임을 처음부터 
+재시작 후 "In Game UI"를 활성화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>클릭 시, 저장되어 있는 데이터를 
+불러오고, "In Game UI"를 활성화하는 
+버튼(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>첫 실행 시 선택 불가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1998,7 +2248,7 @@
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
     <numFmt numFmtId="177" formatCode="0_ "/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2131,8 +2381,34 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2199,8 +2475,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="42">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -2737,13 +3031,220 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2999,6 +3500,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3107,14 +3617,188 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3151,9 +3835,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9046822</xdr:colOff>
+      <xdr:colOff>9050632</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>2799831</xdr:rowOff>
+      <xdr:rowOff>2803641</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3219,7 +3903,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2378559</xdr:colOff>
+      <xdr:colOff>2382369</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>2323893</xdr:rowOff>
     </xdr:to>
@@ -3341,9 +4025,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>3749991</xdr:colOff>
+      <xdr:colOff>3753801</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>3794481</xdr:rowOff>
+      <xdr:rowOff>3790671</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3402,9 +4086,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4212277</xdr:colOff>
+      <xdr:colOff>4208467</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>2301771</xdr:rowOff>
+      <xdr:rowOff>2305581</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3465,7 +4149,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>8195211</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>3027722</xdr:rowOff>
+      <xdr:rowOff>3031532</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3534,9 +4218,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4516235</xdr:colOff>
+      <xdr:colOff>4512425</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>2495502</xdr:rowOff>
+      <xdr:rowOff>2499312</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3597,7 +4281,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>4537365</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>4935071</xdr:rowOff>
+      <xdr:rowOff>4931261</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3656,9 +4340,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>8936083</xdr:colOff>
+      <xdr:colOff>8932273</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>4933235</xdr:rowOff>
+      <xdr:rowOff>4937045</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3717,7 +4401,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4703386</xdr:colOff>
+      <xdr:colOff>4707196</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>4912179</xdr:rowOff>
     </xdr:to>
@@ -3778,9 +4462,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>8745311</xdr:colOff>
+      <xdr:colOff>8741501</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2568727</xdr:rowOff>
+      <xdr:rowOff>2572537</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3839,9 +4523,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9235440</xdr:colOff>
+      <xdr:colOff>9239250</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>5122346</xdr:rowOff>
+      <xdr:rowOff>5126156</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3900,9 +4584,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>3333750</xdr:colOff>
+      <xdr:colOff>3329940</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>5046617</xdr:rowOff>
+      <xdr:rowOff>5050427</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3961,9 +4645,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9202683</xdr:colOff>
+      <xdr:colOff>9198873</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>4895848</xdr:rowOff>
+      <xdr:rowOff>4899658</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4022,7 +4706,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4704261</xdr:colOff>
+      <xdr:colOff>4708071</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>4342463</xdr:rowOff>
     </xdr:to>
@@ -4083,7 +4767,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>8856073</xdr:colOff>
+      <xdr:colOff>8859883</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>2402839</xdr:rowOff>
     </xdr:to>
@@ -4144,7 +4828,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>8664398</xdr:colOff>
+      <xdr:colOff>8668208</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>5143499</xdr:rowOff>
     </xdr:to>
@@ -4205,7 +4889,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4096616</xdr:colOff>
+      <xdr:colOff>4092806</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>5066645</xdr:rowOff>
     </xdr:to>
@@ -4266,9 +4950,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4477862</xdr:colOff>
+      <xdr:colOff>4474052</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>5007379</xdr:rowOff>
+      <xdr:rowOff>5011189</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4325,9 +5009,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>7104439</xdr:colOff>
+      <xdr:colOff>7108249</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>3718559</xdr:rowOff>
+      <xdr:rowOff>3714749</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4386,9 +5070,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>5541198</xdr:colOff>
+      <xdr:colOff>5545008</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2266949</xdr:rowOff>
+      <xdr:rowOff>2270759</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4449,7 +5133,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>5486400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>4743449</xdr:rowOff>
+      <xdr:rowOff>4747259</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4508,7 +5192,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9352852</xdr:colOff>
+      <xdr:colOff>9356662</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>4724400</xdr:rowOff>
     </xdr:to>
@@ -4569,9 +5253,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>3829253</xdr:colOff>
+      <xdr:colOff>3825443</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>3752850</xdr:rowOff>
+      <xdr:rowOff>3749040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4632,7 +5316,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>8915400</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>3219450</xdr:rowOff>
+      <xdr:rowOff>3215640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4691,9 +5375,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9621736</xdr:colOff>
+      <xdr:colOff>9617926</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>4783455</xdr:rowOff>
+      <xdr:rowOff>4779645</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4752,9 +5436,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>6875984</xdr:colOff>
+      <xdr:colOff>6879794</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>5045054</xdr:rowOff>
+      <xdr:rowOff>5048864</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4796,9 +5480,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9428169</xdr:colOff>
+      <xdr:colOff>9431979</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>4931421</xdr:rowOff>
+      <xdr:rowOff>4935231</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4840,9 +5524,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>8855392</xdr:colOff>
+      <xdr:colOff>8859202</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>4479608</xdr:rowOff>
+      <xdr:rowOff>4475798</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4901,9 +5585,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9661154</xdr:colOff>
+      <xdr:colOff>9657344</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>3445436</xdr:rowOff>
+      <xdr:rowOff>3449246</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4962,7 +5646,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>3791956</xdr:colOff>
+      <xdr:colOff>3788146</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>4343400</xdr:rowOff>
     </xdr:to>
@@ -5086,7 +5770,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>2973014</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>3525375</xdr:rowOff>
+      <xdr:rowOff>3521565</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5145,9 +5829,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9013507</xdr:colOff>
+      <xdr:colOff>9009697</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>3907154</xdr:rowOff>
+      <xdr:rowOff>3903344</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5204,9 +5888,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>3522345</xdr:colOff>
+      <xdr:colOff>3526155</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>2499086</xdr:rowOff>
+      <xdr:rowOff>2495276</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5265,9 +5949,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9581197</xdr:colOff>
+      <xdr:colOff>9585007</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>4897264</xdr:rowOff>
+      <xdr:rowOff>4893454</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5326,9 +6010,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4592002</xdr:colOff>
+      <xdr:colOff>4588192</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>4933673</xdr:rowOff>
+      <xdr:rowOff>4937483</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5387,9 +6071,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>7369493</xdr:colOff>
+      <xdr:colOff>7373303</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>4931147</xdr:rowOff>
+      <xdr:rowOff>4934957</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5448,7 +6132,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9620723</xdr:colOff>
+      <xdr:colOff>9616913</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>2587943</xdr:rowOff>
     </xdr:to>
@@ -5507,9 +6191,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>6270866</xdr:colOff>
+      <xdr:colOff>6267056</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>2264091</xdr:rowOff>
+      <xdr:rowOff>2267901</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5566,7 +6250,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4480321</xdr:colOff>
+      <xdr:colOff>4476511</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>3429001</xdr:rowOff>
     </xdr:to>
@@ -5627,9 +6311,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9731061</xdr:colOff>
+      <xdr:colOff>9734871</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>3182303</xdr:rowOff>
+      <xdr:rowOff>3178493</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5688,9 +6372,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9199244</xdr:colOff>
+      <xdr:colOff>9203054</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1696335</xdr:rowOff>
+      <xdr:rowOff>1692525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5749,9 +6433,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>5694044</xdr:colOff>
+      <xdr:colOff>5697854</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1543050</xdr:rowOff>
+      <xdr:rowOff>1539240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5810,9 +6494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4628198</xdr:colOff>
+      <xdr:colOff>4632008</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>5089208</xdr:rowOff>
+      <xdr:rowOff>5085398</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5871,7 +6555,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4706561</xdr:colOff>
+      <xdr:colOff>4702751</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>2667000</xdr:rowOff>
     </xdr:to>
@@ -5932,9 +6616,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9620934</xdr:colOff>
+      <xdr:colOff>9617124</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>4971097</xdr:rowOff>
+      <xdr:rowOff>4974907</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5993,9 +6677,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9087803</xdr:colOff>
+      <xdr:colOff>9083993</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>5013008</xdr:rowOff>
+      <xdr:rowOff>5009198</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6039,182 +6723,6 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1544002</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>397193</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>7713344</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>4742298</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{422CC5BF-DD2D-469F-91DC-A86B219E00B8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17331690" y="95170943"/>
-          <a:ext cx="6169342" cy="4352725"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1664970</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>571500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>7640002</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>5116351</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED127103-B4D1-402C-BB7D-707A23696D2D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="18929033" y="100536375"/>
-          <a:ext cx="5978842" cy="4542946"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1714499</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>159067</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>7715248</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>5001331</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="그림 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D45DA613-E019-4FA6-AABA-305D09E7E84C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="18978562" y="105315067"/>
-          <a:ext cx="6000749" cy="4842264"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1849755</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>179069</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>7981608</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>4808219</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="그림 25">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEDD900A-2484-49FD-BFB9-DBD4AFEC0B86}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19113818" y="110526194"/>
-          <a:ext cx="6131853" cy="4629150"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -6282,6 +6790,231 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>336666</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>145473</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>398154</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>128648</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B0B0B32-CC8D-4A20-9C34-70E42EEA18F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1001684" y="5008418"/>
+          <a:ext cx="6046652" cy="3405248"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>34514</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>143436</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>764038</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F59E3B8-8C90-4219-BCFA-FBA16C8BB9C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="706867" y="4849907"/>
+          <a:ext cx="6626263" cy="3758250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>397707</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>81498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>443058</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>192968</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65B8BAA1-B695-478B-8F8D-220671990388}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1062725" y="524843"/>
+          <a:ext cx="6030515" cy="3390178"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>358668</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>175557</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="그림 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DEE832F-A1F0-4EED-931A-B847C505553C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="962198" y="14344996"/>
+          <a:ext cx="6046652" cy="3439688"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>343918</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>69272</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>455282</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>173478</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="그림 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A4EB7EB-63A9-4185-8BA6-A01AC8E119B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1008936" y="18343417"/>
+          <a:ext cx="6096528" cy="3429297"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -6633,58 +7366,58 @@
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="2" spans="2:12" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="85"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6714,11 +7447,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
@@ -6765,11 +7498,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" x14ac:dyDescent="0.4"/>
@@ -6944,7 +7677,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>97</v>
@@ -7100,7 +7833,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>33</v>
@@ -7189,60 +7922,52 @@
       <c r="G20" s="38"/>
     </row>
     <row r="21" spans="1:7" ht="409.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="91">
+      <c r="A21" s="94">
         <v>20</v>
       </c>
-      <c r="B21" s="88" t="s">
+      <c r="B21" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="88" t="s">
+      <c r="C21" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="103" t="s">
+      <c r="D21" s="106" t="s">
         <v>112</v>
       </c>
-      <c r="E21" s="100" t="s">
+      <c r="E21" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="F21" s="97" t="s">
+      <c r="F21" s="100" t="s">
         <v>113</v>
       </c>
-      <c r="G21" s="94"/>
+      <c r="G21" s="97"/>
     </row>
     <row r="22" spans="1:7" ht="409.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="92"/>
-      <c r="B22" s="89"/>
-      <c r="C22" s="89"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="98"/>
-      <c r="G22" s="95"/>
+      <c r="A22" s="95"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="107"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="98"/>
     </row>
     <row r="23" spans="1:7" ht="409.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="93"/>
-      <c r="B23" s="90"/>
-      <c r="C23" s="90"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="102"/>
-      <c r="F23" s="99"/>
-      <c r="G23" s="96"/>
+      <c r="A23" s="96"/>
+      <c r="B23" s="93"/>
+      <c r="C23" s="93"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="99"/>
     </row>
     <row r="24" spans="1:7" ht="409.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="68">
         <v>21</v>
       </c>
-      <c r="B24" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="C24" s="67" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" s="72" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="71" t="s">
-        <v>143</v>
-      </c>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="71"/>
       <c r="F24" s="70"/>
       <c r="G24" s="69"/>
     </row>
@@ -7250,18 +7975,10 @@
       <c r="A25" s="68">
         <v>22</v>
       </c>
-      <c r="B25" s="71" t="s">
-        <v>148</v>
-      </c>
-      <c r="C25" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="72" t="s">
-        <v>147</v>
-      </c>
-      <c r="E25" s="71" t="s">
-        <v>146</v>
-      </c>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="71"/>
       <c r="F25" s="70"/>
       <c r="G25" s="69"/>
     </row>
@@ -7269,18 +7986,10 @@
       <c r="A26" s="68">
         <v>23</v>
       </c>
-      <c r="B26" s="71" t="s">
-        <v>149</v>
-      </c>
-      <c r="C26" s="67" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="E26" s="71" t="s">
-        <v>146</v>
-      </c>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="71"/>
       <c r="F26" s="70"/>
       <c r="G26" s="69"/>
     </row>
@@ -7288,65 +7997,31 @@
       <c r="A27" s="68">
         <v>24</v>
       </c>
-      <c r="B27" s="71" t="s">
-        <v>151</v>
-      </c>
-      <c r="C27" s="67" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="E27" s="71" t="s">
-        <v>146</v>
-      </c>
-      <c r="F27" s="70"/>
-      <c r="G27" s="69"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="32"/>
     </row>
     <row r="28" spans="1:7" ht="409.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="68">
         <v>25</v>
       </c>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="69"/>
     </row>
     <row r="29" spans="1:7" ht="409.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="68">
         <v>26</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="69"/>
+      <c r="F29"/>
     </row>
     <row r="30" spans="1:7" ht="409.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="68">
         <v>27</v>
       </c>
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="69"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="28"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="32"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.4">
-      <c r="F33"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -7370,9 +8045,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C8A030F-A691-4A55-8AFD-7F71C677C5D4}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T4" sqref="T4"/>
+      <selection pane="bottomLeft" activeCell="O8" sqref="O8:Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -7399,7 +8074,7 @@
         <v>62</v>
       </c>
       <c r="C1" s="73" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>115</v>
@@ -7407,26 +8082,26 @@
       <c r="E1" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="117" t="s">
+      <c r="F1" s="120" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
       <c r="M1" s="80" t="s">
         <v>75</v>
       </c>
       <c r="N1" s="40" t="s">
-        <v>174</v>
-      </c>
-      <c r="O1" s="118" t="s">
+        <v>164</v>
+      </c>
+      <c r="O1" s="121" t="s">
         <v>70</v>
       </c>
-      <c r="P1" s="118"/>
-      <c r="Q1" s="118"/>
+      <c r="P1" s="121"/>
+      <c r="Q1" s="121"/>
       <c r="R1" s="40" t="s">
         <v>76</v>
       </c>
@@ -7435,7 +8110,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="82.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="117" t="s">
         <v>68</v>
       </c>
       <c r="B2" s="47" t="s">
@@ -7445,34 +8120,34 @@
         <v>93</v>
       </c>
       <c r="D2" s="48" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="E2" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="119" t="s">
+      <c r="F2" s="122" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
       <c r="M2" s="81"/>
-      <c r="N2" s="121" t="s">
-        <v>177</v>
-      </c>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
+      <c r="N2" s="85" t="s">
+        <v>167</v>
+      </c>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
       <c r="R2" s="50"/>
       <c r="S2" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="98.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="115"/>
+      <c r="A3" s="118"/>
       <c r="B3" s="51" t="s">
         <v>52</v>
       </c>
@@ -7480,35 +8155,35 @@
         <v>93</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E3" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="106" t="s">
+      <c r="F3" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
-      <c r="K3" s="106"/>
-      <c r="L3" s="106"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
       <c r="M3" s="82"/>
-      <c r="N3" s="122" t="s">
-        <v>180</v>
-      </c>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
+      <c r="N3" s="86" t="s">
+        <v>170</v>
+      </c>
+      <c r="O3" s="111"/>
+      <c r="P3" s="111"/>
+      <c r="Q3" s="111"/>
       <c r="R3" s="55"/>
       <c r="S3" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="408" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="116" t="s">
-        <v>158</v>
+      <c r="A4" s="119" t="s">
+        <v>148</v>
       </c>
       <c r="B4" s="51" t="s">
         <v>54</v>
@@ -7522,31 +8197,31 @@
       <c r="E4" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="106" t="s">
-        <v>173</v>
-      </c>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="106"/>
-      <c r="L4" s="106"/>
+      <c r="F4" s="109" t="s">
+        <v>163</v>
+      </c>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
       <c r="M4" s="82"/>
       <c r="N4" s="84" t="s">
-        <v>181</v>
-      </c>
-      <c r="O4" s="106" t="s">
-        <v>175</v>
-      </c>
-      <c r="P4" s="106"/>
-      <c r="Q4" s="106"/>
+        <v>171</v>
+      </c>
+      <c r="O4" s="109" t="s">
+        <v>165</v>
+      </c>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="109"/>
       <c r="R4" s="55"/>
       <c r="S4" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="116"/>
+      <c r="A5" s="119"/>
       <c r="B5" s="56" t="s">
         <v>63</v>
       </c>
@@ -7559,27 +8234,27 @@
       <c r="E5" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="106" t="s">
+      <c r="F5" s="109" t="s">
         <v>118</v>
       </c>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="106"/>
-      <c r="L5" s="106"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="109"/>
       <c r="M5" s="82"/>
-      <c r="N5" s="123"/>
-      <c r="O5" s="108"/>
-      <c r="P5" s="108"/>
-      <c r="Q5" s="108"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="111"/>
+      <c r="P5" s="111"/>
+      <c r="Q5" s="111"/>
       <c r="R5" s="55"/>
       <c r="S5" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="116"/>
+      <c r="A6" s="119"/>
       <c r="B6" s="56" t="s">
         <v>119</v>
       </c>
@@ -7592,28 +8267,28 @@
       <c r="E6" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="113" t="s">
+      <c r="F6" s="116" t="s">
         <v>137</v>
       </c>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="106"/>
-      <c r="L6" s="106"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
       <c r="M6" s="82"/>
       <c r="N6" s="54"/>
-      <c r="O6" s="108"/>
-      <c r="P6" s="108"/>
-      <c r="Q6" s="108"/>
+      <c r="O6" s="111"/>
+      <c r="P6" s="111"/>
+      <c r="Q6" s="111"/>
       <c r="R6" s="55"/>
       <c r="S6" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="48.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="111" t="s">
-        <v>159</v>
+      <c r="A7" s="114" t="s">
+        <v>149</v>
       </c>
       <c r="B7" s="51" t="s">
         <v>55</v>
@@ -7627,27 +8302,27 @@
       <c r="E7" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="113" t="s">
-        <v>172</v>
-      </c>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="106"/>
-      <c r="L7" s="106"/>
+      <c r="F7" s="116" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="109"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="109"/>
       <c r="M7" s="82"/>
       <c r="N7" s="54"/>
-      <c r="O7" s="108"/>
-      <c r="P7" s="108"/>
-      <c r="Q7" s="108"/>
+      <c r="O7" s="111"/>
+      <c r="P7" s="111"/>
+      <c r="Q7" s="111"/>
       <c r="R7" s="55"/>
       <c r="S7" s="65" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="111"/>
+      <c r="A8" s="114"/>
       <c r="B8" s="57" t="s">
         <v>64</v>
       </c>
@@ -7660,27 +8335,27 @@
       <c r="E8" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="106" t="s">
+      <c r="F8" s="109" t="s">
         <v>123</v>
       </c>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="106"/>
-      <c r="L8" s="106"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="109"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="109"/>
       <c r="M8" s="82"/>
       <c r="N8" s="54"/>
-      <c r="O8" s="108"/>
-      <c r="P8" s="108"/>
-      <c r="Q8" s="108"/>
+      <c r="O8" s="111"/>
+      <c r="P8" s="111"/>
+      <c r="Q8" s="111"/>
       <c r="R8" s="55"/>
       <c r="S8" s="65" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="111"/>
+      <c r="A9" s="114"/>
       <c r="B9" s="58" t="s">
         <v>65</v>
       </c>
@@ -7693,28 +8368,28 @@
       <c r="E9" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="106" t="s">
+      <c r="F9" s="109" t="s">
         <v>125</v>
       </c>
-      <c r="G9" s="106"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="106"/>
-      <c r="J9" s="106"/>
-      <c r="K9" s="106"/>
-      <c r="L9" s="106"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="109"/>
+      <c r="K9" s="109"/>
+      <c r="L9" s="109"/>
       <c r="M9" s="82"/>
       <c r="N9" s="54"/>
-      <c r="O9" s="108"/>
-      <c r="P9" s="108"/>
-      <c r="Q9" s="108"/>
+      <c r="O9" s="111"/>
+      <c r="P9" s="111"/>
+      <c r="Q9" s="111"/>
       <c r="R9" s="55"/>
       <c r="S9" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="53.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="112" t="s">
-        <v>160</v>
+      <c r="A10" s="115" t="s">
+        <v>150</v>
       </c>
       <c r="B10" s="51" t="s">
         <v>56</v>
@@ -7728,32 +8403,32 @@
       <c r="E10" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="F10" s="113" t="s">
-        <v>165</v>
-      </c>
-      <c r="G10" s="106"/>
-      <c r="H10" s="106"/>
-      <c r="I10" s="106"/>
-      <c r="J10" s="106"/>
-      <c r="K10" s="106"/>
-      <c r="L10" s="106"/>
+      <c r="F10" s="116" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="109"/>
+      <c r="K10" s="109"/>
+      <c r="L10" s="109"/>
       <c r="M10" s="82"/>
       <c r="N10" s="54"/>
-      <c r="O10" s="108"/>
-      <c r="P10" s="108"/>
-      <c r="Q10" s="108"/>
+      <c r="O10" s="111"/>
+      <c r="P10" s="111"/>
+      <c r="Q10" s="111"/>
       <c r="R10" s="55"/>
       <c r="S10" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="112"/>
+      <c r="A11" s="115"/>
       <c r="B11" s="58" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="78" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D11" s="52" t="s">
         <v>127</v>
@@ -7761,32 +8436,32 @@
       <c r="E11" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="113" t="s">
+      <c r="F11" s="116" t="s">
         <v>138</v>
       </c>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="106"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="106"/>
-      <c r="L11" s="106"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="109"/>
+      <c r="K11" s="109"/>
+      <c r="L11" s="109"/>
       <c r="M11" s="82"/>
       <c r="N11" s="54"/>
-      <c r="O11" s="108"/>
-      <c r="P11" s="108"/>
-      <c r="Q11" s="108"/>
+      <c r="O11" s="111"/>
+      <c r="P11" s="111"/>
+      <c r="Q11" s="111"/>
       <c r="R11" s="55"/>
       <c r="S11" s="65" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="112"/>
+      <c r="A12" s="115"/>
       <c r="B12" s="58" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D12" s="52" t="s">
         <v>128</v>
@@ -7794,20 +8469,20 @@
       <c r="E12" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="106" t="s">
+      <c r="F12" s="109" t="s">
         <v>129</v>
       </c>
-      <c r="G12" s="106"/>
-      <c r="H12" s="106"/>
-      <c r="I12" s="106"/>
-      <c r="J12" s="106"/>
-      <c r="K12" s="106"/>
-      <c r="L12" s="106"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="109"/>
+      <c r="K12" s="109"/>
+      <c r="L12" s="109"/>
       <c r="M12" s="82"/>
       <c r="N12" s="54"/>
-      <c r="O12" s="108"/>
-      <c r="P12" s="108"/>
-      <c r="Q12" s="108"/>
+      <c r="O12" s="111"/>
+      <c r="P12" s="111"/>
+      <c r="Q12" s="111"/>
       <c r="R12" s="55"/>
       <c r="S12" s="65" t="s">
         <v>92</v>
@@ -7815,13 +8490,13 @@
     </row>
     <row r="13" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="42" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C13" s="78" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D13" s="52" t="s">
         <v>130</v>
@@ -7829,20 +8504,20 @@
       <c r="E13" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="106" t="s">
+      <c r="F13" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="G13" s="106"/>
-      <c r="H13" s="106"/>
-      <c r="I13" s="106"/>
-      <c r="J13" s="106"/>
-      <c r="K13" s="106"/>
-      <c r="L13" s="106"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="109"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="109"/>
+      <c r="K13" s="109"/>
+      <c r="L13" s="109"/>
       <c r="M13" s="82"/>
       <c r="N13" s="54"/>
-      <c r="O13" s="108"/>
-      <c r="P13" s="108"/>
-      <c r="Q13" s="108"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="111"/>
       <c r="R13" s="55"/>
       <c r="S13" s="65" t="s">
         <v>92</v>
@@ -7850,13 +8525,13 @@
     </row>
     <row r="14" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="43" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>131</v>
@@ -7864,20 +8539,20 @@
       <c r="E14" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="F14" s="106" t="s">
+      <c r="F14" s="109" t="s">
         <v>140</v>
       </c>
-      <c r="G14" s="106"/>
-      <c r="H14" s="106"/>
-      <c r="I14" s="106"/>
-      <c r="J14" s="106"/>
-      <c r="K14" s="106"/>
-      <c r="L14" s="106"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="109"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="109"/>
       <c r="M14" s="82"/>
       <c r="N14" s="54"/>
-      <c r="O14" s="108"/>
-      <c r="P14" s="108"/>
-      <c r="Q14" s="108"/>
+      <c r="O14" s="111"/>
+      <c r="P14" s="111"/>
+      <c r="Q14" s="111"/>
       <c r="R14" s="55"/>
       <c r="S14" s="65" t="s">
         <v>92</v>
@@ -7885,13 +8560,13 @@
     </row>
     <row r="15" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="44" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C15" s="78" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D15" s="52" t="s">
         <v>132</v>
@@ -7899,20 +8574,20 @@
       <c r="E15" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="106" t="s">
+      <c r="F15" s="109" t="s">
         <v>141</v>
       </c>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="106"/>
-      <c r="J15" s="106"/>
-      <c r="K15" s="106"/>
-      <c r="L15" s="106"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="109"/>
+      <c r="K15" s="109"/>
+      <c r="L15" s="109"/>
       <c r="M15" s="82"/>
       <c r="N15" s="54"/>
-      <c r="O15" s="108"/>
-      <c r="P15" s="108"/>
-      <c r="Q15" s="108"/>
+      <c r="O15" s="111"/>
+      <c r="P15" s="111"/>
+      <c r="Q15" s="111"/>
       <c r="R15" s="55"/>
       <c r="S15" s="65" t="s">
         <v>93</v>
@@ -7920,13 +8595,13 @@
     </row>
     <row r="16" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="45" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>133</v>
@@ -7934,20 +8609,20 @@
       <c r="E16" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="106" t="s">
+      <c r="F16" s="109" t="s">
         <v>134</v>
       </c>
-      <c r="G16" s="106"/>
-      <c r="H16" s="106"/>
-      <c r="I16" s="106"/>
-      <c r="J16" s="106"/>
-      <c r="K16" s="106"/>
-      <c r="L16" s="106"/>
+      <c r="G16" s="109"/>
+      <c r="H16" s="109"/>
+      <c r="I16" s="109"/>
+      <c r="J16" s="109"/>
+      <c r="K16" s="109"/>
+      <c r="L16" s="109"/>
       <c r="M16" s="82"/>
       <c r="N16" s="54"/>
-      <c r="O16" s="108"/>
-      <c r="P16" s="108"/>
-      <c r="Q16" s="108"/>
+      <c r="O16" s="111"/>
+      <c r="P16" s="111"/>
+      <c r="Q16" s="111"/>
       <c r="R16" s="55"/>
       <c r="S16" s="65" t="s">
         <v>93</v>
@@ -7958,7 +8633,7 @@
         <v>68</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C17" s="75" t="s">
         <v>93</v>
@@ -7969,20 +8644,20 @@
       <c r="E17" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="106" t="s">
-        <v>178</v>
-      </c>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="106"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="106"/>
+      <c r="F17" s="109" t="s">
+        <v>168</v>
+      </c>
+      <c r="G17" s="109"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="109"/>
+      <c r="J17" s="109"/>
+      <c r="K17" s="109"/>
+      <c r="L17" s="109"/>
       <c r="M17" s="82"/>
       <c r="N17" s="54"/>
-      <c r="O17" s="108"/>
-      <c r="P17" s="108"/>
-      <c r="Q17" s="108"/>
+      <c r="O17" s="111"/>
+      <c r="P17" s="111"/>
+      <c r="Q17" s="111"/>
       <c r="R17" s="55"/>
       <c r="S17" s="65" t="s">
         <v>92</v>
@@ -7993,7 +8668,7 @@
         <v>57</v>
       </c>
       <c r="B18" s="59" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C18" s="79" t="s">
         <v>93</v>
@@ -8004,29 +8679,29 @@
       <c r="E18" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="107" t="s">
-        <v>179</v>
-      </c>
-      <c r="G18" s="107"/>
-      <c r="H18" s="107"/>
-      <c r="I18" s="107"/>
-      <c r="J18" s="107"/>
-      <c r="K18" s="107"/>
-      <c r="L18" s="107"/>
+      <c r="F18" s="110" t="s">
+        <v>169</v>
+      </c>
+      <c r="G18" s="110"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="110"/>
+      <c r="J18" s="110"/>
+      <c r="K18" s="110"/>
+      <c r="L18" s="110"/>
       <c r="M18" s="83"/>
       <c r="N18" s="62"/>
-      <c r="O18" s="110"/>
-      <c r="P18" s="110"/>
-      <c r="Q18" s="110"/>
+      <c r="O18" s="113"/>
+      <c r="P18" s="113"/>
+      <c r="Q18" s="113"/>
       <c r="R18" s="63"/>
       <c r="S18" s="66" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="N19" s="109"/>
-      <c r="O19" s="109"/>
-      <c r="P19" s="109"/>
+      <c r="N19" s="112"/>
+      <c r="O19" s="112"/>
+      <c r="P19" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="41">
@@ -8077,4 +8752,1883 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F74CF53-2F48-46EA-9405-9928E75A2E5F}">
+  <dimension ref="B2:Q90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="12" max="12" width="7.5" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="17" max="17" width="19.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B2" s="125" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="124" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="175" t="s">
+        <v>172</v>
+      </c>
+      <c r="M2" s="176" t="s">
+        <v>195</v>
+      </c>
+      <c r="N2" s="128"/>
+      <c r="O2" s="176" t="s">
+        <v>173</v>
+      </c>
+      <c r="P2" s="126"/>
+      <c r="Q2" s="127"/>
+    </row>
+    <row r="3" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="130"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="168">
+        <v>1</v>
+      </c>
+      <c r="M3" s="169" t="s">
+        <v>196</v>
+      </c>
+      <c r="N3" s="170"/>
+      <c r="O3" s="147" t="s">
+        <v>188</v>
+      </c>
+      <c r="P3" s="142"/>
+      <c r="Q3" s="143"/>
+    </row>
+    <row r="4" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="133"/>
+      <c r="C4" s="134"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
+      <c r="H4" s="134"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="135"/>
+      <c r="L4" s="168"/>
+      <c r="M4" s="171"/>
+      <c r="N4" s="172"/>
+      <c r="O4" s="144"/>
+      <c r="P4" s="145"/>
+      <c r="Q4" s="146"/>
+    </row>
+    <row r="5" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="133"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="135"/>
+      <c r="L5" s="168">
+        <v>2</v>
+      </c>
+      <c r="M5" s="169" t="s">
+        <v>197</v>
+      </c>
+      <c r="N5" s="170"/>
+      <c r="O5" s="147" t="s">
+        <v>189</v>
+      </c>
+      <c r="P5" s="142"/>
+      <c r="Q5" s="143"/>
+    </row>
+    <row r="6" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="133"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="135"/>
+      <c r="L6" s="168"/>
+      <c r="M6" s="171"/>
+      <c r="N6" s="172"/>
+      <c r="O6" s="144"/>
+      <c r="P6" s="145"/>
+      <c r="Q6" s="146"/>
+    </row>
+    <row r="7" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="133"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="134"/>
+      <c r="H7" s="134"/>
+      <c r="I7" s="134"/>
+      <c r="J7" s="134"/>
+      <c r="K7" s="135"/>
+      <c r="L7" s="168">
+        <v>3</v>
+      </c>
+      <c r="M7" s="169" t="s">
+        <v>200</v>
+      </c>
+      <c r="N7" s="170"/>
+      <c r="O7" s="147" t="s">
+        <v>221</v>
+      </c>
+      <c r="P7" s="148"/>
+      <c r="Q7" s="149"/>
+    </row>
+    <row r="8" spans="2:17" ht="30.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="133"/>
+      <c r="C8" s="134"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="134"/>
+      <c r="I8" s="134"/>
+      <c r="J8" s="134"/>
+      <c r="K8" s="135"/>
+      <c r="L8" s="168"/>
+      <c r="M8" s="171"/>
+      <c r="N8" s="172"/>
+      <c r="O8" s="150"/>
+      <c r="P8" s="151"/>
+      <c r="Q8" s="152"/>
+    </row>
+    <row r="9" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="133"/>
+      <c r="C9" s="134"/>
+      <c r="D9" s="134"/>
+      <c r="E9" s="134"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="134"/>
+      <c r="I9" s="134"/>
+      <c r="J9" s="134"/>
+      <c r="K9" s="135"/>
+      <c r="L9" s="168">
+        <v>4</v>
+      </c>
+      <c r="M9" s="169" t="s">
+        <v>201</v>
+      </c>
+      <c r="N9" s="170"/>
+      <c r="O9" s="147" t="s">
+        <v>190</v>
+      </c>
+      <c r="P9" s="142"/>
+      <c r="Q9" s="143"/>
+    </row>
+    <row r="10" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="133"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="134"/>
+      <c r="E10" s="134"/>
+      <c r="F10" s="134"/>
+      <c r="G10" s="134"/>
+      <c r="H10" s="134"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
+      <c r="K10" s="135"/>
+      <c r="L10" s="168"/>
+      <c r="M10" s="171"/>
+      <c r="N10" s="172"/>
+      <c r="O10" s="144"/>
+      <c r="P10" s="145"/>
+      <c r="Q10" s="146"/>
+    </row>
+    <row r="11" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="133"/>
+      <c r="C11" s="134"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="134"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="134"/>
+      <c r="H11" s="134"/>
+      <c r="I11" s="134"/>
+      <c r="J11" s="134"/>
+      <c r="K11" s="135"/>
+      <c r="L11" s="168">
+        <v>5</v>
+      </c>
+      <c r="M11" s="169" t="s">
+        <v>199</v>
+      </c>
+      <c r="N11" s="170"/>
+      <c r="O11" s="147" t="s">
+        <v>191</v>
+      </c>
+      <c r="P11" s="148"/>
+      <c r="Q11" s="149"/>
+    </row>
+    <row r="12" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="133"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="134"/>
+      <c r="F12" s="134"/>
+      <c r="G12" s="134"/>
+      <c r="H12" s="134"/>
+      <c r="I12" s="134"/>
+      <c r="J12" s="134"/>
+      <c r="K12" s="135"/>
+      <c r="L12" s="168"/>
+      <c r="M12" s="171"/>
+      <c r="N12" s="172"/>
+      <c r="O12" s="150"/>
+      <c r="P12" s="151"/>
+      <c r="Q12" s="152"/>
+    </row>
+    <row r="13" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="133"/>
+      <c r="C13" s="134"/>
+      <c r="D13" s="134"/>
+      <c r="E13" s="134"/>
+      <c r="F13" s="134"/>
+      <c r="G13" s="134"/>
+      <c r="H13" s="134"/>
+      <c r="I13" s="134"/>
+      <c r="J13" s="134"/>
+      <c r="K13" s="135"/>
+      <c r="L13" s="168">
+        <v>6</v>
+      </c>
+      <c r="M13" s="169" t="s">
+        <v>198</v>
+      </c>
+      <c r="N13" s="170"/>
+      <c r="O13" s="147" t="s">
+        <v>193</v>
+      </c>
+      <c r="P13" s="148"/>
+      <c r="Q13" s="149"/>
+    </row>
+    <row r="14" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="133"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="134"/>
+      <c r="E14" s="134"/>
+      <c r="F14" s="134"/>
+      <c r="G14" s="134"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="134"/>
+      <c r="J14" s="134"/>
+      <c r="K14" s="135"/>
+      <c r="L14" s="168"/>
+      <c r="M14" s="173"/>
+      <c r="N14" s="174"/>
+      <c r="O14" s="162"/>
+      <c r="P14" s="163"/>
+      <c r="Q14" s="164"/>
+    </row>
+    <row r="15" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="133"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="134"/>
+      <c r="E15" s="134"/>
+      <c r="F15" s="134"/>
+      <c r="G15" s="134"/>
+      <c r="H15" s="134"/>
+      <c r="I15" s="134"/>
+      <c r="J15" s="134"/>
+      <c r="K15" s="135"/>
+      <c r="L15" s="168"/>
+      <c r="M15" s="171"/>
+      <c r="N15" s="172"/>
+      <c r="O15" s="150"/>
+      <c r="P15" s="151"/>
+      <c r="Q15" s="152"/>
+    </row>
+    <row r="16" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="133"/>
+      <c r="C16" s="134"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="134"/>
+      <c r="F16" s="134"/>
+      <c r="G16" s="134"/>
+      <c r="H16" s="134"/>
+      <c r="I16" s="134"/>
+      <c r="J16" s="134"/>
+      <c r="K16" s="135"/>
+      <c r="L16" s="168">
+        <v>7</v>
+      </c>
+      <c r="M16" s="169" t="s">
+        <v>202</v>
+      </c>
+      <c r="N16" s="170"/>
+      <c r="O16" s="141" t="s">
+        <v>192</v>
+      </c>
+      <c r="P16" s="142"/>
+      <c r="Q16" s="143"/>
+    </row>
+    <row r="17" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="133"/>
+      <c r="C17" s="134"/>
+      <c r="D17" s="134"/>
+      <c r="E17" s="134"/>
+      <c r="F17" s="134"/>
+      <c r="G17" s="134"/>
+      <c r="H17" s="134"/>
+      <c r="I17" s="134"/>
+      <c r="J17" s="134"/>
+      <c r="K17" s="135"/>
+      <c r="L17" s="168"/>
+      <c r="M17" s="173"/>
+      <c r="N17" s="174"/>
+      <c r="O17" s="165"/>
+      <c r="P17" s="166"/>
+      <c r="Q17" s="167"/>
+    </row>
+    <row r="18" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="136"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="137"/>
+      <c r="G18" s="137"/>
+      <c r="H18" s="137"/>
+      <c r="I18" s="137"/>
+      <c r="J18" s="137"/>
+      <c r="K18" s="138"/>
+      <c r="L18" s="168"/>
+      <c r="M18" s="171"/>
+      <c r="N18" s="172"/>
+      <c r="O18" s="144"/>
+      <c r="P18" s="145"/>
+      <c r="Q18" s="146"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B20" s="125" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" s="126"/>
+      <c r="D20" s="126"/>
+      <c r="E20" s="126"/>
+      <c r="F20" s="128"/>
+      <c r="G20" s="124" t="s">
+        <v>179</v>
+      </c>
+      <c r="H20" s="124"/>
+      <c r="I20" s="124"/>
+      <c r="J20" s="124"/>
+      <c r="K20" s="129"/>
+      <c r="L20" s="175" t="s">
+        <v>172</v>
+      </c>
+      <c r="M20" s="126" t="s">
+        <v>195</v>
+      </c>
+      <c r="N20" s="128"/>
+      <c r="O20" s="176" t="s">
+        <v>173</v>
+      </c>
+      <c r="P20" s="126"/>
+      <c r="Q20" s="127"/>
+    </row>
+    <row r="21" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="130"/>
+      <c r="C21" s="131"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="131"/>
+      <c r="F21" s="131"/>
+      <c r="G21" s="131"/>
+      <c r="H21" s="131"/>
+      <c r="I21" s="131"/>
+      <c r="J21" s="131"/>
+      <c r="K21" s="132"/>
+      <c r="L21" s="168">
+        <v>1</v>
+      </c>
+      <c r="M21" s="169" t="s">
+        <v>206</v>
+      </c>
+      <c r="N21" s="170"/>
+      <c r="O21" s="139" t="s">
+        <v>183</v>
+      </c>
+      <c r="P21" s="139"/>
+      <c r="Q21" s="139"/>
+    </row>
+    <row r="22" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="133"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="134"/>
+      <c r="E22" s="134"/>
+      <c r="F22" s="134"/>
+      <c r="G22" s="134"/>
+      <c r="H22" s="134"/>
+      <c r="I22" s="134"/>
+      <c r="J22" s="134"/>
+      <c r="K22" s="135"/>
+      <c r="L22" s="168"/>
+      <c r="M22" s="173"/>
+      <c r="N22" s="174"/>
+      <c r="O22" s="139"/>
+      <c r="P22" s="139"/>
+      <c r="Q22" s="139"/>
+    </row>
+    <row r="23" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="133"/>
+      <c r="C23" s="134"/>
+      <c r="D23" s="134"/>
+      <c r="E23" s="134"/>
+      <c r="F23" s="134"/>
+      <c r="G23" s="134"/>
+      <c r="H23" s="134"/>
+      <c r="I23" s="134"/>
+      <c r="J23" s="134"/>
+      <c r="K23" s="135"/>
+      <c r="L23" s="168"/>
+      <c r="M23" s="173"/>
+      <c r="N23" s="174"/>
+      <c r="O23" s="139"/>
+      <c r="P23" s="139"/>
+      <c r="Q23" s="139"/>
+    </row>
+    <row r="24" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="133"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="134"/>
+      <c r="F24" s="134"/>
+      <c r="G24" s="134"/>
+      <c r="H24" s="134"/>
+      <c r="I24" s="134"/>
+      <c r="J24" s="134"/>
+      <c r="K24" s="135"/>
+      <c r="L24" s="168"/>
+      <c r="M24" s="171"/>
+      <c r="N24" s="172"/>
+      <c r="O24" s="139"/>
+      <c r="P24" s="139"/>
+      <c r="Q24" s="139"/>
+    </row>
+    <row r="25" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="133"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134"/>
+      <c r="F25" s="134"/>
+      <c r="G25" s="134"/>
+      <c r="H25" s="134"/>
+      <c r="I25" s="134"/>
+      <c r="J25" s="134"/>
+      <c r="K25" s="135"/>
+      <c r="L25" s="168">
+        <v>2</v>
+      </c>
+      <c r="M25" s="169" t="s">
+        <v>203</v>
+      </c>
+      <c r="N25" s="170"/>
+      <c r="O25" s="140" t="s">
+        <v>177</v>
+      </c>
+      <c r="P25" s="139"/>
+      <c r="Q25" s="139"/>
+    </row>
+    <row r="26" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="133"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="134"/>
+      <c r="F26" s="134"/>
+      <c r="G26" s="134"/>
+      <c r="H26" s="134"/>
+      <c r="I26" s="134"/>
+      <c r="J26" s="134"/>
+      <c r="K26" s="135"/>
+      <c r="L26" s="168"/>
+      <c r="M26" s="173"/>
+      <c r="N26" s="174"/>
+      <c r="O26" s="139"/>
+      <c r="P26" s="139"/>
+      <c r="Q26" s="139"/>
+    </row>
+    <row r="27" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="133"/>
+      <c r="C27" s="134"/>
+      <c r="D27" s="134"/>
+      <c r="E27" s="134"/>
+      <c r="F27" s="134"/>
+      <c r="G27" s="134"/>
+      <c r="H27" s="134"/>
+      <c r="I27" s="134"/>
+      <c r="J27" s="134"/>
+      <c r="K27" s="135"/>
+      <c r="L27" s="168"/>
+      <c r="M27" s="173"/>
+      <c r="N27" s="174"/>
+      <c r="O27" s="139"/>
+      <c r="P27" s="139"/>
+      <c r="Q27" s="139"/>
+    </row>
+    <row r="28" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="133"/>
+      <c r="C28" s="134"/>
+      <c r="D28" s="134"/>
+      <c r="E28" s="134"/>
+      <c r="F28" s="134"/>
+      <c r="G28" s="134"/>
+      <c r="H28" s="134"/>
+      <c r="I28" s="134"/>
+      <c r="J28" s="134"/>
+      <c r="K28" s="135"/>
+      <c r="L28" s="168"/>
+      <c r="M28" s="171"/>
+      <c r="N28" s="172"/>
+      <c r="O28" s="139"/>
+      <c r="P28" s="139"/>
+      <c r="Q28" s="139"/>
+    </row>
+    <row r="29" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="133"/>
+      <c r="C29" s="134"/>
+      <c r="D29" s="134"/>
+      <c r="E29" s="134"/>
+      <c r="F29" s="134"/>
+      <c r="G29" s="134"/>
+      <c r="H29" s="134"/>
+      <c r="I29" s="134"/>
+      <c r="J29" s="134"/>
+      <c r="K29" s="135"/>
+      <c r="L29" s="168">
+        <v>3</v>
+      </c>
+      <c r="M29" s="169" t="s">
+        <v>204</v>
+      </c>
+      <c r="N29" s="170"/>
+      <c r="O29" s="140" t="s">
+        <v>182</v>
+      </c>
+      <c r="P29" s="139"/>
+      <c r="Q29" s="139"/>
+    </row>
+    <row r="30" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="133"/>
+      <c r="C30" s="134"/>
+      <c r="D30" s="134"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="134"/>
+      <c r="G30" s="134"/>
+      <c r="H30" s="134"/>
+      <c r="I30" s="134"/>
+      <c r="J30" s="134"/>
+      <c r="K30" s="135"/>
+      <c r="L30" s="168"/>
+      <c r="M30" s="173"/>
+      <c r="N30" s="174"/>
+      <c r="O30" s="139"/>
+      <c r="P30" s="139"/>
+      <c r="Q30" s="139"/>
+    </row>
+    <row r="31" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="133"/>
+      <c r="C31" s="134"/>
+      <c r="D31" s="134"/>
+      <c r="E31" s="134"/>
+      <c r="F31" s="134"/>
+      <c r="G31" s="134"/>
+      <c r="H31" s="134"/>
+      <c r="I31" s="134"/>
+      <c r="J31" s="134"/>
+      <c r="K31" s="135"/>
+      <c r="L31" s="168"/>
+      <c r="M31" s="173"/>
+      <c r="N31" s="174"/>
+      <c r="O31" s="139"/>
+      <c r="P31" s="139"/>
+      <c r="Q31" s="139"/>
+    </row>
+    <row r="32" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="133"/>
+      <c r="C32" s="134"/>
+      <c r="D32" s="134"/>
+      <c r="E32" s="134"/>
+      <c r="F32" s="134"/>
+      <c r="G32" s="134"/>
+      <c r="H32" s="134"/>
+      <c r="I32" s="134"/>
+      <c r="J32" s="134"/>
+      <c r="K32" s="135"/>
+      <c r="L32" s="168"/>
+      <c r="M32" s="171"/>
+      <c r="N32" s="172"/>
+      <c r="O32" s="139"/>
+      <c r="P32" s="139"/>
+      <c r="Q32" s="139"/>
+    </row>
+    <row r="33" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="133"/>
+      <c r="C33" s="134"/>
+      <c r="D33" s="134"/>
+      <c r="E33" s="134"/>
+      <c r="F33" s="134"/>
+      <c r="G33" s="134"/>
+      <c r="H33" s="134"/>
+      <c r="I33" s="134"/>
+      <c r="J33" s="134"/>
+      <c r="K33" s="135"/>
+      <c r="L33" s="168">
+        <v>4</v>
+      </c>
+      <c r="M33" s="169" t="s">
+        <v>205</v>
+      </c>
+      <c r="N33" s="170"/>
+      <c r="O33" s="140" t="s">
+        <v>220</v>
+      </c>
+      <c r="P33" s="139"/>
+      <c r="Q33" s="139"/>
+    </row>
+    <row r="34" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="133"/>
+      <c r="C34" s="134"/>
+      <c r="D34" s="134"/>
+      <c r="E34" s="134"/>
+      <c r="F34" s="134"/>
+      <c r="G34" s="134"/>
+      <c r="H34" s="134"/>
+      <c r="I34" s="134"/>
+      <c r="J34" s="134"/>
+      <c r="K34" s="135"/>
+      <c r="L34" s="168"/>
+      <c r="M34" s="173"/>
+      <c r="N34" s="174"/>
+      <c r="O34" s="139"/>
+      <c r="P34" s="139"/>
+      <c r="Q34" s="139"/>
+    </row>
+    <row r="35" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B35" s="133"/>
+      <c r="C35" s="134"/>
+      <c r="D35" s="134"/>
+      <c r="E35" s="134"/>
+      <c r="F35" s="134"/>
+      <c r="G35" s="134"/>
+      <c r="H35" s="134"/>
+      <c r="I35" s="134"/>
+      <c r="J35" s="134"/>
+      <c r="K35" s="135"/>
+      <c r="L35" s="168"/>
+      <c r="M35" s="173"/>
+      <c r="N35" s="174"/>
+      <c r="O35" s="139"/>
+      <c r="P35" s="139"/>
+      <c r="Q35" s="139"/>
+    </row>
+    <row r="36" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="136"/>
+      <c r="C36" s="137"/>
+      <c r="D36" s="137"/>
+      <c r="E36" s="137"/>
+      <c r="F36" s="137"/>
+      <c r="G36" s="137"/>
+      <c r="H36" s="137"/>
+      <c r="I36" s="137"/>
+      <c r="J36" s="137"/>
+      <c r="K36" s="138"/>
+      <c r="L36" s="168"/>
+      <c r="M36" s="171"/>
+      <c r="N36" s="172"/>
+      <c r="O36" s="139"/>
+      <c r="P36" s="139"/>
+      <c r="Q36" s="139"/>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B38" s="125" t="s">
+        <v>174</v>
+      </c>
+      <c r="C38" s="126"/>
+      <c r="D38" s="126"/>
+      <c r="E38" s="126"/>
+      <c r="F38" s="128"/>
+      <c r="G38" s="124" t="s">
+        <v>180</v>
+      </c>
+      <c r="H38" s="124"/>
+      <c r="I38" s="124"/>
+      <c r="J38" s="124"/>
+      <c r="K38" s="129"/>
+      <c r="L38" s="175" t="s">
+        <v>172</v>
+      </c>
+      <c r="M38" s="177" t="s">
+        <v>195</v>
+      </c>
+      <c r="N38" s="178"/>
+      <c r="O38" s="128" t="s">
+        <v>173</v>
+      </c>
+      <c r="P38" s="179"/>
+      <c r="Q38" s="177"/>
+    </row>
+    <row r="39" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="130"/>
+      <c r="C39" s="131"/>
+      <c r="D39" s="131"/>
+      <c r="E39" s="131"/>
+      <c r="F39" s="131"/>
+      <c r="G39" s="131"/>
+      <c r="H39" s="131"/>
+      <c r="I39" s="131"/>
+      <c r="J39" s="131"/>
+      <c r="K39" s="132"/>
+      <c r="L39" s="169">
+        <v>1</v>
+      </c>
+      <c r="M39" s="168" t="s">
+        <v>206</v>
+      </c>
+      <c r="N39" s="168"/>
+      <c r="O39" s="142" t="s">
+        <v>176</v>
+      </c>
+      <c r="P39" s="142"/>
+      <c r="Q39" s="143"/>
+    </row>
+    <row r="40" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="133"/>
+      <c r="C40" s="134"/>
+      <c r="D40" s="134"/>
+      <c r="E40" s="134"/>
+      <c r="F40" s="134"/>
+      <c r="G40" s="134"/>
+      <c r="H40" s="134"/>
+      <c r="I40" s="134"/>
+      <c r="J40" s="134"/>
+      <c r="K40" s="135"/>
+      <c r="L40" s="171"/>
+      <c r="M40" s="168"/>
+      <c r="N40" s="168"/>
+      <c r="O40" s="145"/>
+      <c r="P40" s="145"/>
+      <c r="Q40" s="146"/>
+    </row>
+    <row r="41" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="133"/>
+      <c r="C41" s="134"/>
+      <c r="D41" s="134"/>
+      <c r="E41" s="134"/>
+      <c r="F41" s="134"/>
+      <c r="G41" s="134"/>
+      <c r="H41" s="134"/>
+      <c r="I41" s="134"/>
+      <c r="J41" s="134"/>
+      <c r="K41" s="135"/>
+      <c r="L41" s="169">
+        <v>2</v>
+      </c>
+      <c r="M41" s="168" t="s">
+        <v>203</v>
+      </c>
+      <c r="N41" s="168"/>
+      <c r="O41" s="148" t="s">
+        <v>178</v>
+      </c>
+      <c r="P41" s="142"/>
+      <c r="Q41" s="143"/>
+    </row>
+    <row r="42" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="133"/>
+      <c r="C42" s="134"/>
+      <c r="D42" s="134"/>
+      <c r="E42" s="134"/>
+      <c r="F42" s="134"/>
+      <c r="G42" s="134"/>
+      <c r="H42" s="134"/>
+      <c r="I42" s="134"/>
+      <c r="J42" s="134"/>
+      <c r="K42" s="135"/>
+      <c r="L42" s="171"/>
+      <c r="M42" s="168"/>
+      <c r="N42" s="168"/>
+      <c r="O42" s="145"/>
+      <c r="P42" s="145"/>
+      <c r="Q42" s="146"/>
+    </row>
+    <row r="43" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="133"/>
+      <c r="C43" s="134"/>
+      <c r="D43" s="134"/>
+      <c r="E43" s="134"/>
+      <c r="F43" s="134"/>
+      <c r="G43" s="134"/>
+      <c r="H43" s="134"/>
+      <c r="I43" s="134"/>
+      <c r="J43" s="134"/>
+      <c r="K43" s="135"/>
+      <c r="L43" s="169">
+        <v>3</v>
+      </c>
+      <c r="M43" s="168" t="s">
+        <v>204</v>
+      </c>
+      <c r="N43" s="168"/>
+      <c r="O43" s="148" t="s">
+        <v>182</v>
+      </c>
+      <c r="P43" s="148"/>
+      <c r="Q43" s="149"/>
+    </row>
+    <row r="44" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B44" s="133"/>
+      <c r="C44" s="134"/>
+      <c r="D44" s="134"/>
+      <c r="E44" s="134"/>
+      <c r="F44" s="134"/>
+      <c r="G44" s="134"/>
+      <c r="H44" s="134"/>
+      <c r="I44" s="134"/>
+      <c r="J44" s="134"/>
+      <c r="K44" s="135"/>
+      <c r="L44" s="171"/>
+      <c r="M44" s="168"/>
+      <c r="N44" s="168"/>
+      <c r="O44" s="151"/>
+      <c r="P44" s="151"/>
+      <c r="Q44" s="152"/>
+    </row>
+    <row r="45" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="133"/>
+      <c r="C45" s="134"/>
+      <c r="D45" s="134"/>
+      <c r="E45" s="134"/>
+      <c r="F45" s="134"/>
+      <c r="G45" s="134"/>
+      <c r="H45" s="134"/>
+      <c r="I45" s="134"/>
+      <c r="J45" s="134"/>
+      <c r="K45" s="135"/>
+      <c r="L45" s="169">
+        <v>4</v>
+      </c>
+      <c r="M45" s="168" t="s">
+        <v>207</v>
+      </c>
+      <c r="N45" s="168"/>
+      <c r="O45" s="148" t="s">
+        <v>181</v>
+      </c>
+      <c r="P45" s="142"/>
+      <c r="Q45" s="143"/>
+    </row>
+    <row r="46" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="133"/>
+      <c r="C46" s="134"/>
+      <c r="D46" s="134"/>
+      <c r="E46" s="134"/>
+      <c r="F46" s="134"/>
+      <c r="G46" s="134"/>
+      <c r="H46" s="134"/>
+      <c r="I46" s="134"/>
+      <c r="J46" s="134"/>
+      <c r="K46" s="135"/>
+      <c r="L46" s="171"/>
+      <c r="M46" s="168"/>
+      <c r="N46" s="168"/>
+      <c r="O46" s="145"/>
+      <c r="P46" s="145"/>
+      <c r="Q46" s="146"/>
+    </row>
+    <row r="47" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="133"/>
+      <c r="C47" s="134"/>
+      <c r="D47" s="134"/>
+      <c r="E47" s="134"/>
+      <c r="F47" s="134"/>
+      <c r="G47" s="134"/>
+      <c r="H47" s="134"/>
+      <c r="I47" s="134"/>
+      <c r="J47" s="134"/>
+      <c r="K47" s="135"/>
+      <c r="L47" s="169">
+        <v>5</v>
+      </c>
+      <c r="M47" s="168" t="s">
+        <v>203</v>
+      </c>
+      <c r="N47" s="168"/>
+      <c r="O47" s="142" t="s">
+        <v>184</v>
+      </c>
+      <c r="P47" s="142"/>
+      <c r="Q47" s="143"/>
+    </row>
+    <row r="48" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B48" s="133"/>
+      <c r="C48" s="134"/>
+      <c r="D48" s="134"/>
+      <c r="E48" s="134"/>
+      <c r="F48" s="134"/>
+      <c r="G48" s="134"/>
+      <c r="H48" s="134"/>
+      <c r="I48" s="134"/>
+      <c r="J48" s="134"/>
+      <c r="K48" s="135"/>
+      <c r="L48" s="171"/>
+      <c r="M48" s="168"/>
+      <c r="N48" s="168"/>
+      <c r="O48" s="145"/>
+      <c r="P48" s="145"/>
+      <c r="Q48" s="146"/>
+    </row>
+    <row r="49" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B49" s="133"/>
+      <c r="C49" s="134"/>
+      <c r="D49" s="134"/>
+      <c r="E49" s="134"/>
+      <c r="F49" s="134"/>
+      <c r="G49" s="134"/>
+      <c r="H49" s="134"/>
+      <c r="I49" s="134"/>
+      <c r="J49" s="134"/>
+      <c r="K49" s="135"/>
+      <c r="L49" s="169">
+        <v>6</v>
+      </c>
+      <c r="M49" s="168" t="s">
+        <v>203</v>
+      </c>
+      <c r="N49" s="168"/>
+      <c r="O49" s="148" t="s">
+        <v>186</v>
+      </c>
+      <c r="P49" s="142"/>
+      <c r="Q49" s="143"/>
+    </row>
+    <row r="50" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B50" s="133"/>
+      <c r="C50" s="134"/>
+      <c r="D50" s="134"/>
+      <c r="E50" s="134"/>
+      <c r="F50" s="134"/>
+      <c r="G50" s="134"/>
+      <c r="H50" s="134"/>
+      <c r="I50" s="134"/>
+      <c r="J50" s="134"/>
+      <c r="K50" s="135"/>
+      <c r="L50" s="171"/>
+      <c r="M50" s="168"/>
+      <c r="N50" s="168"/>
+      <c r="O50" s="145"/>
+      <c r="P50" s="145"/>
+      <c r="Q50" s="146"/>
+    </row>
+    <row r="51" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B51" s="133"/>
+      <c r="C51" s="134"/>
+      <c r="D51" s="134"/>
+      <c r="E51" s="134"/>
+      <c r="F51" s="134"/>
+      <c r="G51" s="134"/>
+      <c r="H51" s="134"/>
+      <c r="I51" s="134"/>
+      <c r="J51" s="134"/>
+      <c r="K51" s="135"/>
+      <c r="L51" s="169">
+        <v>7</v>
+      </c>
+      <c r="M51" s="168" t="s">
+        <v>208</v>
+      </c>
+      <c r="N51" s="168"/>
+      <c r="O51" s="148" t="s">
+        <v>185</v>
+      </c>
+      <c r="P51" s="148"/>
+      <c r="Q51" s="149"/>
+    </row>
+    <row r="52" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B52" s="133"/>
+      <c r="C52" s="134"/>
+      <c r="D52" s="134"/>
+      <c r="E52" s="134"/>
+      <c r="F52" s="134"/>
+      <c r="G52" s="134"/>
+      <c r="H52" s="134"/>
+      <c r="I52" s="134"/>
+      <c r="J52" s="134"/>
+      <c r="K52" s="135"/>
+      <c r="L52" s="171"/>
+      <c r="M52" s="168"/>
+      <c r="N52" s="168"/>
+      <c r="O52" s="151"/>
+      <c r="P52" s="151"/>
+      <c r="Q52" s="152"/>
+    </row>
+    <row r="53" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="133"/>
+      <c r="C53" s="134"/>
+      <c r="D53" s="134"/>
+      <c r="E53" s="134"/>
+      <c r="F53" s="134"/>
+      <c r="G53" s="134"/>
+      <c r="H53" s="134"/>
+      <c r="I53" s="134"/>
+      <c r="J53" s="134"/>
+      <c r="K53" s="135"/>
+      <c r="L53" s="169">
+        <v>8</v>
+      </c>
+      <c r="M53" s="168" t="s">
+        <v>210</v>
+      </c>
+      <c r="N53" s="168"/>
+      <c r="O53" s="148" t="s">
+        <v>187</v>
+      </c>
+      <c r="P53" s="142"/>
+      <c r="Q53" s="143"/>
+    </row>
+    <row r="54" spans="2:17" ht="99.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B54" s="136"/>
+      <c r="C54" s="137"/>
+      <c r="D54" s="137"/>
+      <c r="E54" s="137"/>
+      <c r="F54" s="137"/>
+      <c r="G54" s="137"/>
+      <c r="H54" s="137"/>
+      <c r="I54" s="137"/>
+      <c r="J54" s="137"/>
+      <c r="K54" s="138"/>
+      <c r="L54" s="171"/>
+      <c r="M54" s="168"/>
+      <c r="N54" s="168"/>
+      <c r="O54" s="145"/>
+      <c r="P54" s="145"/>
+      <c r="Q54" s="146"/>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B56" s="125" t="s">
+        <v>174</v>
+      </c>
+      <c r="C56" s="126"/>
+      <c r="D56" s="126"/>
+      <c r="E56" s="126"/>
+      <c r="F56" s="128"/>
+      <c r="G56" s="124" t="s">
+        <v>194</v>
+      </c>
+      <c r="H56" s="124"/>
+      <c r="I56" s="124"/>
+      <c r="J56" s="124"/>
+      <c r="K56" s="129"/>
+      <c r="L56" s="180" t="s">
+        <v>172</v>
+      </c>
+      <c r="M56" s="176" t="s">
+        <v>195</v>
+      </c>
+      <c r="N56" s="128"/>
+      <c r="O56" s="179" t="s">
+        <v>173</v>
+      </c>
+      <c r="P56" s="179"/>
+      <c r="Q56" s="177"/>
+    </row>
+    <row r="57" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B57" s="130"/>
+      <c r="C57" s="131"/>
+      <c r="D57" s="131"/>
+      <c r="E57" s="131"/>
+      <c r="F57" s="131"/>
+      <c r="G57" s="131"/>
+      <c r="H57" s="131"/>
+      <c r="I57" s="131"/>
+      <c r="J57" s="131"/>
+      <c r="K57" s="132"/>
+      <c r="L57" s="168">
+        <v>1</v>
+      </c>
+      <c r="M57" s="169" t="s">
+        <v>206</v>
+      </c>
+      <c r="N57" s="170"/>
+      <c r="O57" s="147" t="s">
+        <v>176</v>
+      </c>
+      <c r="P57" s="142"/>
+      <c r="Q57" s="143"/>
+    </row>
+    <row r="58" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B58" s="133"/>
+      <c r="C58" s="134"/>
+      <c r="D58" s="134"/>
+      <c r="E58" s="134"/>
+      <c r="F58" s="134"/>
+      <c r="G58" s="134"/>
+      <c r="H58" s="134"/>
+      <c r="I58" s="134"/>
+      <c r="J58" s="134"/>
+      <c r="K58" s="135"/>
+      <c r="L58" s="168"/>
+      <c r="M58" s="171"/>
+      <c r="N58" s="172"/>
+      <c r="O58" s="144"/>
+      <c r="P58" s="145"/>
+      <c r="Q58" s="146"/>
+    </row>
+    <row r="59" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B59" s="133"/>
+      <c r="C59" s="134"/>
+      <c r="D59" s="134"/>
+      <c r="E59" s="134"/>
+      <c r="F59" s="134"/>
+      <c r="G59" s="134"/>
+      <c r="H59" s="134"/>
+      <c r="I59" s="134"/>
+      <c r="J59" s="134"/>
+      <c r="K59" s="135"/>
+      <c r="L59" s="168">
+        <v>2</v>
+      </c>
+      <c r="M59" s="169" t="s">
+        <v>204</v>
+      </c>
+      <c r="N59" s="170"/>
+      <c r="O59" s="147" t="s">
+        <v>189</v>
+      </c>
+      <c r="P59" s="142"/>
+      <c r="Q59" s="143"/>
+    </row>
+    <row r="60" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B60" s="133"/>
+      <c r="C60" s="134"/>
+      <c r="D60" s="134"/>
+      <c r="E60" s="134"/>
+      <c r="F60" s="134"/>
+      <c r="G60" s="134"/>
+      <c r="H60" s="134"/>
+      <c r="I60" s="134"/>
+      <c r="J60" s="134"/>
+      <c r="K60" s="135"/>
+      <c r="L60" s="168"/>
+      <c r="M60" s="171"/>
+      <c r="N60" s="172"/>
+      <c r="O60" s="144"/>
+      <c r="P60" s="145"/>
+      <c r="Q60" s="146"/>
+    </row>
+    <row r="61" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B61" s="133"/>
+      <c r="C61" s="134"/>
+      <c r="D61" s="134"/>
+      <c r="E61" s="134"/>
+      <c r="F61" s="134"/>
+      <c r="G61" s="134"/>
+      <c r="H61" s="134"/>
+      <c r="I61" s="134"/>
+      <c r="J61" s="134"/>
+      <c r="K61" s="135"/>
+      <c r="L61" s="168">
+        <v>3</v>
+      </c>
+      <c r="M61" s="169" t="s">
+        <v>203</v>
+      </c>
+      <c r="N61" s="170"/>
+      <c r="O61" s="147" t="s">
+        <v>209</v>
+      </c>
+      <c r="P61" s="148"/>
+      <c r="Q61" s="149"/>
+    </row>
+    <row r="62" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B62" s="133"/>
+      <c r="C62" s="134"/>
+      <c r="D62" s="134"/>
+      <c r="E62" s="134"/>
+      <c r="F62" s="134"/>
+      <c r="G62" s="134"/>
+      <c r="H62" s="134"/>
+      <c r="I62" s="134"/>
+      <c r="J62" s="134"/>
+      <c r="K62" s="135"/>
+      <c r="L62" s="168"/>
+      <c r="M62" s="171"/>
+      <c r="N62" s="172"/>
+      <c r="O62" s="150"/>
+      <c r="P62" s="151"/>
+      <c r="Q62" s="152"/>
+    </row>
+    <row r="63" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B63" s="133"/>
+      <c r="C63" s="134"/>
+      <c r="D63" s="134"/>
+      <c r="E63" s="134"/>
+      <c r="F63" s="134"/>
+      <c r="G63" s="134"/>
+      <c r="H63" s="134"/>
+      <c r="I63" s="134"/>
+      <c r="J63" s="134"/>
+      <c r="K63" s="135"/>
+      <c r="L63" s="168">
+        <v>4</v>
+      </c>
+      <c r="M63" s="169"/>
+      <c r="N63" s="170"/>
+      <c r="O63" s="147" t="s">
+        <v>190</v>
+      </c>
+      <c r="P63" s="142"/>
+      <c r="Q63" s="143"/>
+    </row>
+    <row r="64" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B64" s="133"/>
+      <c r="C64" s="134"/>
+      <c r="D64" s="134"/>
+      <c r="E64" s="134"/>
+      <c r="F64" s="134"/>
+      <c r="G64" s="134"/>
+      <c r="H64" s="134"/>
+      <c r="I64" s="134"/>
+      <c r="J64" s="134"/>
+      <c r="K64" s="135"/>
+      <c r="L64" s="168"/>
+      <c r="M64" s="171"/>
+      <c r="N64" s="172"/>
+      <c r="O64" s="144"/>
+      <c r="P64" s="145"/>
+      <c r="Q64" s="146"/>
+    </row>
+    <row r="65" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B65" s="133"/>
+      <c r="C65" s="134"/>
+      <c r="D65" s="134"/>
+      <c r="E65" s="134"/>
+      <c r="F65" s="134"/>
+      <c r="G65" s="134"/>
+      <c r="H65" s="134"/>
+      <c r="I65" s="134"/>
+      <c r="J65" s="134"/>
+      <c r="K65" s="135"/>
+      <c r="L65" s="168">
+        <v>5</v>
+      </c>
+      <c r="M65" s="169" t="s">
+        <v>211</v>
+      </c>
+      <c r="N65" s="170"/>
+      <c r="O65" s="147" t="s">
+        <v>191</v>
+      </c>
+      <c r="P65" s="148"/>
+      <c r="Q65" s="149"/>
+    </row>
+    <row r="66" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B66" s="133"/>
+      <c r="C66" s="134"/>
+      <c r="D66" s="134"/>
+      <c r="E66" s="134"/>
+      <c r="F66" s="134"/>
+      <c r="G66" s="134"/>
+      <c r="H66" s="134"/>
+      <c r="I66" s="134"/>
+      <c r="J66" s="134"/>
+      <c r="K66" s="135"/>
+      <c r="L66" s="168"/>
+      <c r="M66" s="171"/>
+      <c r="N66" s="172"/>
+      <c r="O66" s="150"/>
+      <c r="P66" s="151"/>
+      <c r="Q66" s="152"/>
+    </row>
+    <row r="67" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B67" s="133"/>
+      <c r="C67" s="134"/>
+      <c r="D67" s="134"/>
+      <c r="E67" s="134"/>
+      <c r="F67" s="134"/>
+      <c r="G67" s="134"/>
+      <c r="H67" s="134"/>
+      <c r="I67" s="134"/>
+      <c r="J67" s="134"/>
+      <c r="K67" s="135"/>
+      <c r="L67" s="168">
+        <v>6</v>
+      </c>
+      <c r="M67" s="169" t="s">
+        <v>212</v>
+      </c>
+      <c r="N67" s="170"/>
+      <c r="O67" s="181" t="s">
+        <v>213</v>
+      </c>
+      <c r="P67" s="148"/>
+      <c r="Q67" s="149"/>
+    </row>
+    <row r="68" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B68" s="133"/>
+      <c r="C68" s="134"/>
+      <c r="D68" s="134"/>
+      <c r="E68" s="134"/>
+      <c r="F68" s="134"/>
+      <c r="G68" s="134"/>
+      <c r="H68" s="134"/>
+      <c r="I68" s="134"/>
+      <c r="J68" s="134"/>
+      <c r="K68" s="135"/>
+      <c r="L68" s="168"/>
+      <c r="M68" s="173"/>
+      <c r="N68" s="174"/>
+      <c r="O68" s="162"/>
+      <c r="P68" s="163"/>
+      <c r="Q68" s="164"/>
+    </row>
+    <row r="69" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B69" s="133"/>
+      <c r="C69" s="134"/>
+      <c r="D69" s="134"/>
+      <c r="E69" s="134"/>
+      <c r="F69" s="134"/>
+      <c r="G69" s="134"/>
+      <c r="H69" s="134"/>
+      <c r="I69" s="134"/>
+      <c r="J69" s="134"/>
+      <c r="K69" s="135"/>
+      <c r="L69" s="168"/>
+      <c r="M69" s="171"/>
+      <c r="N69" s="172"/>
+      <c r="O69" s="150"/>
+      <c r="P69" s="151"/>
+      <c r="Q69" s="152"/>
+    </row>
+    <row r="70" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B70" s="133"/>
+      <c r="C70" s="134"/>
+      <c r="D70" s="134"/>
+      <c r="E70" s="134"/>
+      <c r="F70" s="134"/>
+      <c r="G70" s="134"/>
+      <c r="H70" s="134"/>
+      <c r="I70" s="134"/>
+      <c r="J70" s="134"/>
+      <c r="K70" s="135"/>
+      <c r="L70" s="168">
+        <v>7</v>
+      </c>
+      <c r="M70" s="169" t="s">
+        <v>212</v>
+      </c>
+      <c r="N70" s="170"/>
+      <c r="O70" s="181" t="s">
+        <v>214</v>
+      </c>
+      <c r="P70" s="142"/>
+      <c r="Q70" s="143"/>
+    </row>
+    <row r="71" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B71" s="133"/>
+      <c r="C71" s="134"/>
+      <c r="D71" s="134"/>
+      <c r="E71" s="134"/>
+      <c r="F71" s="134"/>
+      <c r="G71" s="134"/>
+      <c r="H71" s="134"/>
+      <c r="I71" s="134"/>
+      <c r="J71" s="134"/>
+      <c r="K71" s="135"/>
+      <c r="L71" s="168"/>
+      <c r="M71" s="173"/>
+      <c r="N71" s="174"/>
+      <c r="O71" s="165"/>
+      <c r="P71" s="166"/>
+      <c r="Q71" s="167"/>
+    </row>
+    <row r="72" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B72" s="136"/>
+      <c r="C72" s="137"/>
+      <c r="D72" s="137"/>
+      <c r="E72" s="137"/>
+      <c r="F72" s="137"/>
+      <c r="G72" s="137"/>
+      <c r="H72" s="137"/>
+      <c r="I72" s="137"/>
+      <c r="J72" s="137"/>
+      <c r="K72" s="138"/>
+      <c r="L72" s="168"/>
+      <c r="M72" s="171"/>
+      <c r="N72" s="172"/>
+      <c r="O72" s="144"/>
+      <c r="P72" s="145"/>
+      <c r="Q72" s="146"/>
+    </row>
+    <row r="74" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B74" s="125" t="s">
+        <v>174</v>
+      </c>
+      <c r="C74" s="126"/>
+      <c r="D74" s="126"/>
+      <c r="E74" s="126"/>
+      <c r="F74" s="128"/>
+      <c r="G74" s="124" t="s">
+        <v>219</v>
+      </c>
+      <c r="H74" s="124"/>
+      <c r="I74" s="124"/>
+      <c r="J74" s="124"/>
+      <c r="K74" s="129"/>
+      <c r="L74" s="180" t="s">
+        <v>172</v>
+      </c>
+      <c r="M74" s="176" t="s">
+        <v>195</v>
+      </c>
+      <c r="N74" s="128"/>
+      <c r="O74" s="179" t="s">
+        <v>173</v>
+      </c>
+      <c r="P74" s="179"/>
+      <c r="Q74" s="177"/>
+    </row>
+    <row r="75" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B75" s="130"/>
+      <c r="C75" s="131"/>
+      <c r="D75" s="131"/>
+      <c r="E75" s="131"/>
+      <c r="F75" s="131"/>
+      <c r="G75" s="131"/>
+      <c r="H75" s="131"/>
+      <c r="I75" s="131"/>
+      <c r="J75" s="131"/>
+      <c r="K75" s="132"/>
+      <c r="L75" s="182">
+        <v>1</v>
+      </c>
+      <c r="M75" s="169" t="s">
+        <v>215</v>
+      </c>
+      <c r="N75" s="170"/>
+      <c r="O75" s="153" t="s">
+        <v>218</v>
+      </c>
+      <c r="P75" s="154"/>
+      <c r="Q75" s="155"/>
+    </row>
+    <row r="76" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B76" s="133"/>
+      <c r="C76" s="134"/>
+      <c r="D76" s="134"/>
+      <c r="E76" s="134"/>
+      <c r="F76" s="134"/>
+      <c r="G76" s="134"/>
+      <c r="H76" s="134"/>
+      <c r="I76" s="134"/>
+      <c r="J76" s="134"/>
+      <c r="K76" s="135"/>
+      <c r="L76" s="183"/>
+      <c r="M76" s="173"/>
+      <c r="N76" s="174"/>
+      <c r="O76" s="159"/>
+      <c r="P76" s="160"/>
+      <c r="Q76" s="161"/>
+    </row>
+    <row r="77" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B77" s="133"/>
+      <c r="C77" s="134"/>
+      <c r="D77" s="134"/>
+      <c r="E77" s="134"/>
+      <c r="F77" s="134"/>
+      <c r="G77" s="134"/>
+      <c r="H77" s="134"/>
+      <c r="I77" s="134"/>
+      <c r="J77" s="134"/>
+      <c r="K77" s="135"/>
+      <c r="L77" s="183"/>
+      <c r="M77" s="173"/>
+      <c r="N77" s="174"/>
+      <c r="O77" s="159"/>
+      <c r="P77" s="160"/>
+      <c r="Q77" s="161"/>
+    </row>
+    <row r="78" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B78" s="133"/>
+      <c r="C78" s="134"/>
+      <c r="D78" s="134"/>
+      <c r="E78" s="134"/>
+      <c r="F78" s="134"/>
+      <c r="G78" s="134"/>
+      <c r="H78" s="134"/>
+      <c r="I78" s="134"/>
+      <c r="J78" s="134"/>
+      <c r="K78" s="135"/>
+      <c r="L78" s="183"/>
+      <c r="M78" s="173"/>
+      <c r="N78" s="174"/>
+      <c r="O78" s="159"/>
+      <c r="P78" s="160"/>
+      <c r="Q78" s="161"/>
+    </row>
+    <row r="79" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B79" s="133"/>
+      <c r="C79" s="134"/>
+      <c r="D79" s="134"/>
+      <c r="E79" s="134"/>
+      <c r="F79" s="134"/>
+      <c r="G79" s="134"/>
+      <c r="H79" s="134"/>
+      <c r="I79" s="134"/>
+      <c r="J79" s="134"/>
+      <c r="K79" s="135"/>
+      <c r="L79" s="183"/>
+      <c r="M79" s="173"/>
+      <c r="N79" s="174"/>
+      <c r="O79" s="159"/>
+      <c r="P79" s="160"/>
+      <c r="Q79" s="161"/>
+    </row>
+    <row r="80" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B80" s="133"/>
+      <c r="C80" s="134"/>
+      <c r="D80" s="134"/>
+      <c r="E80" s="134"/>
+      <c r="F80" s="134"/>
+      <c r="G80" s="134"/>
+      <c r="H80" s="134"/>
+      <c r="I80" s="134"/>
+      <c r="J80" s="134"/>
+      <c r="K80" s="135"/>
+      <c r="L80" s="183"/>
+      <c r="M80" s="173"/>
+      <c r="N80" s="174"/>
+      <c r="O80" s="159"/>
+      <c r="P80" s="160"/>
+      <c r="Q80" s="161"/>
+    </row>
+    <row r="81" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B81" s="133"/>
+      <c r="C81" s="134"/>
+      <c r="D81" s="134"/>
+      <c r="E81" s="134"/>
+      <c r="F81" s="134"/>
+      <c r="G81" s="134"/>
+      <c r="H81" s="134"/>
+      <c r="I81" s="134"/>
+      <c r="J81" s="134"/>
+      <c r="K81" s="135"/>
+      <c r="L81" s="183"/>
+      <c r="M81" s="173"/>
+      <c r="N81" s="174"/>
+      <c r="O81" s="159"/>
+      <c r="P81" s="160"/>
+      <c r="Q81" s="161"/>
+    </row>
+    <row r="82" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B82" s="133"/>
+      <c r="C82" s="134"/>
+      <c r="D82" s="134"/>
+      <c r="E82" s="134"/>
+      <c r="F82" s="134"/>
+      <c r="G82" s="134"/>
+      <c r="H82" s="134"/>
+      <c r="I82" s="134"/>
+      <c r="J82" s="134"/>
+      <c r="K82" s="135"/>
+      <c r="L82" s="184"/>
+      <c r="M82" s="171"/>
+      <c r="N82" s="172"/>
+      <c r="O82" s="156"/>
+      <c r="P82" s="157"/>
+      <c r="Q82" s="158"/>
+    </row>
+    <row r="83" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B83" s="133"/>
+      <c r="C83" s="134"/>
+      <c r="D83" s="134"/>
+      <c r="E83" s="134"/>
+      <c r="F83" s="134"/>
+      <c r="G83" s="134"/>
+      <c r="H83" s="134"/>
+      <c r="I83" s="134"/>
+      <c r="J83" s="134"/>
+      <c r="K83" s="135"/>
+      <c r="L83" s="182">
+        <v>2</v>
+      </c>
+      <c r="M83" s="169" t="s">
+        <v>216</v>
+      </c>
+      <c r="N83" s="170"/>
+      <c r="O83" s="153" t="s">
+        <v>217</v>
+      </c>
+      <c r="P83" s="154"/>
+      <c r="Q83" s="155"/>
+    </row>
+    <row r="84" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B84" s="133"/>
+      <c r="C84" s="134"/>
+      <c r="D84" s="134"/>
+      <c r="E84" s="134"/>
+      <c r="F84" s="134"/>
+      <c r="G84" s="134"/>
+      <c r="H84" s="134"/>
+      <c r="I84" s="134"/>
+      <c r="J84" s="134"/>
+      <c r="K84" s="135"/>
+      <c r="L84" s="183"/>
+      <c r="M84" s="173"/>
+      <c r="N84" s="174"/>
+      <c r="O84" s="159"/>
+      <c r="P84" s="160"/>
+      <c r="Q84" s="161"/>
+    </row>
+    <row r="85" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B85" s="133"/>
+      <c r="C85" s="134"/>
+      <c r="D85" s="134"/>
+      <c r="E85" s="134"/>
+      <c r="F85" s="134"/>
+      <c r="G85" s="134"/>
+      <c r="H85" s="134"/>
+      <c r="I85" s="134"/>
+      <c r="J85" s="134"/>
+      <c r="K85" s="135"/>
+      <c r="L85" s="183"/>
+      <c r="M85" s="173"/>
+      <c r="N85" s="174"/>
+      <c r="O85" s="159"/>
+      <c r="P85" s="160"/>
+      <c r="Q85" s="161"/>
+    </row>
+    <row r="86" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B86" s="133"/>
+      <c r="C86" s="134"/>
+      <c r="D86" s="134"/>
+      <c r="E86" s="134"/>
+      <c r="F86" s="134"/>
+      <c r="G86" s="134"/>
+      <c r="H86" s="134"/>
+      <c r="I86" s="134"/>
+      <c r="J86" s="134"/>
+      <c r="K86" s="135"/>
+      <c r="L86" s="183"/>
+      <c r="M86" s="173"/>
+      <c r="N86" s="174"/>
+      <c r="O86" s="159"/>
+      <c r="P86" s="160"/>
+      <c r="Q86" s="161"/>
+    </row>
+    <row r="87" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B87" s="133"/>
+      <c r="C87" s="134"/>
+      <c r="D87" s="134"/>
+      <c r="E87" s="134"/>
+      <c r="F87" s="134"/>
+      <c r="G87" s="134"/>
+      <c r="H87" s="134"/>
+      <c r="I87" s="134"/>
+      <c r="J87" s="134"/>
+      <c r="K87" s="135"/>
+      <c r="L87" s="183"/>
+      <c r="M87" s="173"/>
+      <c r="N87" s="174"/>
+      <c r="O87" s="159"/>
+      <c r="P87" s="160"/>
+      <c r="Q87" s="161"/>
+    </row>
+    <row r="88" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B88" s="133"/>
+      <c r="C88" s="134"/>
+      <c r="D88" s="134"/>
+      <c r="E88" s="134"/>
+      <c r="F88" s="134"/>
+      <c r="G88" s="134"/>
+      <c r="H88" s="134"/>
+      <c r="I88" s="134"/>
+      <c r="J88" s="134"/>
+      <c r="K88" s="135"/>
+      <c r="L88" s="183"/>
+      <c r="M88" s="173"/>
+      <c r="N88" s="174"/>
+      <c r="O88" s="159"/>
+      <c r="P88" s="160"/>
+      <c r="Q88" s="161"/>
+    </row>
+    <row r="89" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B89" s="133"/>
+      <c r="C89" s="134"/>
+      <c r="D89" s="134"/>
+      <c r="E89" s="134"/>
+      <c r="F89" s="134"/>
+      <c r="G89" s="134"/>
+      <c r="H89" s="134"/>
+      <c r="I89" s="134"/>
+      <c r="J89" s="134"/>
+      <c r="K89" s="135"/>
+      <c r="L89" s="183"/>
+      <c r="M89" s="173"/>
+      <c r="N89" s="174"/>
+      <c r="O89" s="159"/>
+      <c r="P89" s="160"/>
+      <c r="Q89" s="161"/>
+    </row>
+    <row r="90" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B90" s="136"/>
+      <c r="C90" s="137"/>
+      <c r="D90" s="137"/>
+      <c r="E90" s="137"/>
+      <c r="F90" s="137"/>
+      <c r="G90" s="137"/>
+      <c r="H90" s="137"/>
+      <c r="I90" s="137"/>
+      <c r="J90" s="137"/>
+      <c r="K90" s="138"/>
+      <c r="L90" s="184"/>
+      <c r="M90" s="171"/>
+      <c r="N90" s="172"/>
+      <c r="O90" s="156"/>
+      <c r="P90" s="157"/>
+      <c r="Q90" s="158"/>
+    </row>
+  </sheetData>
+  <mergeCells count="109">
+    <mergeCell ref="L83:L90"/>
+    <mergeCell ref="L75:L82"/>
+    <mergeCell ref="M83:N90"/>
+    <mergeCell ref="M75:N82"/>
+    <mergeCell ref="O83:Q90"/>
+    <mergeCell ref="O75:Q82"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="G74:K74"/>
+    <mergeCell ref="M74:N74"/>
+    <mergeCell ref="O74:Q74"/>
+    <mergeCell ref="B75:K90"/>
+    <mergeCell ref="M39:N40"/>
+    <mergeCell ref="M56:N56"/>
+    <mergeCell ref="M57:N58"/>
+    <mergeCell ref="M59:N60"/>
+    <mergeCell ref="M61:N62"/>
+    <mergeCell ref="M63:N64"/>
+    <mergeCell ref="M29:N32"/>
+    <mergeCell ref="M25:N28"/>
+    <mergeCell ref="M21:N24"/>
+    <mergeCell ref="M53:N54"/>
+    <mergeCell ref="M51:N52"/>
+    <mergeCell ref="M49:N50"/>
+    <mergeCell ref="M47:N48"/>
+    <mergeCell ref="M45:N46"/>
+    <mergeCell ref="M43:N44"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M16:N18"/>
+    <mergeCell ref="M13:N15"/>
+    <mergeCell ref="M11:N12"/>
+    <mergeCell ref="M9:N10"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="M5:N6"/>
+    <mergeCell ref="M3:N4"/>
+    <mergeCell ref="L67:L69"/>
+    <mergeCell ref="L70:L72"/>
+    <mergeCell ref="O67:Q69"/>
+    <mergeCell ref="O70:Q72"/>
+    <mergeCell ref="M70:N72"/>
+    <mergeCell ref="M67:N69"/>
+    <mergeCell ref="O61:Q62"/>
+    <mergeCell ref="L63:L64"/>
+    <mergeCell ref="O63:Q64"/>
+    <mergeCell ref="L65:L66"/>
+    <mergeCell ref="O65:Q66"/>
+    <mergeCell ref="M65:N66"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="G56:K56"/>
+    <mergeCell ref="O56:Q56"/>
+    <mergeCell ref="B57:K72"/>
+    <mergeCell ref="L57:L58"/>
+    <mergeCell ref="O57:Q58"/>
+    <mergeCell ref="L59:L60"/>
+    <mergeCell ref="O59:Q60"/>
+    <mergeCell ref="L61:L62"/>
+    <mergeCell ref="O3:Q4"/>
+    <mergeCell ref="O5:Q6"/>
+    <mergeCell ref="O7:Q8"/>
+    <mergeCell ref="O9:Q10"/>
+    <mergeCell ref="O11:Q12"/>
+    <mergeCell ref="O16:Q18"/>
+    <mergeCell ref="O13:Q15"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="B3:K18"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="O53:Q54"/>
+    <mergeCell ref="O51:Q52"/>
+    <mergeCell ref="O49:Q50"/>
+    <mergeCell ref="O47:Q48"/>
+    <mergeCell ref="O45:Q46"/>
+    <mergeCell ref="O43:Q44"/>
+    <mergeCell ref="O41:Q42"/>
+    <mergeCell ref="O39:Q40"/>
+    <mergeCell ref="M41:N42"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="L53:L54"/>
+    <mergeCell ref="L51:L52"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="B39:K54"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="O33:Q36"/>
+    <mergeCell ref="O29:Q32"/>
+    <mergeCell ref="O25:Q28"/>
+    <mergeCell ref="O21:Q24"/>
+    <mergeCell ref="O38:Q38"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="G38:K38"/>
+    <mergeCell ref="M33:N36"/>
+    <mergeCell ref="B21:K36"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="L21:L24"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="L29:L32"/>
+    <mergeCell ref="L33:L36"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
(DB, Share)UI 수정, Share 시스템 추가
</commit_message>
<xml_diff>
--- a/Documents/Aphelios_Database.xlsx
+++ b/Documents/Aphelios_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03ad4a8e8f7310f3/project/GangsterHamster/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="360" documentId="13_ncr:1_{01041995-EAED-4FCF-B70E-09E89BBA756B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAEEEEC3-A8F4-440F-A9B9-8350966DEAC1}"/>
+  <xr:revisionPtr revIDLastSave="378" documentId="13_ncr:1_{01041995-EAED-4FCF-B70E-09E89BBA756B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67E16B2F-7250-4540-BEC5-D9CCB171417C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1989,11 +1989,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>스테이지의 광경을 
-넣을 이미지박스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>스테이지에서 진행될 시나리오
 초반 부분을 넣을 텍스트박스</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2223,7 +2218,29 @@
   </si>
   <si>
     <r>
-      <t>클릭 시, 버튼에 저장된 스테이지 로딩
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>모든 스테이지들이 버튼 형식으로 있으며</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+클릭 시, 버튼에 저장된 스테이지 로딩
+(아직 클리어하지 못한 스테이지는 블러처리)
 "</t>
     </r>
     <r>
@@ -2249,6 +2266,10 @@
       </rPr>
       <t>" 시스템 참조</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테이지의 광경을 넣을 이미지박스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3243,7 +3264,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3577,6 +3598,39 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3589,182 +3643,152 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="12" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6820,7 +6844,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>627530</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>647496</xdr:rowOff>
+      <xdr:rowOff>549525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8048,26 +8072,26 @@
       <c r="E1" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="111" t="s">
+      <c r="F1" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
       <c r="M1" s="80" t="s">
         <v>75</v>
       </c>
       <c r="N1" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="O1" s="112" t="s">
+      <c r="O1" s="123" t="s">
         <v>70</v>
       </c>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
+      <c r="P1" s="123"/>
+      <c r="Q1" s="123"/>
       <c r="R1" s="40" t="s">
         <v>76</v>
       </c>
@@ -8076,7 +8100,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="82.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="119" t="s">
         <v>68</v>
       </c>
       <c r="B2" s="47" t="s">
@@ -8091,29 +8115,29 @@
       <c r="E2" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="113" t="s">
+      <c r="F2" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="124"/>
+      <c r="L2" s="124"/>
       <c r="M2" s="81"/>
       <c r="N2" s="85" t="s">
         <v>167</v>
       </c>
-      <c r="O2" s="114"/>
-      <c r="P2" s="114"/>
-      <c r="Q2" s="114"/>
+      <c r="O2" s="125"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="125"/>
       <c r="R2" s="50"/>
       <c r="S2" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="98.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="118"/>
+      <c r="A3" s="120"/>
       <c r="B3" s="51" t="s">
         <v>52</v>
       </c>
@@ -8126,29 +8150,29 @@
       <c r="E3" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="115" t="s">
+      <c r="F3" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="115"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
       <c r="M3" s="82"/>
       <c r="N3" s="86" t="s">
         <v>170</v>
       </c>
-      <c r="O3" s="116"/>
-      <c r="P3" s="116"/>
-      <c r="Q3" s="116"/>
+      <c r="O3" s="113"/>
+      <c r="P3" s="113"/>
+      <c r="Q3" s="113"/>
       <c r="R3" s="55"/>
       <c r="S3" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="408" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="121" t="s">
         <v>148</v>
       </c>
       <c r="B4" s="51" t="s">
@@ -8163,31 +8187,31 @@
       <c r="E4" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="115" t="s">
+      <c r="F4" s="111" t="s">
         <v>163</v>
       </c>
-      <c r="G4" s="115"/>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="111"/>
+      <c r="L4" s="111"/>
       <c r="M4" s="82"/>
       <c r="N4" s="84" t="s">
         <v>171</v>
       </c>
-      <c r="O4" s="115" t="s">
+      <c r="O4" s="111" t="s">
         <v>165</v>
       </c>
-      <c r="P4" s="115"/>
-      <c r="Q4" s="115"/>
+      <c r="P4" s="111"/>
+      <c r="Q4" s="111"/>
       <c r="R4" s="55"/>
       <c r="S4" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="119"/>
+      <c r="A5" s="121"/>
       <c r="B5" s="56" t="s">
         <v>63</v>
       </c>
@@ -8200,27 +8224,27 @@
       <c r="E5" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="115" t="s">
+      <c r="F5" s="111" t="s">
         <v>118</v>
       </c>
-      <c r="G5" s="115"/>
-      <c r="H5" s="115"/>
-      <c r="I5" s="115"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="111"/>
       <c r="M5" s="82"/>
       <c r="N5" s="87"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="116"/>
+      <c r="O5" s="113"/>
+      <c r="P5" s="113"/>
+      <c r="Q5" s="113"/>
       <c r="R5" s="55"/>
       <c r="S5" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="119"/>
+      <c r="A6" s="121"/>
       <c r="B6" s="56" t="s">
         <v>119</v>
       </c>
@@ -8233,27 +8257,27 @@
       <c r="E6" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="122" t="s">
+      <c r="F6" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="G6" s="115"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="115"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="111"/>
+      <c r="L6" s="111"/>
       <c r="M6" s="82"/>
       <c r="N6" s="54"/>
-      <c r="O6" s="116"/>
-      <c r="P6" s="116"/>
-      <c r="Q6" s="116"/>
+      <c r="O6" s="113"/>
+      <c r="P6" s="113"/>
+      <c r="Q6" s="113"/>
       <c r="R6" s="55"/>
       <c r="S6" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="48.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="120" t="s">
+      <c r="A7" s="116" t="s">
         <v>149</v>
       </c>
       <c r="B7" s="51" t="s">
@@ -8268,27 +8292,27 @@
       <c r="E7" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="122" t="s">
+      <c r="F7" s="118" t="s">
         <v>162</v>
       </c>
-      <c r="G7" s="115"/>
-      <c r="H7" s="115"/>
-      <c r="I7" s="115"/>
-      <c r="J7" s="115"/>
-      <c r="K7" s="115"/>
-      <c r="L7" s="115"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="111"/>
+      <c r="L7" s="111"/>
       <c r="M7" s="82"/>
       <c r="N7" s="54"/>
-      <c r="O7" s="116"/>
-      <c r="P7" s="116"/>
-      <c r="Q7" s="116"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="113"/>
+      <c r="Q7" s="113"/>
       <c r="R7" s="55"/>
       <c r="S7" s="65" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="120"/>
+      <c r="A8" s="116"/>
       <c r="B8" s="57" t="s">
         <v>64</v>
       </c>
@@ -8301,27 +8325,27 @@
       <c r="E8" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="115" t="s">
+      <c r="F8" s="111" t="s">
         <v>123</v>
       </c>
-      <c r="G8" s="115"/>
-      <c r="H8" s="115"/>
-      <c r="I8" s="115"/>
-      <c r="J8" s="115"/>
-      <c r="K8" s="115"/>
-      <c r="L8" s="115"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="111"/>
+      <c r="L8" s="111"/>
       <c r="M8" s="82"/>
       <c r="N8" s="54"/>
-      <c r="O8" s="116"/>
-      <c r="P8" s="116"/>
-      <c r="Q8" s="116"/>
+      <c r="O8" s="113"/>
+      <c r="P8" s="113"/>
+      <c r="Q8" s="113"/>
       <c r="R8" s="55"/>
       <c r="S8" s="65" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="120"/>
+      <c r="A9" s="116"/>
       <c r="B9" s="58" t="s">
         <v>65</v>
       </c>
@@ -8334,27 +8358,27 @@
       <c r="E9" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="115" t="s">
+      <c r="F9" s="111" t="s">
         <v>125</v>
       </c>
-      <c r="G9" s="115"/>
-      <c r="H9" s="115"/>
-      <c r="I9" s="115"/>
-      <c r="J9" s="115"/>
-      <c r="K9" s="115"/>
-      <c r="L9" s="115"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="111"/>
       <c r="M9" s="82"/>
       <c r="N9" s="54"/>
-      <c r="O9" s="116"/>
-      <c r="P9" s="116"/>
-      <c r="Q9" s="116"/>
+      <c r="O9" s="113"/>
+      <c r="P9" s="113"/>
+      <c r="Q9" s="113"/>
       <c r="R9" s="55"/>
       <c r="S9" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="53.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="117" t="s">
         <v>150</v>
       </c>
       <c r="B10" s="51" t="s">
@@ -8369,27 +8393,27 @@
       <c r="E10" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="F10" s="122" t="s">
+      <c r="F10" s="118" t="s">
         <v>155</v>
       </c>
-      <c r="G10" s="115"/>
-      <c r="H10" s="115"/>
-      <c r="I10" s="115"/>
-      <c r="J10" s="115"/>
-      <c r="K10" s="115"/>
-      <c r="L10" s="115"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="111"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="111"/>
+      <c r="K10" s="111"/>
+      <c r="L10" s="111"/>
       <c r="M10" s="82"/>
       <c r="N10" s="54"/>
-      <c r="O10" s="116"/>
-      <c r="P10" s="116"/>
-      <c r="Q10" s="116"/>
+      <c r="O10" s="113"/>
+      <c r="P10" s="113"/>
+      <c r="Q10" s="113"/>
       <c r="R10" s="55"/>
       <c r="S10" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="121"/>
+      <c r="A11" s="117"/>
       <c r="B11" s="58" t="s">
         <v>66</v>
       </c>
@@ -8402,27 +8426,27 @@
       <c r="E11" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="122" t="s">
+      <c r="F11" s="118" t="s">
         <v>138</v>
       </c>
-      <c r="G11" s="115"/>
-      <c r="H11" s="115"/>
-      <c r="I11" s="115"/>
-      <c r="J11" s="115"/>
-      <c r="K11" s="115"/>
-      <c r="L11" s="115"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="111"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="111"/>
+      <c r="L11" s="111"/>
       <c r="M11" s="82"/>
       <c r="N11" s="54"/>
-      <c r="O11" s="116"/>
-      <c r="P11" s="116"/>
-      <c r="Q11" s="116"/>
+      <c r="O11" s="113"/>
+      <c r="P11" s="113"/>
+      <c r="Q11" s="113"/>
       <c r="R11" s="55"/>
       <c r="S11" s="65" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="121"/>
+      <c r="A12" s="117"/>
       <c r="B12" s="58" t="s">
         <v>67</v>
       </c>
@@ -8435,20 +8459,20 @@
       <c r="E12" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="115" t="s">
+      <c r="F12" s="111" t="s">
         <v>129</v>
       </c>
-      <c r="G12" s="115"/>
-      <c r="H12" s="115"/>
-      <c r="I12" s="115"/>
-      <c r="J12" s="115"/>
-      <c r="K12" s="115"/>
-      <c r="L12" s="115"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="111"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="111"/>
+      <c r="L12" s="111"/>
       <c r="M12" s="82"/>
       <c r="N12" s="54"/>
-      <c r="O12" s="116"/>
-      <c r="P12" s="116"/>
-      <c r="Q12" s="116"/>
+      <c r="O12" s="113"/>
+      <c r="P12" s="113"/>
+      <c r="Q12" s="113"/>
       <c r="R12" s="55"/>
       <c r="S12" s="65" t="s">
         <v>92</v>
@@ -8470,20 +8494,20 @@
       <c r="E13" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="115" t="s">
+      <c r="F13" s="111" t="s">
         <v>139</v>
       </c>
-      <c r="G13" s="115"/>
-      <c r="H13" s="115"/>
-      <c r="I13" s="115"/>
-      <c r="J13" s="115"/>
-      <c r="K13" s="115"/>
-      <c r="L13" s="115"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="111"/>
       <c r="M13" s="82"/>
       <c r="N13" s="54"/>
-      <c r="O13" s="116"/>
-      <c r="P13" s="116"/>
-      <c r="Q13" s="116"/>
+      <c r="O13" s="113"/>
+      <c r="P13" s="113"/>
+      <c r="Q13" s="113"/>
       <c r="R13" s="55"/>
       <c r="S13" s="65" t="s">
         <v>92</v>
@@ -8505,20 +8529,20 @@
       <c r="E14" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="F14" s="115" t="s">
+      <c r="F14" s="111" t="s">
         <v>140</v>
       </c>
-      <c r="G14" s="115"/>
-      <c r="H14" s="115"/>
-      <c r="I14" s="115"/>
-      <c r="J14" s="115"/>
-      <c r="K14" s="115"/>
-      <c r="L14" s="115"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="111"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="111"/>
+      <c r="K14" s="111"/>
+      <c r="L14" s="111"/>
       <c r="M14" s="82"/>
       <c r="N14" s="54"/>
-      <c r="O14" s="116"/>
-      <c r="P14" s="116"/>
-      <c r="Q14" s="116"/>
+      <c r="O14" s="113"/>
+      <c r="P14" s="113"/>
+      <c r="Q14" s="113"/>
       <c r="R14" s="55"/>
       <c r="S14" s="65" t="s">
         <v>92</v>
@@ -8540,20 +8564,20 @@
       <c r="E15" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="115" t="s">
+      <c r="F15" s="111" t="s">
         <v>141</v>
       </c>
-      <c r="G15" s="115"/>
-      <c r="H15" s="115"/>
-      <c r="I15" s="115"/>
-      <c r="J15" s="115"/>
-      <c r="K15" s="115"/>
-      <c r="L15" s="115"/>
+      <c r="G15" s="111"/>
+      <c r="H15" s="111"/>
+      <c r="I15" s="111"/>
+      <c r="J15" s="111"/>
+      <c r="K15" s="111"/>
+      <c r="L15" s="111"/>
       <c r="M15" s="82"/>
       <c r="N15" s="54"/>
-      <c r="O15" s="116"/>
-      <c r="P15" s="116"/>
-      <c r="Q15" s="116"/>
+      <c r="O15" s="113"/>
+      <c r="P15" s="113"/>
+      <c r="Q15" s="113"/>
       <c r="R15" s="55"/>
       <c r="S15" s="65" t="s">
         <v>93</v>
@@ -8575,20 +8599,20 @@
       <c r="E16" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="115" t="s">
+      <c r="F16" s="111" t="s">
         <v>134</v>
       </c>
-      <c r="G16" s="115"/>
-      <c r="H16" s="115"/>
-      <c r="I16" s="115"/>
-      <c r="J16" s="115"/>
-      <c r="K16" s="115"/>
-      <c r="L16" s="115"/>
+      <c r="G16" s="111"/>
+      <c r="H16" s="111"/>
+      <c r="I16" s="111"/>
+      <c r="J16" s="111"/>
+      <c r="K16" s="111"/>
+      <c r="L16" s="111"/>
       <c r="M16" s="82"/>
       <c r="N16" s="54"/>
-      <c r="O16" s="116"/>
-      <c r="P16" s="116"/>
-      <c r="Q16" s="116"/>
+      <c r="O16" s="113"/>
+      <c r="P16" s="113"/>
+      <c r="Q16" s="113"/>
       <c r="R16" s="55"/>
       <c r="S16" s="65" t="s">
         <v>93</v>
@@ -8610,20 +8634,20 @@
       <c r="E17" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="115" t="s">
+      <c r="F17" s="111" t="s">
         <v>168</v>
       </c>
-      <c r="G17" s="115"/>
-      <c r="H17" s="115"/>
-      <c r="I17" s="115"/>
-      <c r="J17" s="115"/>
-      <c r="K17" s="115"/>
-      <c r="L17" s="115"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="111"/>
+      <c r="I17" s="111"/>
+      <c r="J17" s="111"/>
+      <c r="K17" s="111"/>
+      <c r="L17" s="111"/>
       <c r="M17" s="82"/>
       <c r="N17" s="54"/>
-      <c r="O17" s="116"/>
-      <c r="P17" s="116"/>
-      <c r="Q17" s="116"/>
+      <c r="O17" s="113"/>
+      <c r="P17" s="113"/>
+      <c r="Q17" s="113"/>
       <c r="R17" s="55"/>
       <c r="S17" s="65" t="s">
         <v>92</v>
@@ -8645,32 +8669,59 @@
       <c r="E18" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="125" t="s">
+      <c r="F18" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G18" s="125"/>
-      <c r="H18" s="125"/>
-      <c r="I18" s="125"/>
-      <c r="J18" s="125"/>
-      <c r="K18" s="125"/>
-      <c r="L18" s="125"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="112"/>
+      <c r="K18" s="112"/>
+      <c r="L18" s="112"/>
       <c r="M18" s="83"/>
       <c r="N18" s="62"/>
-      <c r="O18" s="124"/>
-      <c r="P18" s="124"/>
-      <c r="Q18" s="124"/>
+      <c r="O18" s="115"/>
+      <c r="P18" s="115"/>
+      <c r="Q18" s="115"/>
       <c r="R18" s="63"/>
       <c r="S18" s="66" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="N19" s="123"/>
-      <c r="O19" s="123"/>
-      <c r="P19" s="123"/>
+      <c r="N19" s="114"/>
+      <c r="O19" s="114"/>
+      <c r="P19" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="F3:L3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="F5:L5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="F6:L6"/>
+    <mergeCell ref="F7:L7"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="F9:L9"/>
+    <mergeCell ref="F10:L10"/>
+    <mergeCell ref="F11:L11"/>
+    <mergeCell ref="F12:L12"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="O18:Q18"/>
     <mergeCell ref="F16:L16"/>
     <mergeCell ref="F17:L17"/>
     <mergeCell ref="F18:L18"/>
@@ -8685,33 +8736,6 @@
     <mergeCell ref="O12:Q12"/>
     <mergeCell ref="O13:Q13"/>
     <mergeCell ref="O14:Q14"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="F6:L6"/>
-    <mergeCell ref="F7:L7"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="F9:L9"/>
-    <mergeCell ref="F10:L10"/>
-    <mergeCell ref="F11:L11"/>
-    <mergeCell ref="F12:L12"/>
-    <mergeCell ref="F4:L4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="F5:L5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="F3:L3"/>
-    <mergeCell ref="O3:Q3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8725,1781 +8749,1851 @@
   <dimension ref="B2:Q90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V48" sqref="V48"/>
+      <selection activeCell="B38" sqref="B38:Q54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="12" max="12" width="7.5" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="17" max="17" width="19.19921875" customWidth="1"/>
+    <col min="17" max="17" width="22.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="131" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="129" t="s">
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="133" t="s">
         <v>175</v>
       </c>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="130"/>
+      <c r="H2" s="133"/>
+      <c r="I2" s="133"/>
+      <c r="J2" s="133"/>
+      <c r="K2" s="134"/>
       <c r="L2" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="M2" s="131" t="s">
+      <c r="M2" s="150" t="s">
+        <v>192</v>
+      </c>
+      <c r="N2" s="128"/>
+      <c r="O2" s="150" t="s">
+        <v>173</v>
+      </c>
+      <c r="P2" s="132"/>
+      <c r="Q2" s="151"/>
+    </row>
+    <row r="3" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="141"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="143"/>
+      <c r="L3" s="127">
+        <v>1</v>
+      </c>
+      <c r="M3" s="135" t="s">
         <v>193</v>
       </c>
-      <c r="N2" s="127"/>
-      <c r="O2" s="131" t="s">
-        <v>173</v>
-      </c>
-      <c r="P2" s="126"/>
-      <c r="Q2" s="170"/>
-    </row>
-    <row r="3" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="136"/>
-      <c r="L3" s="143">
-        <v>1</v>
-      </c>
-      <c r="M3" s="144" t="s">
+      <c r="N3" s="136"/>
+      <c r="O3" s="162" t="s">
+        <v>185</v>
+      </c>
+      <c r="P3" s="155"/>
+      <c r="Q3" s="156"/>
+    </row>
+    <row r="4" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="144"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="145"/>
+      <c r="H4" s="145"/>
+      <c r="I4" s="145"/>
+      <c r="J4" s="145"/>
+      <c r="K4" s="146"/>
+      <c r="L4" s="127"/>
+      <c r="M4" s="139"/>
+      <c r="N4" s="140"/>
+      <c r="O4" s="163"/>
+      <c r="P4" s="157"/>
+      <c r="Q4" s="158"/>
+    </row>
+    <row r="5" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="144"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="145"/>
+      <c r="K5" s="146"/>
+      <c r="L5" s="127">
+        <v>2</v>
+      </c>
+      <c r="M5" s="135" t="s">
         <v>194</v>
       </c>
-      <c r="N3" s="145"/>
-      <c r="O3" s="150" t="s">
+      <c r="N5" s="136"/>
+      <c r="O5" s="162" t="s">
         <v>186</v>
       </c>
-      <c r="P3" s="151"/>
-      <c r="Q3" s="152"/>
-    </row>
-    <row r="4" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="137"/>
-      <c r="C4" s="138"/>
-      <c r="D4" s="138"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="138"/>
-      <c r="G4" s="138"/>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="138"/>
-      <c r="K4" s="139"/>
-      <c r="L4" s="143"/>
-      <c r="M4" s="146"/>
-      <c r="N4" s="147"/>
-      <c r="O4" s="153"/>
-      <c r="P4" s="154"/>
-      <c r="Q4" s="155"/>
-    </row>
-    <row r="5" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="137"/>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="138"/>
-      <c r="G5" s="138"/>
-      <c r="H5" s="138"/>
-      <c r="I5" s="138"/>
-      <c r="J5" s="138"/>
-      <c r="K5" s="139"/>
-      <c r="L5" s="143">
-        <v>2</v>
-      </c>
-      <c r="M5" s="144" t="s">
+      <c r="P5" s="155"/>
+      <c r="Q5" s="156"/>
+    </row>
+    <row r="6" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="144"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="145"/>
+      <c r="J6" s="145"/>
+      <c r="K6" s="146"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="139"/>
+      <c r="N6" s="140"/>
+      <c r="O6" s="163"/>
+      <c r="P6" s="157"/>
+      <c r="Q6" s="158"/>
+    </row>
+    <row r="7" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="144"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="145"/>
+      <c r="F7" s="145"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
+      <c r="K7" s="146"/>
+      <c r="L7" s="127">
+        <v>3</v>
+      </c>
+      <c r="M7" s="135" t="s">
+        <v>197</v>
+      </c>
+      <c r="N7" s="136"/>
+      <c r="O7" s="162" t="s">
+        <v>216</v>
+      </c>
+      <c r="P7" s="154"/>
+      <c r="Q7" s="159"/>
+    </row>
+    <row r="8" spans="2:17" ht="30.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="144"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="145"/>
+      <c r="E8" s="145"/>
+      <c r="F8" s="145"/>
+      <c r="G8" s="145"/>
+      <c r="H8" s="145"/>
+      <c r="I8" s="145"/>
+      <c r="J8" s="145"/>
+      <c r="K8" s="146"/>
+      <c r="L8" s="127"/>
+      <c r="M8" s="139"/>
+      <c r="N8" s="140"/>
+      <c r="O8" s="164"/>
+      <c r="P8" s="160"/>
+      <c r="Q8" s="161"/>
+    </row>
+    <row r="9" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="144"/>
+      <c r="C9" s="145"/>
+      <c r="D9" s="145"/>
+      <c r="E9" s="145"/>
+      <c r="F9" s="145"/>
+      <c r="G9" s="145"/>
+      <c r="H9" s="145"/>
+      <c r="I9" s="145"/>
+      <c r="J9" s="145"/>
+      <c r="K9" s="146"/>
+      <c r="L9" s="127">
+        <v>4</v>
+      </c>
+      <c r="M9" s="135" t="s">
+        <v>198</v>
+      </c>
+      <c r="N9" s="136"/>
+      <c r="O9" s="162" t="s">
+        <v>187</v>
+      </c>
+      <c r="P9" s="155"/>
+      <c r="Q9" s="156"/>
+    </row>
+    <row r="10" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="144"/>
+      <c r="C10" s="145"/>
+      <c r="D10" s="145"/>
+      <c r="E10" s="145"/>
+      <c r="F10" s="145"/>
+      <c r="G10" s="145"/>
+      <c r="H10" s="145"/>
+      <c r="I10" s="145"/>
+      <c r="J10" s="145"/>
+      <c r="K10" s="146"/>
+      <c r="L10" s="127"/>
+      <c r="M10" s="139"/>
+      <c r="N10" s="140"/>
+      <c r="O10" s="163"/>
+      <c r="P10" s="157"/>
+      <c r="Q10" s="158"/>
+    </row>
+    <row r="11" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="144"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="145"/>
+      <c r="E11" s="145"/>
+      <c r="F11" s="145"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="145"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="145"/>
+      <c r="K11" s="146"/>
+      <c r="L11" s="127">
+        <v>5</v>
+      </c>
+      <c r="M11" s="135" t="s">
+        <v>196</v>
+      </c>
+      <c r="N11" s="136"/>
+      <c r="O11" s="162" t="s">
+        <v>188</v>
+      </c>
+      <c r="P11" s="154"/>
+      <c r="Q11" s="159"/>
+    </row>
+    <row r="12" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="144"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="145"/>
+      <c r="E12" s="145"/>
+      <c r="F12" s="145"/>
+      <c r="G12" s="145"/>
+      <c r="H12" s="145"/>
+      <c r="I12" s="145"/>
+      <c r="J12" s="145"/>
+      <c r="K12" s="146"/>
+      <c r="L12" s="127"/>
+      <c r="M12" s="139"/>
+      <c r="N12" s="140"/>
+      <c r="O12" s="164"/>
+      <c r="P12" s="160"/>
+      <c r="Q12" s="161"/>
+    </row>
+    <row r="13" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="144"/>
+      <c r="C13" s="145"/>
+      <c r="D13" s="145"/>
+      <c r="E13" s="145"/>
+      <c r="F13" s="145"/>
+      <c r="G13" s="145"/>
+      <c r="H13" s="145"/>
+      <c r="I13" s="145"/>
+      <c r="J13" s="145"/>
+      <c r="K13" s="146"/>
+      <c r="L13" s="127">
+        <v>6</v>
+      </c>
+      <c r="M13" s="135" t="s">
         <v>195</v>
       </c>
-      <c r="N5" s="145"/>
-      <c r="O5" s="150" t="s">
-        <v>187</v>
-      </c>
-      <c r="P5" s="151"/>
-      <c r="Q5" s="152"/>
-    </row>
-    <row r="6" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="137"/>
-      <c r="C6" s="138"/>
-      <c r="D6" s="138"/>
-      <c r="E6" s="138"/>
-      <c r="F6" s="138"/>
-      <c r="G6" s="138"/>
-      <c r="H6" s="138"/>
-      <c r="I6" s="138"/>
-      <c r="J6" s="138"/>
-      <c r="K6" s="139"/>
-      <c r="L6" s="143"/>
-      <c r="M6" s="146"/>
-      <c r="N6" s="147"/>
-      <c r="O6" s="153"/>
-      <c r="P6" s="154"/>
-      <c r="Q6" s="155"/>
-    </row>
-    <row r="7" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="137"/>
-      <c r="C7" s="138"/>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
-      <c r="G7" s="138"/>
-      <c r="H7" s="138"/>
-      <c r="I7" s="138"/>
-      <c r="J7" s="138"/>
-      <c r="K7" s="139"/>
-      <c r="L7" s="143">
-        <v>3</v>
-      </c>
-      <c r="M7" s="144" t="s">
-        <v>198</v>
-      </c>
-      <c r="N7" s="145"/>
-      <c r="O7" s="150" t="s">
-        <v>217</v>
-      </c>
-      <c r="P7" s="156"/>
-      <c r="Q7" s="157"/>
-    </row>
-    <row r="8" spans="2:17" ht="30.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="137"/>
-      <c r="C8" s="138"/>
-      <c r="D8" s="138"/>
-      <c r="E8" s="138"/>
-      <c r="F8" s="138"/>
-      <c r="G8" s="138"/>
-      <c r="H8" s="138"/>
-      <c r="I8" s="138"/>
-      <c r="J8" s="138"/>
-      <c r="K8" s="139"/>
-      <c r="L8" s="143"/>
-      <c r="M8" s="146"/>
-      <c r="N8" s="147"/>
-      <c r="O8" s="164"/>
-      <c r="P8" s="158"/>
-      <c r="Q8" s="159"/>
-    </row>
-    <row r="9" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="137"/>
-      <c r="C9" s="138"/>
-      <c r="D9" s="138"/>
-      <c r="E9" s="138"/>
-      <c r="F9" s="138"/>
-      <c r="G9" s="138"/>
-      <c r="H9" s="138"/>
-      <c r="I9" s="138"/>
-      <c r="J9" s="138"/>
-      <c r="K9" s="139"/>
-      <c r="L9" s="143">
-        <v>4</v>
-      </c>
-      <c r="M9" s="144" t="s">
+      <c r="N13" s="136"/>
+      <c r="O13" s="162" t="s">
+        <v>190</v>
+      </c>
+      <c r="P13" s="154"/>
+      <c r="Q13" s="159"/>
+    </row>
+    <row r="14" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="144"/>
+      <c r="C14" s="145"/>
+      <c r="D14" s="145"/>
+      <c r="E14" s="145"/>
+      <c r="F14" s="145"/>
+      <c r="G14" s="145"/>
+      <c r="H14" s="145"/>
+      <c r="I14" s="145"/>
+      <c r="J14" s="145"/>
+      <c r="K14" s="146"/>
+      <c r="L14" s="127"/>
+      <c r="M14" s="137"/>
+      <c r="N14" s="138"/>
+      <c r="O14" s="169"/>
+      <c r="P14" s="170"/>
+      <c r="Q14" s="171"/>
+    </row>
+    <row r="15" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="144"/>
+      <c r="C15" s="145"/>
+      <c r="D15" s="145"/>
+      <c r="E15" s="145"/>
+      <c r="F15" s="145"/>
+      <c r="G15" s="145"/>
+      <c r="H15" s="145"/>
+      <c r="I15" s="145"/>
+      <c r="J15" s="145"/>
+      <c r="K15" s="146"/>
+      <c r="L15" s="127"/>
+      <c r="M15" s="139"/>
+      <c r="N15" s="140"/>
+      <c r="O15" s="164"/>
+      <c r="P15" s="160"/>
+      <c r="Q15" s="161"/>
+    </row>
+    <row r="16" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="144"/>
+      <c r="C16" s="145"/>
+      <c r="D16" s="145"/>
+      <c r="E16" s="145"/>
+      <c r="F16" s="145"/>
+      <c r="G16" s="145"/>
+      <c r="H16" s="145"/>
+      <c r="I16" s="145"/>
+      <c r="J16" s="145"/>
+      <c r="K16" s="146"/>
+      <c r="L16" s="127">
+        <v>7</v>
+      </c>
+      <c r="M16" s="135" t="s">
         <v>199</v>
       </c>
-      <c r="N9" s="145"/>
-      <c r="O9" s="150" t="s">
-        <v>188</v>
-      </c>
-      <c r="P9" s="151"/>
-      <c r="Q9" s="152"/>
-    </row>
-    <row r="10" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="137"/>
-      <c r="C10" s="138"/>
-      <c r="D10" s="138"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="138"/>
-      <c r="G10" s="138"/>
-      <c r="H10" s="138"/>
-      <c r="I10" s="138"/>
-      <c r="J10" s="138"/>
-      <c r="K10" s="139"/>
-      <c r="L10" s="143"/>
-      <c r="M10" s="146"/>
-      <c r="N10" s="147"/>
-      <c r="O10" s="153"/>
-      <c r="P10" s="154"/>
-      <c r="Q10" s="155"/>
-    </row>
-    <row r="11" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="137"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="138"/>
-      <c r="F11" s="138"/>
-      <c r="G11" s="138"/>
-      <c r="H11" s="138"/>
-      <c r="I11" s="138"/>
-      <c r="J11" s="138"/>
-      <c r="K11" s="139"/>
-      <c r="L11" s="143">
-        <v>5</v>
-      </c>
-      <c r="M11" s="144" t="s">
-        <v>197</v>
-      </c>
-      <c r="N11" s="145"/>
-      <c r="O11" s="150" t="s">
+      <c r="N16" s="136"/>
+      <c r="O16" s="165" t="s">
         <v>189</v>
       </c>
-      <c r="P11" s="156"/>
-      <c r="Q11" s="157"/>
-    </row>
-    <row r="12" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="137"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="138"/>
-      <c r="G12" s="138"/>
-      <c r="H12" s="138"/>
-      <c r="I12" s="138"/>
-      <c r="J12" s="138"/>
-      <c r="K12" s="139"/>
-      <c r="L12" s="143"/>
-      <c r="M12" s="146"/>
-      <c r="N12" s="147"/>
-      <c r="O12" s="164"/>
-      <c r="P12" s="158"/>
-      <c r="Q12" s="159"/>
-    </row>
-    <row r="13" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="137"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="138"/>
-      <c r="F13" s="138"/>
-      <c r="G13" s="138"/>
-      <c r="H13" s="138"/>
-      <c r="I13" s="138"/>
-      <c r="J13" s="138"/>
-      <c r="K13" s="139"/>
-      <c r="L13" s="143">
-        <v>6</v>
-      </c>
-      <c r="M13" s="144" t="s">
-        <v>196</v>
-      </c>
-      <c r="N13" s="145"/>
-      <c r="O13" s="150" t="s">
-        <v>191</v>
-      </c>
-      <c r="P13" s="156"/>
-      <c r="Q13" s="157"/>
-    </row>
-    <row r="14" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="137"/>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138"/>
-      <c r="E14" s="138"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="138"/>
-      <c r="H14" s="138"/>
-      <c r="I14" s="138"/>
-      <c r="J14" s="138"/>
-      <c r="K14" s="139"/>
-      <c r="L14" s="143"/>
-      <c r="M14" s="148"/>
-      <c r="N14" s="149"/>
-      <c r="O14" s="161"/>
-      <c r="P14" s="162"/>
-      <c r="Q14" s="163"/>
-    </row>
-    <row r="15" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="137"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="138"/>
-      <c r="F15" s="138"/>
-      <c r="G15" s="138"/>
-      <c r="H15" s="138"/>
-      <c r="I15" s="138"/>
-      <c r="J15" s="138"/>
-      <c r="K15" s="139"/>
-      <c r="L15" s="143"/>
-      <c r="M15" s="146"/>
-      <c r="N15" s="147"/>
-      <c r="O15" s="164"/>
-      <c r="P15" s="158"/>
-      <c r="Q15" s="159"/>
-    </row>
-    <row r="16" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="137"/>
-      <c r="C16" s="138"/>
-      <c r="D16" s="138"/>
-      <c r="E16" s="138"/>
-      <c r="F16" s="138"/>
-      <c r="G16" s="138"/>
-      <c r="H16" s="138"/>
-      <c r="I16" s="138"/>
-      <c r="J16" s="138"/>
-      <c r="K16" s="139"/>
-      <c r="L16" s="143">
-        <v>7</v>
-      </c>
-      <c r="M16" s="144" t="s">
-        <v>200</v>
-      </c>
-      <c r="N16" s="145"/>
-      <c r="O16" s="168" t="s">
-        <v>190</v>
-      </c>
-      <c r="P16" s="151"/>
-      <c r="Q16" s="152"/>
+      <c r="P16" s="155"/>
+      <c r="Q16" s="156"/>
     </row>
     <row r="17" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="137"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
-      <c r="E17" s="138"/>
-      <c r="F17" s="138"/>
-      <c r="G17" s="138"/>
-      <c r="H17" s="138"/>
-      <c r="I17" s="138"/>
-      <c r="J17" s="138"/>
-      <c r="K17" s="139"/>
-      <c r="L17" s="143"/>
-      <c r="M17" s="148"/>
-      <c r="N17" s="149"/>
-      <c r="O17" s="165"/>
-      <c r="P17" s="166"/>
-      <c r="Q17" s="167"/>
+      <c r="B17" s="144"/>
+      <c r="C17" s="145"/>
+      <c r="D17" s="145"/>
+      <c r="E17" s="145"/>
+      <c r="F17" s="145"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="145"/>
+      <c r="I17" s="145"/>
+      <c r="J17" s="145"/>
+      <c r="K17" s="146"/>
+      <c r="L17" s="127"/>
+      <c r="M17" s="137"/>
+      <c r="N17" s="138"/>
+      <c r="O17" s="166"/>
+      <c r="P17" s="167"/>
+      <c r="Q17" s="168"/>
     </row>
     <row r="18" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="140"/>
-      <c r="C18" s="141"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="141"/>
-      <c r="G18" s="141"/>
-      <c r="H18" s="141"/>
-      <c r="I18" s="141"/>
-      <c r="J18" s="141"/>
-      <c r="K18" s="142"/>
-      <c r="L18" s="143"/>
-      <c r="M18" s="146"/>
-      <c r="N18" s="147"/>
-      <c r="O18" s="153"/>
-      <c r="P18" s="154"/>
-      <c r="Q18" s="155"/>
+      <c r="B18" s="147"/>
+      <c r="C18" s="148"/>
+      <c r="D18" s="148"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="148"/>
+      <c r="G18" s="148"/>
+      <c r="H18" s="148"/>
+      <c r="I18" s="148"/>
+      <c r="J18" s="148"/>
+      <c r="K18" s="149"/>
+      <c r="L18" s="127"/>
+      <c r="M18" s="139"/>
+      <c r="N18" s="140"/>
+      <c r="O18" s="163"/>
+      <c r="P18" s="157"/>
+      <c r="Q18" s="158"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B20" s="128" t="s">
+      <c r="B20" s="131" t="s">
         <v>174</v>
       </c>
-      <c r="C20" s="126"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="127"/>
-      <c r="G20" s="129" t="s">
+      <c r="C20" s="132"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="132"/>
+      <c r="F20" s="128"/>
+      <c r="G20" s="133" t="s">
         <v>179</v>
       </c>
-      <c r="H20" s="129"/>
-      <c r="I20" s="129"/>
-      <c r="J20" s="129"/>
-      <c r="K20" s="130"/>
+      <c r="H20" s="133"/>
+      <c r="I20" s="133"/>
+      <c r="J20" s="133"/>
+      <c r="K20" s="134"/>
       <c r="L20" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="M20" s="126" t="s">
-        <v>193</v>
-      </c>
-      <c r="N20" s="127"/>
-      <c r="O20" s="131" t="s">
+      <c r="M20" s="132" t="s">
+        <v>192</v>
+      </c>
+      <c r="N20" s="128"/>
+      <c r="O20" s="150" t="s">
         <v>173</v>
       </c>
-      <c r="P20" s="126"/>
-      <c r="Q20" s="170"/>
+      <c r="P20" s="132"/>
+      <c r="Q20" s="151"/>
     </row>
     <row r="21" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="134"/>
-      <c r="C21" s="135"/>
-      <c r="D21" s="135"/>
-      <c r="E21" s="135"/>
-      <c r="F21" s="135"/>
-      <c r="G21" s="135"/>
-      <c r="H21" s="135"/>
-      <c r="I21" s="135"/>
-      <c r="J21" s="135"/>
-      <c r="K21" s="136"/>
-      <c r="L21" s="143">
+      <c r="B21" s="141"/>
+      <c r="C21" s="142"/>
+      <c r="D21" s="142"/>
+      <c r="E21" s="142"/>
+      <c r="F21" s="142"/>
+      <c r="G21" s="142"/>
+      <c r="H21" s="142"/>
+      <c r="I21" s="142"/>
+      <c r="J21" s="142"/>
+      <c r="K21" s="143"/>
+      <c r="L21" s="127">
         <v>1</v>
       </c>
-      <c r="M21" s="144" t="s">
-        <v>204</v>
-      </c>
-      <c r="N21" s="145"/>
-      <c r="O21" s="172" t="s">
+      <c r="M21" s="135" t="s">
+        <v>203</v>
+      </c>
+      <c r="N21" s="136"/>
+      <c r="O21" s="153" t="s">
         <v>181</v>
       </c>
-      <c r="P21" s="172"/>
-      <c r="Q21" s="172"/>
+      <c r="P21" s="153"/>
+      <c r="Q21" s="153"/>
     </row>
     <row r="22" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="137"/>
-      <c r="C22" s="138"/>
-      <c r="D22" s="138"/>
-      <c r="E22" s="138"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="138"/>
-      <c r="H22" s="138"/>
-      <c r="I22" s="138"/>
-      <c r="J22" s="138"/>
-      <c r="K22" s="139"/>
-      <c r="L22" s="143"/>
-      <c r="M22" s="148"/>
-      <c r="N22" s="149"/>
-      <c r="O22" s="172"/>
-      <c r="P22" s="172"/>
-      <c r="Q22" s="172"/>
+      <c r="B22" s="144"/>
+      <c r="C22" s="145"/>
+      <c r="D22" s="145"/>
+      <c r="E22" s="145"/>
+      <c r="F22" s="145"/>
+      <c r="G22" s="145"/>
+      <c r="H22" s="145"/>
+      <c r="I22" s="145"/>
+      <c r="J22" s="145"/>
+      <c r="K22" s="146"/>
+      <c r="L22" s="127"/>
+      <c r="M22" s="137"/>
+      <c r="N22" s="138"/>
+      <c r="O22" s="153"/>
+      <c r="P22" s="153"/>
+      <c r="Q22" s="153"/>
     </row>
     <row r="23" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="137"/>
-      <c r="C23" s="138"/>
-      <c r="D23" s="138"/>
-      <c r="E23" s="138"/>
-      <c r="F23" s="138"/>
-      <c r="G23" s="138"/>
-      <c r="H23" s="138"/>
-      <c r="I23" s="138"/>
-      <c r="J23" s="138"/>
-      <c r="K23" s="139"/>
-      <c r="L23" s="143"/>
-      <c r="M23" s="148"/>
-      <c r="N23" s="149"/>
-      <c r="O23" s="172"/>
-      <c r="P23" s="172"/>
-      <c r="Q23" s="172"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="145"/>
+      <c r="D23" s="145"/>
+      <c r="E23" s="145"/>
+      <c r="F23" s="145"/>
+      <c r="G23" s="145"/>
+      <c r="H23" s="145"/>
+      <c r="I23" s="145"/>
+      <c r="J23" s="145"/>
+      <c r="K23" s="146"/>
+      <c r="L23" s="127"/>
+      <c r="M23" s="137"/>
+      <c r="N23" s="138"/>
+      <c r="O23" s="153"/>
+      <c r="P23" s="153"/>
+      <c r="Q23" s="153"/>
     </row>
     <row r="24" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="137"/>
-      <c r="C24" s="138"/>
-      <c r="D24" s="138"/>
-      <c r="E24" s="138"/>
-      <c r="F24" s="138"/>
-      <c r="G24" s="138"/>
-      <c r="H24" s="138"/>
-      <c r="I24" s="138"/>
-      <c r="J24" s="138"/>
-      <c r="K24" s="139"/>
-      <c r="L24" s="143"/>
-      <c r="M24" s="146"/>
-      <c r="N24" s="147"/>
-      <c r="O24" s="172"/>
-      <c r="P24" s="172"/>
-      <c r="Q24" s="172"/>
+      <c r="B24" s="144"/>
+      <c r="C24" s="145"/>
+      <c r="D24" s="145"/>
+      <c r="E24" s="145"/>
+      <c r="F24" s="145"/>
+      <c r="G24" s="145"/>
+      <c r="H24" s="145"/>
+      <c r="I24" s="145"/>
+      <c r="J24" s="145"/>
+      <c r="K24" s="146"/>
+      <c r="L24" s="127"/>
+      <c r="M24" s="139"/>
+      <c r="N24" s="140"/>
+      <c r="O24" s="153"/>
+      <c r="P24" s="153"/>
+      <c r="Q24" s="153"/>
     </row>
     <row r="25" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="137"/>
-      <c r="C25" s="138"/>
-      <c r="D25" s="138"/>
-      <c r="E25" s="138"/>
-      <c r="F25" s="138"/>
-      <c r="G25" s="138"/>
-      <c r="H25" s="138"/>
-      <c r="I25" s="138"/>
-      <c r="J25" s="138"/>
-      <c r="K25" s="139"/>
-      <c r="L25" s="143">
+      <c r="B25" s="144"/>
+      <c r="C25" s="145"/>
+      <c r="D25" s="145"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
+      <c r="H25" s="145"/>
+      <c r="I25" s="145"/>
+      <c r="J25" s="145"/>
+      <c r="K25" s="146"/>
+      <c r="L25" s="127">
         <v>2</v>
       </c>
-      <c r="M25" s="144" t="s">
+      <c r="M25" s="135" t="s">
+        <v>200</v>
+      </c>
+      <c r="N25" s="136"/>
+      <c r="O25" s="152" t="s">
+        <v>177</v>
+      </c>
+      <c r="P25" s="153"/>
+      <c r="Q25" s="153"/>
+    </row>
+    <row r="26" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="144"/>
+      <c r="C26" s="145"/>
+      <c r="D26" s="145"/>
+      <c r="E26" s="145"/>
+      <c r="F26" s="145"/>
+      <c r="G26" s="145"/>
+      <c r="H26" s="145"/>
+      <c r="I26" s="145"/>
+      <c r="J26" s="145"/>
+      <c r="K26" s="146"/>
+      <c r="L26" s="127"/>
+      <c r="M26" s="137"/>
+      <c r="N26" s="138"/>
+      <c r="O26" s="153"/>
+      <c r="P26" s="153"/>
+      <c r="Q26" s="153"/>
+    </row>
+    <row r="27" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="144"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
+      <c r="H27" s="145"/>
+      <c r="I27" s="145"/>
+      <c r="J27" s="145"/>
+      <c r="K27" s="146"/>
+      <c r="L27" s="127"/>
+      <c r="M27" s="137"/>
+      <c r="N27" s="138"/>
+      <c r="O27" s="153"/>
+      <c r="P27" s="153"/>
+      <c r="Q27" s="153"/>
+    </row>
+    <row r="28" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="144"/>
+      <c r="C28" s="145"/>
+      <c r="D28" s="145"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="145"/>
+      <c r="H28" s="145"/>
+      <c r="I28" s="145"/>
+      <c r="J28" s="145"/>
+      <c r="K28" s="146"/>
+      <c r="L28" s="127"/>
+      <c r="M28" s="139"/>
+      <c r="N28" s="140"/>
+      <c r="O28" s="153"/>
+      <c r="P28" s="153"/>
+      <c r="Q28" s="153"/>
+    </row>
+    <row r="29" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="144"/>
+      <c r="C29" s="145"/>
+      <c r="D29" s="145"/>
+      <c r="E29" s="145"/>
+      <c r="F29" s="145"/>
+      <c r="G29" s="145"/>
+      <c r="H29" s="145"/>
+      <c r="I29" s="145"/>
+      <c r="J29" s="145"/>
+      <c r="K29" s="146"/>
+      <c r="L29" s="127">
+        <v>3</v>
+      </c>
+      <c r="M29" s="135" t="s">
         <v>201</v>
       </c>
-      <c r="N25" s="145"/>
-      <c r="O25" s="171" t="s">
-        <v>177</v>
-      </c>
-      <c r="P25" s="172"/>
-      <c r="Q25" s="172"/>
-    </row>
-    <row r="26" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="137"/>
-      <c r="C26" s="138"/>
-      <c r="D26" s="138"/>
-      <c r="E26" s="138"/>
-      <c r="F26" s="138"/>
-      <c r="G26" s="138"/>
-      <c r="H26" s="138"/>
-      <c r="I26" s="138"/>
-      <c r="J26" s="138"/>
-      <c r="K26" s="139"/>
-      <c r="L26" s="143"/>
-      <c r="M26" s="148"/>
-      <c r="N26" s="149"/>
-      <c r="O26" s="172"/>
-      <c r="P26" s="172"/>
-      <c r="Q26" s="172"/>
-    </row>
-    <row r="27" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="137"/>
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
-      <c r="E27" s="138"/>
-      <c r="F27" s="138"/>
-      <c r="G27" s="138"/>
-      <c r="H27" s="138"/>
-      <c r="I27" s="138"/>
-      <c r="J27" s="138"/>
-      <c r="K27" s="139"/>
-      <c r="L27" s="143"/>
-      <c r="M27" s="148"/>
-      <c r="N27" s="149"/>
-      <c r="O27" s="172"/>
-      <c r="P27" s="172"/>
-      <c r="Q27" s="172"/>
-    </row>
-    <row r="28" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="137"/>
-      <c r="C28" s="138"/>
-      <c r="D28" s="138"/>
-      <c r="E28" s="138"/>
-      <c r="F28" s="138"/>
-      <c r="G28" s="138"/>
-      <c r="H28" s="138"/>
-      <c r="I28" s="138"/>
-      <c r="J28" s="138"/>
-      <c r="K28" s="139"/>
-      <c r="L28" s="143"/>
-      <c r="M28" s="146"/>
-      <c r="N28" s="147"/>
-      <c r="O28" s="172"/>
-      <c r="P28" s="172"/>
-      <c r="Q28" s="172"/>
-    </row>
-    <row r="29" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="137"/>
-      <c r="C29" s="138"/>
-      <c r="D29" s="138"/>
-      <c r="E29" s="138"/>
-      <c r="F29" s="138"/>
-      <c r="G29" s="138"/>
-      <c r="H29" s="138"/>
-      <c r="I29" s="138"/>
-      <c r="J29" s="138"/>
-      <c r="K29" s="139"/>
-      <c r="L29" s="143">
-        <v>3</v>
-      </c>
-      <c r="M29" s="144" t="s">
+      <c r="N29" s="136"/>
+      <c r="O29" s="152" t="s">
+        <v>218</v>
+      </c>
+      <c r="P29" s="153"/>
+      <c r="Q29" s="153"/>
+    </row>
+    <row r="30" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="144"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
+      <c r="H30" s="145"/>
+      <c r="I30" s="145"/>
+      <c r="J30" s="145"/>
+      <c r="K30" s="146"/>
+      <c r="L30" s="127"/>
+      <c r="M30" s="137"/>
+      <c r="N30" s="138"/>
+      <c r="O30" s="153"/>
+      <c r="P30" s="153"/>
+      <c r="Q30" s="153"/>
+    </row>
+    <row r="31" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="144"/>
+      <c r="C31" s="145"/>
+      <c r="D31" s="145"/>
+      <c r="E31" s="145"/>
+      <c r="F31" s="145"/>
+      <c r="G31" s="145"/>
+      <c r="H31" s="145"/>
+      <c r="I31" s="145"/>
+      <c r="J31" s="145"/>
+      <c r="K31" s="146"/>
+      <c r="L31" s="127"/>
+      <c r="M31" s="137"/>
+      <c r="N31" s="138"/>
+      <c r="O31" s="153"/>
+      <c r="P31" s="153"/>
+      <c r="Q31" s="153"/>
+    </row>
+    <row r="32" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="144"/>
+      <c r="C32" s="145"/>
+      <c r="D32" s="145"/>
+      <c r="E32" s="145"/>
+      <c r="F32" s="145"/>
+      <c r="G32" s="145"/>
+      <c r="H32" s="145"/>
+      <c r="I32" s="145"/>
+      <c r="J32" s="145"/>
+      <c r="K32" s="146"/>
+      <c r="L32" s="127"/>
+      <c r="M32" s="139"/>
+      <c r="N32" s="140"/>
+      <c r="O32" s="153"/>
+      <c r="P32" s="153"/>
+      <c r="Q32" s="153"/>
+    </row>
+    <row r="33" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="144"/>
+      <c r="C33" s="145"/>
+      <c r="D33" s="145"/>
+      <c r="E33" s="145"/>
+      <c r="F33" s="145"/>
+      <c r="G33" s="145"/>
+      <c r="H33" s="145"/>
+      <c r="I33" s="145"/>
+      <c r="J33" s="145"/>
+      <c r="K33" s="146"/>
+      <c r="L33" s="127">
+        <v>4</v>
+      </c>
+      <c r="M33" s="135" t="s">
         <v>202</v>
       </c>
-      <c r="N29" s="145"/>
-      <c r="O29" s="171" t="s">
-        <v>219</v>
-      </c>
-      <c r="P29" s="172"/>
-      <c r="Q29" s="172"/>
-    </row>
-    <row r="30" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="137"/>
-      <c r="C30" s="138"/>
-      <c r="D30" s="138"/>
-      <c r="E30" s="138"/>
-      <c r="F30" s="138"/>
-      <c r="G30" s="138"/>
-      <c r="H30" s="138"/>
-      <c r="I30" s="138"/>
-      <c r="J30" s="138"/>
-      <c r="K30" s="139"/>
-      <c r="L30" s="143"/>
-      <c r="M30" s="148"/>
-      <c r="N30" s="149"/>
-      <c r="O30" s="172"/>
-      <c r="P30" s="172"/>
-      <c r="Q30" s="172"/>
-    </row>
-    <row r="31" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="137"/>
-      <c r="C31" s="138"/>
-      <c r="D31" s="138"/>
-      <c r="E31" s="138"/>
-      <c r="F31" s="138"/>
-      <c r="G31" s="138"/>
-      <c r="H31" s="138"/>
-      <c r="I31" s="138"/>
-      <c r="J31" s="138"/>
-      <c r="K31" s="139"/>
-      <c r="L31" s="143"/>
-      <c r="M31" s="148"/>
-      <c r="N31" s="149"/>
-      <c r="O31" s="172"/>
-      <c r="P31" s="172"/>
-      <c r="Q31" s="172"/>
-    </row>
-    <row r="32" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="137"/>
-      <c r="C32" s="138"/>
-      <c r="D32" s="138"/>
-      <c r="E32" s="138"/>
-      <c r="F32" s="138"/>
-      <c r="G32" s="138"/>
-      <c r="H32" s="138"/>
-      <c r="I32" s="138"/>
-      <c r="J32" s="138"/>
-      <c r="K32" s="139"/>
-      <c r="L32" s="143"/>
-      <c r="M32" s="146"/>
-      <c r="N32" s="147"/>
-      <c r="O32" s="172"/>
-      <c r="P32" s="172"/>
-      <c r="Q32" s="172"/>
-    </row>
-    <row r="33" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="137"/>
-      <c r="C33" s="138"/>
-      <c r="D33" s="138"/>
-      <c r="E33" s="138"/>
-      <c r="F33" s="138"/>
-      <c r="G33" s="138"/>
-      <c r="H33" s="138"/>
-      <c r="I33" s="138"/>
-      <c r="J33" s="138"/>
-      <c r="K33" s="139"/>
-      <c r="L33" s="143">
-        <v>4</v>
-      </c>
-      <c r="M33" s="144" t="s">
-        <v>203</v>
-      </c>
-      <c r="N33" s="145"/>
-      <c r="O33" s="171" t="s">
-        <v>216</v>
-      </c>
-      <c r="P33" s="172"/>
-      <c r="Q33" s="172"/>
+      <c r="N33" s="136"/>
+      <c r="O33" s="152" t="s">
+        <v>215</v>
+      </c>
+      <c r="P33" s="153"/>
+      <c r="Q33" s="153"/>
     </row>
     <row r="34" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="137"/>
-      <c r="C34" s="138"/>
-      <c r="D34" s="138"/>
-      <c r="E34" s="138"/>
-      <c r="F34" s="138"/>
-      <c r="G34" s="138"/>
-      <c r="H34" s="138"/>
-      <c r="I34" s="138"/>
-      <c r="J34" s="138"/>
-      <c r="K34" s="139"/>
-      <c r="L34" s="143"/>
-      <c r="M34" s="148"/>
-      <c r="N34" s="149"/>
-      <c r="O34" s="172"/>
-      <c r="P34" s="172"/>
-      <c r="Q34" s="172"/>
+      <c r="B34" s="144"/>
+      <c r="C34" s="145"/>
+      <c r="D34" s="145"/>
+      <c r="E34" s="145"/>
+      <c r="F34" s="145"/>
+      <c r="G34" s="145"/>
+      <c r="H34" s="145"/>
+      <c r="I34" s="145"/>
+      <c r="J34" s="145"/>
+      <c r="K34" s="146"/>
+      <c r="L34" s="127"/>
+      <c r="M34" s="137"/>
+      <c r="N34" s="138"/>
+      <c r="O34" s="153"/>
+      <c r="P34" s="153"/>
+      <c r="Q34" s="153"/>
     </row>
     <row r="35" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="137"/>
-      <c r="C35" s="138"/>
-      <c r="D35" s="138"/>
-      <c r="E35" s="138"/>
-      <c r="F35" s="138"/>
-      <c r="G35" s="138"/>
-      <c r="H35" s="138"/>
-      <c r="I35" s="138"/>
-      <c r="J35" s="138"/>
-      <c r="K35" s="139"/>
-      <c r="L35" s="143"/>
-      <c r="M35" s="148"/>
-      <c r="N35" s="149"/>
-      <c r="O35" s="172"/>
-      <c r="P35" s="172"/>
-      <c r="Q35" s="172"/>
+      <c r="B35" s="144"/>
+      <c r="C35" s="145"/>
+      <c r="D35" s="145"/>
+      <c r="E35" s="145"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="145"/>
+      <c r="H35" s="145"/>
+      <c r="I35" s="145"/>
+      <c r="J35" s="145"/>
+      <c r="K35" s="146"/>
+      <c r="L35" s="127"/>
+      <c r="M35" s="137"/>
+      <c r="N35" s="138"/>
+      <c r="O35" s="153"/>
+      <c r="P35" s="153"/>
+      <c r="Q35" s="153"/>
     </row>
     <row r="36" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="140"/>
-      <c r="C36" s="141"/>
-      <c r="D36" s="141"/>
-      <c r="E36" s="141"/>
-      <c r="F36" s="141"/>
-      <c r="G36" s="141"/>
-      <c r="H36" s="141"/>
-      <c r="I36" s="141"/>
-      <c r="J36" s="141"/>
-      <c r="K36" s="142"/>
-      <c r="L36" s="143"/>
-      <c r="M36" s="146"/>
-      <c r="N36" s="147"/>
-      <c r="O36" s="172"/>
-      <c r="P36" s="172"/>
-      <c r="Q36" s="172"/>
+      <c r="B36" s="147"/>
+      <c r="C36" s="148"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="148"/>
+      <c r="G36" s="148"/>
+      <c r="H36" s="148"/>
+      <c r="I36" s="148"/>
+      <c r="J36" s="148"/>
+      <c r="K36" s="149"/>
+      <c r="L36" s="127"/>
+      <c r="M36" s="139"/>
+      <c r="N36" s="140"/>
+      <c r="O36" s="153"/>
+      <c r="P36" s="153"/>
+      <c r="Q36" s="153"/>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B38" s="128" t="s">
+      <c r="B38" s="131" t="s">
         <v>174</v>
       </c>
-      <c r="C38" s="126"/>
-      <c r="D38" s="126"/>
-      <c r="E38" s="126"/>
-      <c r="F38" s="127"/>
-      <c r="G38" s="129" t="s">
+      <c r="C38" s="132"/>
+      <c r="D38" s="132"/>
+      <c r="E38" s="132"/>
+      <c r="F38" s="128"/>
+      <c r="G38" s="133" t="s">
         <v>180</v>
       </c>
-      <c r="H38" s="129"/>
-      <c r="I38" s="129"/>
-      <c r="J38" s="129"/>
-      <c r="K38" s="130"/>
+      <c r="H38" s="133"/>
+      <c r="I38" s="133"/>
+      <c r="J38" s="133"/>
+      <c r="K38" s="134"/>
       <c r="L38" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="M38" s="133" t="s">
-        <v>193</v>
-      </c>
-      <c r="N38" s="169"/>
-      <c r="O38" s="127" t="s">
+      <c r="M38" s="130" t="s">
+        <v>192</v>
+      </c>
+      <c r="N38" s="172"/>
+      <c r="O38" s="128" t="s">
         <v>173</v>
       </c>
-      <c r="P38" s="132"/>
-      <c r="Q38" s="133"/>
-    </row>
-    <row r="39" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="134"/>
-      <c r="C39" s="135"/>
-      <c r="D39" s="135"/>
-      <c r="E39" s="135"/>
-      <c r="F39" s="135"/>
-      <c r="G39" s="135"/>
-      <c r="H39" s="135"/>
-      <c r="I39" s="135"/>
-      <c r="J39" s="135"/>
-      <c r="K39" s="136"/>
-      <c r="L39" s="144">
+      <c r="P38" s="129"/>
+      <c r="Q38" s="130"/>
+    </row>
+    <row r="39" spans="2:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="141"/>
+      <c r="C39" s="142"/>
+      <c r="D39" s="142"/>
+      <c r="E39" s="142"/>
+      <c r="F39" s="142"/>
+      <c r="G39" s="142"/>
+      <c r="H39" s="142"/>
+      <c r="I39" s="142"/>
+      <c r="J39" s="142"/>
+      <c r="K39" s="143"/>
+      <c r="L39" s="135">
         <v>1</v>
       </c>
-      <c r="M39" s="143" t="s">
+      <c r="M39" s="127" t="s">
+        <v>203</v>
+      </c>
+      <c r="N39" s="127"/>
+      <c r="O39" s="155" t="s">
+        <v>176</v>
+      </c>
+      <c r="P39" s="155"/>
+      <c r="Q39" s="156"/>
+    </row>
+    <row r="40" spans="2:17" ht="9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="144"/>
+      <c r="C40" s="145"/>
+      <c r="D40" s="145"/>
+      <c r="E40" s="145"/>
+      <c r="F40" s="145"/>
+      <c r="G40" s="145"/>
+      <c r="H40" s="145"/>
+      <c r="I40" s="145"/>
+      <c r="J40" s="145"/>
+      <c r="K40" s="146"/>
+      <c r="L40" s="139"/>
+      <c r="M40" s="127"/>
+      <c r="N40" s="127"/>
+      <c r="O40" s="157"/>
+      <c r="P40" s="157"/>
+      <c r="Q40" s="158"/>
+    </row>
+    <row r="41" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="144"/>
+      <c r="C41" s="145"/>
+      <c r="D41" s="145"/>
+      <c r="E41" s="145"/>
+      <c r="F41" s="145"/>
+      <c r="G41" s="145"/>
+      <c r="H41" s="145"/>
+      <c r="I41" s="145"/>
+      <c r="J41" s="145"/>
+      <c r="K41" s="146"/>
+      <c r="L41" s="135">
+        <v>2</v>
+      </c>
+      <c r="M41" s="127" t="s">
+        <v>200</v>
+      </c>
+      <c r="N41" s="127"/>
+      <c r="O41" s="154" t="s">
+        <v>178</v>
+      </c>
+      <c r="P41" s="155"/>
+      <c r="Q41" s="156"/>
+    </row>
+    <row r="42" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="144"/>
+      <c r="C42" s="145"/>
+      <c r="D42" s="145"/>
+      <c r="E42" s="145"/>
+      <c r="F42" s="145"/>
+      <c r="G42" s="145"/>
+      <c r="H42" s="145"/>
+      <c r="I42" s="145"/>
+      <c r="J42" s="145"/>
+      <c r="K42" s="146"/>
+      <c r="L42" s="139"/>
+      <c r="M42" s="127"/>
+      <c r="N42" s="127"/>
+      <c r="O42" s="157"/>
+      <c r="P42" s="157"/>
+      <c r="Q42" s="158"/>
+    </row>
+    <row r="43" spans="2:17" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="144"/>
+      <c r="C43" s="145"/>
+      <c r="D43" s="145"/>
+      <c r="E43" s="145"/>
+      <c r="F43" s="145"/>
+      <c r="G43" s="145"/>
+      <c r="H43" s="145"/>
+      <c r="I43" s="145"/>
+      <c r="J43" s="145"/>
+      <c r="K43" s="146"/>
+      <c r="L43" s="135">
+        <v>3</v>
+      </c>
+      <c r="M43" s="127" t="s">
+        <v>201</v>
+      </c>
+      <c r="N43" s="127"/>
+      <c r="O43" s="154" t="s">
+        <v>218</v>
+      </c>
+      <c r="P43" s="154"/>
+      <c r="Q43" s="159"/>
+    </row>
+    <row r="44" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B44" s="144"/>
+      <c r="C44" s="145"/>
+      <c r="D44" s="145"/>
+      <c r="E44" s="145"/>
+      <c r="F44" s="145"/>
+      <c r="G44" s="145"/>
+      <c r="H44" s="145"/>
+      <c r="I44" s="145"/>
+      <c r="J44" s="145"/>
+      <c r="K44" s="146"/>
+      <c r="L44" s="139"/>
+      <c r="M44" s="127"/>
+      <c r="N44" s="127"/>
+      <c r="O44" s="160"/>
+      <c r="P44" s="160"/>
+      <c r="Q44" s="161"/>
+    </row>
+    <row r="45" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="144"/>
+      <c r="C45" s="145"/>
+      <c r="D45" s="145"/>
+      <c r="E45" s="145"/>
+      <c r="F45" s="145"/>
+      <c r="G45" s="145"/>
+      <c r="H45" s="145"/>
+      <c r="I45" s="145"/>
+      <c r="J45" s="145"/>
+      <c r="K45" s="146"/>
+      <c r="L45" s="135">
+        <v>4</v>
+      </c>
+      <c r="M45" s="127" t="s">
+        <v>208</v>
+      </c>
+      <c r="N45" s="127"/>
+      <c r="O45" s="174" t="s">
+        <v>222</v>
+      </c>
+      <c r="P45" s="155"/>
+      <c r="Q45" s="156"/>
+    </row>
+    <row r="46" spans="2:17" ht="52.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="144"/>
+      <c r="C46" s="145"/>
+      <c r="D46" s="145"/>
+      <c r="E46" s="145"/>
+      <c r="F46" s="145"/>
+      <c r="G46" s="145"/>
+      <c r="H46" s="145"/>
+      <c r="I46" s="145"/>
+      <c r="J46" s="145"/>
+      <c r="K46" s="146"/>
+      <c r="L46" s="139"/>
+      <c r="M46" s="127"/>
+      <c r="N46" s="127"/>
+      <c r="O46" s="157"/>
+      <c r="P46" s="157"/>
+      <c r="Q46" s="158"/>
+    </row>
+    <row r="47" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="144"/>
+      <c r="C47" s="145"/>
+      <c r="D47" s="145"/>
+      <c r="E47" s="145"/>
+      <c r="F47" s="145"/>
+      <c r="G47" s="145"/>
+      <c r="H47" s="145"/>
+      <c r="I47" s="145"/>
+      <c r="J47" s="145"/>
+      <c r="K47" s="146"/>
+      <c r="L47" s="135">
+        <v>5</v>
+      </c>
+      <c r="M47" s="127" t="s">
+        <v>200</v>
+      </c>
+      <c r="N47" s="127"/>
+      <c r="O47" s="155" t="s">
+        <v>182</v>
+      </c>
+      <c r="P47" s="155"/>
+      <c r="Q47" s="156"/>
+    </row>
+    <row r="48" spans="2:17" ht="3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B48" s="144"/>
+      <c r="C48" s="145"/>
+      <c r="D48" s="145"/>
+      <c r="E48" s="145"/>
+      <c r="F48" s="145"/>
+      <c r="G48" s="145"/>
+      <c r="H48" s="145"/>
+      <c r="I48" s="145"/>
+      <c r="J48" s="145"/>
+      <c r="K48" s="146"/>
+      <c r="L48" s="139"/>
+      <c r="M48" s="127"/>
+      <c r="N48" s="127"/>
+      <c r="O48" s="157"/>
+      <c r="P48" s="157"/>
+      <c r="Q48" s="158"/>
+    </row>
+    <row r="49" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B49" s="144"/>
+      <c r="C49" s="145"/>
+      <c r="D49" s="145"/>
+      <c r="E49" s="145"/>
+      <c r="F49" s="145"/>
+      <c r="G49" s="145"/>
+      <c r="H49" s="145"/>
+      <c r="I49" s="145"/>
+      <c r="J49" s="145"/>
+      <c r="K49" s="146"/>
+      <c r="L49" s="135">
+        <v>6</v>
+      </c>
+      <c r="M49" s="127" t="s">
+        <v>200</v>
+      </c>
+      <c r="N49" s="127"/>
+      <c r="O49" s="154" t="s">
+        <v>183</v>
+      </c>
+      <c r="P49" s="155"/>
+      <c r="Q49" s="156"/>
+    </row>
+    <row r="50" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B50" s="144"/>
+      <c r="C50" s="145"/>
+      <c r="D50" s="145"/>
+      <c r="E50" s="145"/>
+      <c r="F50" s="145"/>
+      <c r="G50" s="145"/>
+      <c r="H50" s="145"/>
+      <c r="I50" s="145"/>
+      <c r="J50" s="145"/>
+      <c r="K50" s="146"/>
+      <c r="L50" s="139"/>
+      <c r="M50" s="127"/>
+      <c r="N50" s="127"/>
+      <c r="O50" s="157"/>
+      <c r="P50" s="157"/>
+      <c r="Q50" s="158"/>
+    </row>
+    <row r="51" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B51" s="144"/>
+      <c r="C51" s="145"/>
+      <c r="D51" s="145"/>
+      <c r="E51" s="145"/>
+      <c r="F51" s="145"/>
+      <c r="G51" s="145"/>
+      <c r="H51" s="145"/>
+      <c r="I51" s="145"/>
+      <c r="J51" s="145"/>
+      <c r="K51" s="146"/>
+      <c r="L51" s="135">
+        <v>7</v>
+      </c>
+      <c r="M51" s="127" t="s">
         <v>204</v>
       </c>
-      <c r="N39" s="143"/>
-      <c r="O39" s="151" t="s">
-        <v>176</v>
-      </c>
-      <c r="P39" s="151"/>
-      <c r="Q39" s="152"/>
-    </row>
-    <row r="40" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="137"/>
-      <c r="C40" s="138"/>
-      <c r="D40" s="138"/>
-      <c r="E40" s="138"/>
-      <c r="F40" s="138"/>
-      <c r="G40" s="138"/>
-      <c r="H40" s="138"/>
-      <c r="I40" s="138"/>
-      <c r="J40" s="138"/>
-      <c r="K40" s="139"/>
-      <c r="L40" s="146"/>
-      <c r="M40" s="143"/>
-      <c r="N40" s="143"/>
-      <c r="O40" s="154"/>
-      <c r="P40" s="154"/>
-      <c r="Q40" s="155"/>
-    </row>
-    <row r="41" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="137"/>
-      <c r="C41" s="138"/>
-      <c r="D41" s="138"/>
-      <c r="E41" s="138"/>
-      <c r="F41" s="138"/>
-      <c r="G41" s="138"/>
-      <c r="H41" s="138"/>
-      <c r="I41" s="138"/>
-      <c r="J41" s="138"/>
-      <c r="K41" s="139"/>
-      <c r="L41" s="144">
-        <v>2</v>
-      </c>
-      <c r="M41" s="143" t="s">
-        <v>201</v>
-      </c>
-      <c r="N41" s="143"/>
-      <c r="O41" s="156" t="s">
-        <v>178</v>
-      </c>
-      <c r="P41" s="151"/>
-      <c r="Q41" s="152"/>
-    </row>
-    <row r="42" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="137"/>
-      <c r="C42" s="138"/>
-      <c r="D42" s="138"/>
-      <c r="E42" s="138"/>
-      <c r="F42" s="138"/>
-      <c r="G42" s="138"/>
-      <c r="H42" s="138"/>
-      <c r="I42" s="138"/>
-      <c r="J42" s="138"/>
-      <c r="K42" s="139"/>
-      <c r="L42" s="146"/>
-      <c r="M42" s="143"/>
-      <c r="N42" s="143"/>
-      <c r="O42" s="154"/>
-      <c r="P42" s="154"/>
-      <c r="Q42" s="155"/>
-    </row>
-    <row r="43" spans="2:17" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="137"/>
-      <c r="C43" s="138"/>
-      <c r="D43" s="138"/>
-      <c r="E43" s="138"/>
-      <c r="F43" s="138"/>
-      <c r="G43" s="138"/>
-      <c r="H43" s="138"/>
-      <c r="I43" s="138"/>
-      <c r="J43" s="138"/>
-      <c r="K43" s="139"/>
-      <c r="L43" s="144">
-        <v>3</v>
-      </c>
-      <c r="M43" s="143" t="s">
-        <v>202</v>
-      </c>
-      <c r="N43" s="143"/>
-      <c r="O43" s="156" t="s">
-        <v>219</v>
-      </c>
-      <c r="P43" s="156"/>
-      <c r="Q43" s="157"/>
-    </row>
-    <row r="44" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="137"/>
-      <c r="C44" s="138"/>
-      <c r="D44" s="138"/>
-      <c r="E44" s="138"/>
-      <c r="F44" s="138"/>
-      <c r="G44" s="138"/>
-      <c r="H44" s="138"/>
-      <c r="I44" s="138"/>
-      <c r="J44" s="138"/>
-      <c r="K44" s="139"/>
-      <c r="L44" s="146"/>
-      <c r="M44" s="143"/>
-      <c r="N44" s="143"/>
-      <c r="O44" s="158"/>
-      <c r="P44" s="158"/>
-      <c r="Q44" s="159"/>
-    </row>
-    <row r="45" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="137"/>
-      <c r="C45" s="138"/>
-      <c r="D45" s="138"/>
-      <c r="E45" s="138"/>
-      <c r="F45" s="138"/>
-      <c r="G45" s="138"/>
-      <c r="H45" s="138"/>
-      <c r="I45" s="138"/>
-      <c r="J45" s="138"/>
-      <c r="K45" s="139"/>
-      <c r="L45" s="144">
-        <v>4</v>
-      </c>
-      <c r="M45" s="143" t="s">
-        <v>209</v>
-      </c>
-      <c r="N45" s="143"/>
-      <c r="O45" s="156" t="s">
+      <c r="N51" s="127"/>
+      <c r="O51" s="154" t="s">
         <v>223</v>
       </c>
-      <c r="P45" s="151"/>
-      <c r="Q45" s="152"/>
-    </row>
-    <row r="46" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="137"/>
-      <c r="C46" s="138"/>
-      <c r="D46" s="138"/>
-      <c r="E46" s="138"/>
-      <c r="F46" s="138"/>
-      <c r="G46" s="138"/>
-      <c r="H46" s="138"/>
-      <c r="I46" s="138"/>
-      <c r="J46" s="138"/>
-      <c r="K46" s="139"/>
-      <c r="L46" s="146"/>
-      <c r="M46" s="143"/>
-      <c r="N46" s="143"/>
-      <c r="O46" s="154"/>
-      <c r="P46" s="154"/>
-      <c r="Q46" s="155"/>
-    </row>
-    <row r="47" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="137"/>
-      <c r="C47" s="138"/>
-      <c r="D47" s="138"/>
-      <c r="E47" s="138"/>
-      <c r="F47" s="138"/>
-      <c r="G47" s="138"/>
-      <c r="H47" s="138"/>
-      <c r="I47" s="138"/>
-      <c r="J47" s="138"/>
-      <c r="K47" s="139"/>
-      <c r="L47" s="144">
-        <v>5</v>
-      </c>
-      <c r="M47" s="143" t="s">
-        <v>201</v>
-      </c>
-      <c r="N47" s="143"/>
-      <c r="O47" s="151" t="s">
-        <v>182</v>
-      </c>
-      <c r="P47" s="151"/>
-      <c r="Q47" s="152"/>
-    </row>
-    <row r="48" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="137"/>
-      <c r="C48" s="138"/>
-      <c r="D48" s="138"/>
-      <c r="E48" s="138"/>
-      <c r="F48" s="138"/>
-      <c r="G48" s="138"/>
-      <c r="H48" s="138"/>
-      <c r="I48" s="138"/>
-      <c r="J48" s="138"/>
-      <c r="K48" s="139"/>
-      <c r="L48" s="146"/>
-      <c r="M48" s="143"/>
-      <c r="N48" s="143"/>
-      <c r="O48" s="154"/>
-      <c r="P48" s="154"/>
-      <c r="Q48" s="155"/>
-    </row>
-    <row r="49" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B49" s="137"/>
-      <c r="C49" s="138"/>
-      <c r="D49" s="138"/>
-      <c r="E49" s="138"/>
-      <c r="F49" s="138"/>
-      <c r="G49" s="138"/>
-      <c r="H49" s="138"/>
-      <c r="I49" s="138"/>
-      <c r="J49" s="138"/>
-      <c r="K49" s="139"/>
-      <c r="L49" s="144">
-        <v>6</v>
-      </c>
-      <c r="M49" s="143" t="s">
-        <v>201</v>
-      </c>
-      <c r="N49" s="143"/>
-      <c r="O49" s="156" t="s">
+      <c r="P51" s="154"/>
+      <c r="Q51" s="159"/>
+    </row>
+    <row r="52" spans="2:17" ht="2.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B52" s="144"/>
+      <c r="C52" s="145"/>
+      <c r="D52" s="145"/>
+      <c r="E52" s="145"/>
+      <c r="F52" s="145"/>
+      <c r="G52" s="145"/>
+      <c r="H52" s="145"/>
+      <c r="I52" s="145"/>
+      <c r="J52" s="145"/>
+      <c r="K52" s="146"/>
+      <c r="L52" s="139"/>
+      <c r="M52" s="127"/>
+      <c r="N52" s="127"/>
+      <c r="O52" s="160"/>
+      <c r="P52" s="160"/>
+      <c r="Q52" s="161"/>
+    </row>
+    <row r="53" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="144"/>
+      <c r="C53" s="145"/>
+      <c r="D53" s="145"/>
+      <c r="E53" s="145"/>
+      <c r="F53" s="145"/>
+      <c r="G53" s="145"/>
+      <c r="H53" s="145"/>
+      <c r="I53" s="145"/>
+      <c r="J53" s="145"/>
+      <c r="K53" s="146"/>
+      <c r="L53" s="135">
+        <v>8</v>
+      </c>
+      <c r="M53" s="127" t="s">
+        <v>206</v>
+      </c>
+      <c r="N53" s="127"/>
+      <c r="O53" s="154" t="s">
         <v>184</v>
       </c>
-      <c r="P49" s="151"/>
-      <c r="Q49" s="152"/>
-    </row>
-    <row r="50" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="137"/>
-      <c r="C50" s="138"/>
-      <c r="D50" s="138"/>
-      <c r="E50" s="138"/>
-      <c r="F50" s="138"/>
-      <c r="G50" s="138"/>
-      <c r="H50" s="138"/>
-      <c r="I50" s="138"/>
-      <c r="J50" s="138"/>
-      <c r="K50" s="139"/>
-      <c r="L50" s="146"/>
-      <c r="M50" s="143"/>
-      <c r="N50" s="143"/>
-      <c r="O50" s="154"/>
-      <c r="P50" s="154"/>
-      <c r="Q50" s="155"/>
-    </row>
-    <row r="51" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="137"/>
-      <c r="C51" s="138"/>
-      <c r="D51" s="138"/>
-      <c r="E51" s="138"/>
-      <c r="F51" s="138"/>
-      <c r="G51" s="138"/>
-      <c r="H51" s="138"/>
-      <c r="I51" s="138"/>
-      <c r="J51" s="138"/>
-      <c r="K51" s="139"/>
-      <c r="L51" s="144">
-        <v>7</v>
-      </c>
-      <c r="M51" s="143" t="s">
-        <v>205</v>
-      </c>
-      <c r="N51" s="143"/>
-      <c r="O51" s="156" t="s">
-        <v>183</v>
-      </c>
-      <c r="P51" s="156"/>
-      <c r="Q51" s="157"/>
-    </row>
-    <row r="52" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="137"/>
-      <c r="C52" s="138"/>
-      <c r="D52" s="138"/>
-      <c r="E52" s="138"/>
-      <c r="F52" s="138"/>
-      <c r="G52" s="138"/>
-      <c r="H52" s="138"/>
-      <c r="I52" s="138"/>
-      <c r="J52" s="138"/>
-      <c r="K52" s="139"/>
-      <c r="L52" s="146"/>
-      <c r="M52" s="143"/>
-      <c r="N52" s="143"/>
-      <c r="O52" s="158"/>
-      <c r="P52" s="158"/>
-      <c r="Q52" s="159"/>
-    </row>
-    <row r="53" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="137"/>
-      <c r="C53" s="138"/>
-      <c r="D53" s="138"/>
-      <c r="E53" s="138"/>
-      <c r="F53" s="138"/>
-      <c r="G53" s="138"/>
-      <c r="H53" s="138"/>
-      <c r="I53" s="138"/>
-      <c r="J53" s="138"/>
-      <c r="K53" s="139"/>
-      <c r="L53" s="144">
-        <v>8</v>
-      </c>
-      <c r="M53" s="143" t="s">
-        <v>207</v>
-      </c>
-      <c r="N53" s="143"/>
-      <c r="O53" s="156" t="s">
-        <v>185</v>
-      </c>
-      <c r="P53" s="151"/>
-      <c r="Q53" s="152"/>
-    </row>
-    <row r="54" spans="2:17" ht="99.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="140"/>
-      <c r="C54" s="141"/>
-      <c r="D54" s="141"/>
-      <c r="E54" s="141"/>
-      <c r="F54" s="141"/>
-      <c r="G54" s="141"/>
-      <c r="H54" s="141"/>
-      <c r="I54" s="141"/>
-      <c r="J54" s="141"/>
-      <c r="K54" s="142"/>
-      <c r="L54" s="146"/>
-      <c r="M54" s="143"/>
-      <c r="N54" s="143"/>
-      <c r="O54" s="154"/>
-      <c r="P54" s="154"/>
-      <c r="Q54" s="155"/>
+      <c r="P53" s="155"/>
+      <c r="Q53" s="156"/>
+    </row>
+    <row r="54" spans="2:17" ht="91.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B54" s="147"/>
+      <c r="C54" s="148"/>
+      <c r="D54" s="148"/>
+      <c r="E54" s="148"/>
+      <c r="F54" s="148"/>
+      <c r="G54" s="148"/>
+      <c r="H54" s="148"/>
+      <c r="I54" s="148"/>
+      <c r="J54" s="148"/>
+      <c r="K54" s="149"/>
+      <c r="L54" s="139"/>
+      <c r="M54" s="127"/>
+      <c r="N54" s="127"/>
+      <c r="O54" s="157"/>
+      <c r="P54" s="157"/>
+      <c r="Q54" s="158"/>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B56" s="128" t="s">
+      <c r="B56" s="131" t="s">
         <v>174</v>
       </c>
-      <c r="C56" s="126"/>
-      <c r="D56" s="126"/>
-      <c r="E56" s="126"/>
-      <c r="F56" s="127"/>
-      <c r="G56" s="129" t="s">
-        <v>192</v>
-      </c>
-      <c r="H56" s="129"/>
-      <c r="I56" s="129"/>
-      <c r="J56" s="129"/>
-      <c r="K56" s="130"/>
+      <c r="C56" s="132"/>
+      <c r="D56" s="132"/>
+      <c r="E56" s="132"/>
+      <c r="F56" s="128"/>
+      <c r="G56" s="133" t="s">
+        <v>191</v>
+      </c>
+      <c r="H56" s="133"/>
+      <c r="I56" s="133"/>
+      <c r="J56" s="133"/>
+      <c r="K56" s="134"/>
       <c r="L56" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="M56" s="131" t="s">
-        <v>193</v>
-      </c>
-      <c r="N56" s="127"/>
-      <c r="O56" s="132" t="s">
+      <c r="M56" s="150" t="s">
+        <v>192</v>
+      </c>
+      <c r="N56" s="128"/>
+      <c r="O56" s="129" t="s">
         <v>173</v>
       </c>
-      <c r="P56" s="132"/>
-      <c r="Q56" s="133"/>
+      <c r="P56" s="129"/>
+      <c r="Q56" s="130"/>
     </row>
     <row r="57" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B57" s="134"/>
-      <c r="C57" s="135"/>
-      <c r="D57" s="135"/>
-      <c r="E57" s="135"/>
-      <c r="F57" s="135"/>
-      <c r="G57" s="135"/>
-      <c r="H57" s="135"/>
-      <c r="I57" s="135"/>
-      <c r="J57" s="135"/>
-      <c r="K57" s="136"/>
-      <c r="L57" s="143">
+      <c r="B57" s="141"/>
+      <c r="C57" s="142"/>
+      <c r="D57" s="142"/>
+      <c r="E57" s="142"/>
+      <c r="F57" s="142"/>
+      <c r="G57" s="142"/>
+      <c r="H57" s="142"/>
+      <c r="I57" s="142"/>
+      <c r="J57" s="142"/>
+      <c r="K57" s="143"/>
+      <c r="L57" s="127">
         <v>1</v>
       </c>
-      <c r="M57" s="144" t="s">
-        <v>204</v>
-      </c>
-      <c r="N57" s="145"/>
-      <c r="O57" s="150" t="s">
+      <c r="M57" s="135" t="s">
+        <v>203</v>
+      </c>
+      <c r="N57" s="136"/>
+      <c r="O57" s="162" t="s">
         <v>176</v>
       </c>
-      <c r="P57" s="151"/>
-      <c r="Q57" s="152"/>
+      <c r="P57" s="155"/>
+      <c r="Q57" s="156"/>
     </row>
     <row r="58" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="137"/>
-      <c r="C58" s="138"/>
-      <c r="D58" s="138"/>
-      <c r="E58" s="138"/>
-      <c r="F58" s="138"/>
-      <c r="G58" s="138"/>
-      <c r="H58" s="138"/>
-      <c r="I58" s="138"/>
-      <c r="J58" s="138"/>
-      <c r="K58" s="139"/>
-      <c r="L58" s="143"/>
-      <c r="M58" s="146"/>
-      <c r="N58" s="147"/>
-      <c r="O58" s="153"/>
-      <c r="P58" s="154"/>
-      <c r="Q58" s="155"/>
+      <c r="B58" s="144"/>
+      <c r="C58" s="145"/>
+      <c r="D58" s="145"/>
+      <c r="E58" s="145"/>
+      <c r="F58" s="145"/>
+      <c r="G58" s="145"/>
+      <c r="H58" s="145"/>
+      <c r="I58" s="145"/>
+      <c r="J58" s="145"/>
+      <c r="K58" s="146"/>
+      <c r="L58" s="127"/>
+      <c r="M58" s="139"/>
+      <c r="N58" s="140"/>
+      <c r="O58" s="163"/>
+      <c r="P58" s="157"/>
+      <c r="Q58" s="158"/>
     </row>
     <row r="59" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B59" s="137"/>
-      <c r="C59" s="138"/>
-      <c r="D59" s="138"/>
-      <c r="E59" s="138"/>
-      <c r="F59" s="138"/>
-      <c r="G59" s="138"/>
-      <c r="H59" s="138"/>
-      <c r="I59" s="138"/>
-      <c r="J59" s="138"/>
-      <c r="K59" s="139"/>
-      <c r="L59" s="143">
+      <c r="B59" s="144"/>
+      <c r="C59" s="145"/>
+      <c r="D59" s="145"/>
+      <c r="E59" s="145"/>
+      <c r="F59" s="145"/>
+      <c r="G59" s="145"/>
+      <c r="H59" s="145"/>
+      <c r="I59" s="145"/>
+      <c r="J59" s="145"/>
+      <c r="K59" s="146"/>
+      <c r="L59" s="127">
         <v>2</v>
       </c>
-      <c r="M59" s="144" t="s">
-        <v>202</v>
-      </c>
-      <c r="N59" s="145"/>
-      <c r="O59" s="156" t="s">
-        <v>219</v>
-      </c>
-      <c r="P59" s="156"/>
-      <c r="Q59" s="157"/>
+      <c r="M59" s="135" t="s">
+        <v>201</v>
+      </c>
+      <c r="N59" s="136"/>
+      <c r="O59" s="154" t="s">
+        <v>218</v>
+      </c>
+      <c r="P59" s="154"/>
+      <c r="Q59" s="159"/>
     </row>
     <row r="60" spans="2:17" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B60" s="137"/>
-      <c r="C60" s="138"/>
-      <c r="D60" s="138"/>
-      <c r="E60" s="138"/>
-      <c r="F60" s="138"/>
-      <c r="G60" s="138"/>
-      <c r="H60" s="138"/>
-      <c r="I60" s="138"/>
-      <c r="J60" s="138"/>
-      <c r="K60" s="139"/>
-      <c r="L60" s="143"/>
-      <c r="M60" s="146"/>
-      <c r="N60" s="147"/>
-      <c r="O60" s="158"/>
-      <c r="P60" s="158"/>
-      <c r="Q60" s="159"/>
+      <c r="B60" s="144"/>
+      <c r="C60" s="145"/>
+      <c r="D60" s="145"/>
+      <c r="E60" s="145"/>
+      <c r="F60" s="145"/>
+      <c r="G60" s="145"/>
+      <c r="H60" s="145"/>
+      <c r="I60" s="145"/>
+      <c r="J60" s="145"/>
+      <c r="K60" s="146"/>
+      <c r="L60" s="127"/>
+      <c r="M60" s="139"/>
+      <c r="N60" s="140"/>
+      <c r="O60" s="160"/>
+      <c r="P60" s="160"/>
+      <c r="Q60" s="161"/>
     </row>
     <row r="61" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="137"/>
-      <c r="C61" s="138"/>
-      <c r="D61" s="138"/>
-      <c r="E61" s="138"/>
-      <c r="F61" s="138"/>
-      <c r="G61" s="138"/>
-      <c r="H61" s="138"/>
-      <c r="I61" s="138"/>
-      <c r="J61" s="138"/>
-      <c r="K61" s="139"/>
-      <c r="L61" s="143">
+      <c r="B61" s="144"/>
+      <c r="C61" s="145"/>
+      <c r="D61" s="145"/>
+      <c r="E61" s="145"/>
+      <c r="F61" s="145"/>
+      <c r="G61" s="145"/>
+      <c r="H61" s="145"/>
+      <c r="I61" s="145"/>
+      <c r="J61" s="145"/>
+      <c r="K61" s="146"/>
+      <c r="L61" s="127">
         <v>3</v>
       </c>
-      <c r="M61" s="144" t="s">
-        <v>201</v>
-      </c>
-      <c r="N61" s="145"/>
-      <c r="O61" s="150" t="s">
-        <v>206</v>
-      </c>
-      <c r="P61" s="156"/>
-      <c r="Q61" s="157"/>
+      <c r="M61" s="135" t="s">
+        <v>200</v>
+      </c>
+      <c r="N61" s="136"/>
+      <c r="O61" s="162" t="s">
+        <v>205</v>
+      </c>
+      <c r="P61" s="154"/>
+      <c r="Q61" s="159"/>
     </row>
     <row r="62" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="137"/>
-      <c r="C62" s="138"/>
-      <c r="D62" s="138"/>
-      <c r="E62" s="138"/>
-      <c r="F62" s="138"/>
-      <c r="G62" s="138"/>
-      <c r="H62" s="138"/>
-      <c r="I62" s="138"/>
-      <c r="J62" s="138"/>
-      <c r="K62" s="139"/>
-      <c r="L62" s="143"/>
-      <c r="M62" s="146"/>
-      <c r="N62" s="147"/>
+      <c r="B62" s="144"/>
+      <c r="C62" s="145"/>
+      <c r="D62" s="145"/>
+      <c r="E62" s="145"/>
+      <c r="F62" s="145"/>
+      <c r="G62" s="145"/>
+      <c r="H62" s="145"/>
+      <c r="I62" s="145"/>
+      <c r="J62" s="145"/>
+      <c r="K62" s="146"/>
+      <c r="L62" s="127"/>
+      <c r="M62" s="139"/>
+      <c r="N62" s="140"/>
       <c r="O62" s="164"/>
-      <c r="P62" s="158"/>
-      <c r="Q62" s="159"/>
+      <c r="P62" s="160"/>
+      <c r="Q62" s="161"/>
     </row>
     <row r="63" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="137"/>
-      <c r="C63" s="138"/>
-      <c r="D63" s="138"/>
-      <c r="E63" s="138"/>
-      <c r="F63" s="138"/>
-      <c r="G63" s="138"/>
-      <c r="H63" s="138"/>
-      <c r="I63" s="138"/>
-      <c r="J63" s="138"/>
-      <c r="K63" s="139"/>
-      <c r="L63" s="143">
+      <c r="B63" s="144"/>
+      <c r="C63" s="145"/>
+      <c r="D63" s="145"/>
+      <c r="E63" s="145"/>
+      <c r="F63" s="145"/>
+      <c r="G63" s="145"/>
+      <c r="H63" s="145"/>
+      <c r="I63" s="145"/>
+      <c r="J63" s="145"/>
+      <c r="K63" s="146"/>
+      <c r="L63" s="127">
         <v>4</v>
       </c>
-      <c r="M63" s="144" t="s">
+      <c r="M63" s="135" t="s">
+        <v>220</v>
+      </c>
+      <c r="N63" s="136"/>
+      <c r="O63" s="162" t="s">
         <v>221</v>
       </c>
-      <c r="N63" s="145"/>
-      <c r="O63" s="150" t="s">
-        <v>222</v>
-      </c>
-      <c r="P63" s="151"/>
-      <c r="Q63" s="152"/>
+      <c r="P63" s="155"/>
+      <c r="Q63" s="156"/>
     </row>
     <row r="64" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B64" s="137"/>
-      <c r="C64" s="138"/>
-      <c r="D64" s="138"/>
-      <c r="E64" s="138"/>
-      <c r="F64" s="138"/>
-      <c r="G64" s="138"/>
-      <c r="H64" s="138"/>
-      <c r="I64" s="138"/>
-      <c r="J64" s="138"/>
-      <c r="K64" s="139"/>
-      <c r="L64" s="143"/>
-      <c r="M64" s="146"/>
-      <c r="N64" s="147"/>
-      <c r="O64" s="153"/>
-      <c r="P64" s="154"/>
-      <c r="Q64" s="155"/>
+      <c r="B64" s="144"/>
+      <c r="C64" s="145"/>
+      <c r="D64" s="145"/>
+      <c r="E64" s="145"/>
+      <c r="F64" s="145"/>
+      <c r="G64" s="145"/>
+      <c r="H64" s="145"/>
+      <c r="I64" s="145"/>
+      <c r="J64" s="145"/>
+      <c r="K64" s="146"/>
+      <c r="L64" s="127"/>
+      <c r="M64" s="139"/>
+      <c r="N64" s="140"/>
+      <c r="O64" s="163"/>
+      <c r="P64" s="157"/>
+      <c r="Q64" s="158"/>
     </row>
     <row r="65" spans="2:17" ht="105" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B65" s="137"/>
-      <c r="C65" s="138"/>
-      <c r="D65" s="138"/>
-      <c r="E65" s="138"/>
-      <c r="F65" s="138"/>
-      <c r="G65" s="138"/>
-      <c r="H65" s="138"/>
-      <c r="I65" s="138"/>
-      <c r="J65" s="138"/>
-      <c r="K65" s="139"/>
-      <c r="L65" s="143">
+      <c r="B65" s="144"/>
+      <c r="C65" s="145"/>
+      <c r="D65" s="145"/>
+      <c r="E65" s="145"/>
+      <c r="F65" s="145"/>
+      <c r="G65" s="145"/>
+      <c r="H65" s="145"/>
+      <c r="I65" s="145"/>
+      <c r="J65" s="145"/>
+      <c r="K65" s="146"/>
+      <c r="L65" s="127">
         <v>5</v>
       </c>
-      <c r="M65" s="144" t="s">
+      <c r="M65" s="135" t="s">
+        <v>207</v>
+      </c>
+      <c r="N65" s="136"/>
+      <c r="O65" s="154" t="s">
+        <v>217</v>
+      </c>
+      <c r="P65" s="155"/>
+      <c r="Q65" s="156"/>
+    </row>
+    <row r="66" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B66" s="144"/>
+      <c r="C66" s="145"/>
+      <c r="D66" s="145"/>
+      <c r="E66" s="145"/>
+      <c r="F66" s="145"/>
+      <c r="G66" s="145"/>
+      <c r="H66" s="145"/>
+      <c r="I66" s="145"/>
+      <c r="J66" s="145"/>
+      <c r="K66" s="146"/>
+      <c r="L66" s="127"/>
+      <c r="M66" s="139"/>
+      <c r="N66" s="140"/>
+      <c r="O66" s="157"/>
+      <c r="P66" s="157"/>
+      <c r="Q66" s="158"/>
+    </row>
+    <row r="67" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B67" s="144"/>
+      <c r="C67" s="145"/>
+      <c r="D67" s="145"/>
+      <c r="E67" s="145"/>
+      <c r="F67" s="145"/>
+      <c r="G67" s="145"/>
+      <c r="H67" s="145"/>
+      <c r="I67" s="145"/>
+      <c r="J67" s="145"/>
+      <c r="K67" s="146"/>
+      <c r="L67" s="127">
+        <v>6</v>
+      </c>
+      <c r="M67" s="135" t="s">
         <v>208</v>
       </c>
-      <c r="N65" s="145"/>
-      <c r="O65" s="156" t="s">
-        <v>218</v>
-      </c>
-      <c r="P65" s="151"/>
-      <c r="Q65" s="152"/>
-    </row>
-    <row r="66" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B66" s="137"/>
-      <c r="C66" s="138"/>
-      <c r="D66" s="138"/>
-      <c r="E66" s="138"/>
-      <c r="F66" s="138"/>
-      <c r="G66" s="138"/>
-      <c r="H66" s="138"/>
-      <c r="I66" s="138"/>
-      <c r="J66" s="138"/>
-      <c r="K66" s="139"/>
-      <c r="L66" s="143"/>
-      <c r="M66" s="146"/>
-      <c r="N66" s="147"/>
-      <c r="O66" s="154"/>
-      <c r="P66" s="154"/>
-      <c r="Q66" s="155"/>
-    </row>
-    <row r="67" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B67" s="137"/>
-      <c r="C67" s="138"/>
-      <c r="D67" s="138"/>
-      <c r="E67" s="138"/>
-      <c r="F67" s="138"/>
-      <c r="G67" s="138"/>
-      <c r="H67" s="138"/>
-      <c r="I67" s="138"/>
-      <c r="J67" s="138"/>
-      <c r="K67" s="139"/>
-      <c r="L67" s="143">
-        <v>6</v>
-      </c>
-      <c r="M67" s="144" t="s">
+      <c r="N67" s="136"/>
+      <c r="O67" s="173" t="s">
         <v>209</v>
       </c>
-      <c r="N67" s="145"/>
-      <c r="O67" s="160" t="s">
-        <v>210</v>
-      </c>
-      <c r="P67" s="156"/>
-      <c r="Q67" s="157"/>
+      <c r="P67" s="154"/>
+      <c r="Q67" s="159"/>
     </row>
     <row r="68" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B68" s="137"/>
-      <c r="C68" s="138"/>
-      <c r="D68" s="138"/>
-      <c r="E68" s="138"/>
-      <c r="F68" s="138"/>
-      <c r="G68" s="138"/>
-      <c r="H68" s="138"/>
-      <c r="I68" s="138"/>
-      <c r="J68" s="138"/>
-      <c r="K68" s="139"/>
-      <c r="L68" s="143"/>
-      <c r="M68" s="148"/>
-      <c r="N68" s="149"/>
-      <c r="O68" s="161"/>
-      <c r="P68" s="162"/>
-      <c r="Q68" s="163"/>
+      <c r="B68" s="144"/>
+      <c r="C68" s="145"/>
+      <c r="D68" s="145"/>
+      <c r="E68" s="145"/>
+      <c r="F68" s="145"/>
+      <c r="G68" s="145"/>
+      <c r="H68" s="145"/>
+      <c r="I68" s="145"/>
+      <c r="J68" s="145"/>
+      <c r="K68" s="146"/>
+      <c r="L68" s="127"/>
+      <c r="M68" s="137"/>
+      <c r="N68" s="138"/>
+      <c r="O68" s="169"/>
+      <c r="P68" s="170"/>
+      <c r="Q68" s="171"/>
     </row>
     <row r="69" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B69" s="137"/>
-      <c r="C69" s="138"/>
-      <c r="D69" s="138"/>
-      <c r="E69" s="138"/>
-      <c r="F69" s="138"/>
-      <c r="G69" s="138"/>
-      <c r="H69" s="138"/>
-      <c r="I69" s="138"/>
-      <c r="J69" s="138"/>
-      <c r="K69" s="139"/>
-      <c r="L69" s="143"/>
-      <c r="M69" s="146"/>
-      <c r="N69" s="147"/>
+      <c r="B69" s="144"/>
+      <c r="C69" s="145"/>
+      <c r="D69" s="145"/>
+      <c r="E69" s="145"/>
+      <c r="F69" s="145"/>
+      <c r="G69" s="145"/>
+      <c r="H69" s="145"/>
+      <c r="I69" s="145"/>
+      <c r="J69" s="145"/>
+      <c r="K69" s="146"/>
+      <c r="L69" s="127"/>
+      <c r="M69" s="139"/>
+      <c r="N69" s="140"/>
       <c r="O69" s="164"/>
-      <c r="P69" s="158"/>
-      <c r="Q69" s="159"/>
+      <c r="P69" s="160"/>
+      <c r="Q69" s="161"/>
     </row>
     <row r="70" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B70" s="137"/>
-      <c r="C70" s="138"/>
-      <c r="D70" s="138"/>
-      <c r="E70" s="138"/>
-      <c r="F70" s="138"/>
-      <c r="G70" s="138"/>
-      <c r="H70" s="138"/>
-      <c r="I70" s="138"/>
-      <c r="J70" s="138"/>
-      <c r="K70" s="139"/>
-      <c r="L70" s="143">
+      <c r="B70" s="144"/>
+      <c r="C70" s="145"/>
+      <c r="D70" s="145"/>
+      <c r="E70" s="145"/>
+      <c r="F70" s="145"/>
+      <c r="G70" s="145"/>
+      <c r="H70" s="145"/>
+      <c r="I70" s="145"/>
+      <c r="J70" s="145"/>
+      <c r="K70" s="146"/>
+      <c r="L70" s="127">
         <v>7</v>
       </c>
-      <c r="M70" s="144" t="s">
+      <c r="M70" s="135" t="s">
+        <v>208</v>
+      </c>
+      <c r="N70" s="136"/>
+      <c r="O70" s="173" t="s">
         <v>209</v>
       </c>
-      <c r="N70" s="145"/>
-      <c r="O70" s="160" t="s">
-        <v>210</v>
-      </c>
-      <c r="P70" s="151"/>
-      <c r="Q70" s="152"/>
+      <c r="P70" s="155"/>
+      <c r="Q70" s="156"/>
     </row>
     <row r="71" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B71" s="137"/>
-      <c r="C71" s="138"/>
-      <c r="D71" s="138"/>
-      <c r="E71" s="138"/>
-      <c r="F71" s="138"/>
-      <c r="G71" s="138"/>
-      <c r="H71" s="138"/>
-      <c r="I71" s="138"/>
-      <c r="J71" s="138"/>
-      <c r="K71" s="139"/>
-      <c r="L71" s="143"/>
-      <c r="M71" s="148"/>
-      <c r="N71" s="149"/>
-      <c r="O71" s="165"/>
-      <c r="P71" s="166"/>
-      <c r="Q71" s="167"/>
+      <c r="B71" s="144"/>
+      <c r="C71" s="145"/>
+      <c r="D71" s="145"/>
+      <c r="E71" s="145"/>
+      <c r="F71" s="145"/>
+      <c r="G71" s="145"/>
+      <c r="H71" s="145"/>
+      <c r="I71" s="145"/>
+      <c r="J71" s="145"/>
+      <c r="K71" s="146"/>
+      <c r="L71" s="127"/>
+      <c r="M71" s="137"/>
+      <c r="N71" s="138"/>
+      <c r="O71" s="166"/>
+      <c r="P71" s="167"/>
+      <c r="Q71" s="168"/>
     </row>
     <row r="72" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B72" s="140"/>
-      <c r="C72" s="141"/>
-      <c r="D72" s="141"/>
-      <c r="E72" s="141"/>
-      <c r="F72" s="141"/>
-      <c r="G72" s="141"/>
-      <c r="H72" s="141"/>
-      <c r="I72" s="141"/>
-      <c r="J72" s="141"/>
-      <c r="K72" s="142"/>
-      <c r="L72" s="143"/>
-      <c r="M72" s="146"/>
-      <c r="N72" s="147"/>
-      <c r="O72" s="153"/>
-      <c r="P72" s="154"/>
-      <c r="Q72" s="155"/>
+      <c r="B72" s="147"/>
+      <c r="C72" s="148"/>
+      <c r="D72" s="148"/>
+      <c r="E72" s="148"/>
+      <c r="F72" s="148"/>
+      <c r="G72" s="148"/>
+      <c r="H72" s="148"/>
+      <c r="I72" s="148"/>
+      <c r="J72" s="148"/>
+      <c r="K72" s="149"/>
+      <c r="L72" s="127"/>
+      <c r="M72" s="139"/>
+      <c r="N72" s="140"/>
+      <c r="O72" s="163"/>
+      <c r="P72" s="157"/>
+      <c r="Q72" s="158"/>
     </row>
     <row r="74" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B74" s="128" t="s">
+      <c r="B74" s="131" t="s">
         <v>174</v>
       </c>
-      <c r="C74" s="126"/>
-      <c r="D74" s="126"/>
-      <c r="E74" s="126"/>
-      <c r="F74" s="127"/>
-      <c r="G74" s="129" t="s">
-        <v>215</v>
-      </c>
-      <c r="H74" s="129"/>
-      <c r="I74" s="129"/>
-      <c r="J74" s="129"/>
-      <c r="K74" s="130"/>
+      <c r="C74" s="132"/>
+      <c r="D74" s="132"/>
+      <c r="E74" s="132"/>
+      <c r="F74" s="128"/>
+      <c r="G74" s="133" t="s">
+        <v>214</v>
+      </c>
+      <c r="H74" s="133"/>
+      <c r="I74" s="133"/>
+      <c r="J74" s="133"/>
+      <c r="K74" s="134"/>
       <c r="L74" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="M74" s="131" t="s">
+      <c r="M74" s="150" t="s">
+        <v>192</v>
+      </c>
+      <c r="N74" s="128"/>
+      <c r="O74" s="129" t="s">
+        <v>173</v>
+      </c>
+      <c r="P74" s="129"/>
+      <c r="Q74" s="130"/>
+    </row>
+    <row r="75" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B75" s="141"/>
+      <c r="C75" s="142"/>
+      <c r="D75" s="142"/>
+      <c r="E75" s="142"/>
+      <c r="F75" s="142"/>
+      <c r="G75" s="142"/>
+      <c r="H75" s="142"/>
+      <c r="I75" s="142"/>
+      <c r="J75" s="142"/>
+      <c r="K75" s="143"/>
+      <c r="L75" s="127">
+        <v>1</v>
+      </c>
+      <c r="M75" s="127" t="s">
+        <v>210</v>
+      </c>
+      <c r="N75" s="127"/>
+      <c r="O75" s="126" t="s">
+        <v>213</v>
+      </c>
+      <c r="P75" s="126"/>
+      <c r="Q75" s="126"/>
+    </row>
+    <row r="76" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B76" s="144"/>
+      <c r="C76" s="145"/>
+      <c r="D76" s="145"/>
+      <c r="E76" s="145"/>
+      <c r="F76" s="145"/>
+      <c r="G76" s="145"/>
+      <c r="H76" s="145"/>
+      <c r="I76" s="145"/>
+      <c r="J76" s="145"/>
+      <c r="K76" s="146"/>
+      <c r="L76" s="127"/>
+      <c r="M76" s="127"/>
+      <c r="N76" s="127"/>
+      <c r="O76" s="126"/>
+      <c r="P76" s="126"/>
+      <c r="Q76" s="126"/>
+    </row>
+    <row r="77" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B77" s="144"/>
+      <c r="C77" s="145"/>
+      <c r="D77" s="145"/>
+      <c r="E77" s="145"/>
+      <c r="F77" s="145"/>
+      <c r="G77" s="145"/>
+      <c r="H77" s="145"/>
+      <c r="I77" s="145"/>
+      <c r="J77" s="145"/>
+      <c r="K77" s="146"/>
+      <c r="L77" s="127"/>
+      <c r="M77" s="127"/>
+      <c r="N77" s="127"/>
+      <c r="O77" s="126"/>
+      <c r="P77" s="126"/>
+      <c r="Q77" s="126"/>
+    </row>
+    <row r="78" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B78" s="144"/>
+      <c r="C78" s="145"/>
+      <c r="D78" s="145"/>
+      <c r="E78" s="145"/>
+      <c r="F78" s="145"/>
+      <c r="G78" s="145"/>
+      <c r="H78" s="145"/>
+      <c r="I78" s="145"/>
+      <c r="J78" s="145"/>
+      <c r="K78" s="146"/>
+      <c r="L78" s="127"/>
+      <c r="M78" s="127"/>
+      <c r="N78" s="127"/>
+      <c r="O78" s="126"/>
+      <c r="P78" s="126"/>
+      <c r="Q78" s="126"/>
+    </row>
+    <row r="79" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B79" s="144"/>
+      <c r="C79" s="145"/>
+      <c r="D79" s="145"/>
+      <c r="E79" s="145"/>
+      <c r="F79" s="145"/>
+      <c r="G79" s="145"/>
+      <c r="H79" s="145"/>
+      <c r="I79" s="145"/>
+      <c r="J79" s="145"/>
+      <c r="K79" s="146"/>
+      <c r="L79" s="127"/>
+      <c r="M79" s="127"/>
+      <c r="N79" s="127"/>
+      <c r="O79" s="126"/>
+      <c r="P79" s="126"/>
+      <c r="Q79" s="126"/>
+    </row>
+    <row r="80" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B80" s="144"/>
+      <c r="C80" s="145"/>
+      <c r="D80" s="145"/>
+      <c r="E80" s="145"/>
+      <c r="F80" s="145"/>
+      <c r="G80" s="145"/>
+      <c r="H80" s="145"/>
+      <c r="I80" s="145"/>
+      <c r="J80" s="145"/>
+      <c r="K80" s="146"/>
+      <c r="L80" s="127">
+        <v>2</v>
+      </c>
+      <c r="M80" s="127" t="s">
+        <v>211</v>
+      </c>
+      <c r="N80" s="127"/>
+      <c r="O80" s="126" t="s">
+        <v>212</v>
+      </c>
+      <c r="P80" s="126"/>
+      <c r="Q80" s="126"/>
+    </row>
+    <row r="81" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B81" s="144"/>
+      <c r="C81" s="145"/>
+      <c r="D81" s="145"/>
+      <c r="E81" s="145"/>
+      <c r="F81" s="145"/>
+      <c r="G81" s="145"/>
+      <c r="H81" s="145"/>
+      <c r="I81" s="145"/>
+      <c r="J81" s="145"/>
+      <c r="K81" s="146"/>
+      <c r="L81" s="127"/>
+      <c r="M81" s="127"/>
+      <c r="N81" s="127"/>
+      <c r="O81" s="126"/>
+      <c r="P81" s="126"/>
+      <c r="Q81" s="126"/>
+    </row>
+    <row r="82" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B82" s="144"/>
+      <c r="C82" s="145"/>
+      <c r="D82" s="145"/>
+      <c r="E82" s="145"/>
+      <c r="F82" s="145"/>
+      <c r="G82" s="145"/>
+      <c r="H82" s="145"/>
+      <c r="I82" s="145"/>
+      <c r="J82" s="145"/>
+      <c r="K82" s="146"/>
+      <c r="L82" s="127"/>
+      <c r="M82" s="127"/>
+      <c r="N82" s="127"/>
+      <c r="O82" s="126"/>
+      <c r="P82" s="126"/>
+      <c r="Q82" s="126"/>
+    </row>
+    <row r="83" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B83" s="144"/>
+      <c r="C83" s="145"/>
+      <c r="D83" s="145"/>
+      <c r="E83" s="145"/>
+      <c r="F83" s="145"/>
+      <c r="G83" s="145"/>
+      <c r="H83" s="145"/>
+      <c r="I83" s="145"/>
+      <c r="J83" s="145"/>
+      <c r="K83" s="146"/>
+      <c r="L83" s="127"/>
+      <c r="M83" s="127"/>
+      <c r="N83" s="127"/>
+      <c r="O83" s="126"/>
+      <c r="P83" s="126"/>
+      <c r="Q83" s="126"/>
+    </row>
+    <row r="84" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B84" s="144"/>
+      <c r="C84" s="145"/>
+      <c r="D84" s="145"/>
+      <c r="E84" s="145"/>
+      <c r="F84" s="145"/>
+      <c r="G84" s="145"/>
+      <c r="H84" s="145"/>
+      <c r="I84" s="145"/>
+      <c r="J84" s="145"/>
+      <c r="K84" s="146"/>
+      <c r="L84" s="127"/>
+      <c r="M84" s="127"/>
+      <c r="N84" s="127"/>
+      <c r="O84" s="126"/>
+      <c r="P84" s="126"/>
+      <c r="Q84" s="126"/>
+    </row>
+    <row r="85" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B85" s="144"/>
+      <c r="C85" s="145"/>
+      <c r="D85" s="145"/>
+      <c r="E85" s="145"/>
+      <c r="F85" s="145"/>
+      <c r="G85" s="145"/>
+      <c r="H85" s="145"/>
+      <c r="I85" s="145"/>
+      <c r="J85" s="145"/>
+      <c r="K85" s="146"/>
+      <c r="L85" s="127"/>
+      <c r="M85" s="127"/>
+      <c r="N85" s="127"/>
+      <c r="O85" s="126"/>
+      <c r="P85" s="126"/>
+      <c r="Q85" s="126"/>
+    </row>
+    <row r="86" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B86" s="144"/>
+      <c r="C86" s="145"/>
+      <c r="D86" s="145"/>
+      <c r="E86" s="145"/>
+      <c r="F86" s="145"/>
+      <c r="G86" s="145"/>
+      <c r="H86" s="145"/>
+      <c r="I86" s="145"/>
+      <c r="J86" s="145"/>
+      <c r="K86" s="146"/>
+      <c r="L86" s="127">
+        <v>3</v>
+      </c>
+      <c r="M86" s="127" t="s">
         <v>193</v>
       </c>
-      <c r="N74" s="127"/>
-      <c r="O74" s="132" t="s">
-        <v>173</v>
-      </c>
-      <c r="P74" s="132"/>
-      <c r="Q74" s="133"/>
-    </row>
-    <row r="75" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B75" s="134"/>
-      <c r="C75" s="135"/>
-      <c r="D75" s="135"/>
-      <c r="E75" s="135"/>
-      <c r="F75" s="135"/>
-      <c r="G75" s="135"/>
-      <c r="H75" s="135"/>
-      <c r="I75" s="135"/>
-      <c r="J75" s="135"/>
-      <c r="K75" s="136"/>
-      <c r="L75" s="143">
-        <v>1</v>
-      </c>
-      <c r="M75" s="143" t="s">
-        <v>211</v>
-      </c>
-      <c r="N75" s="143"/>
-      <c r="O75" s="173" t="s">
-        <v>214</v>
-      </c>
-      <c r="P75" s="173"/>
-      <c r="Q75" s="173"/>
-    </row>
-    <row r="76" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B76" s="137"/>
-      <c r="C76" s="138"/>
-      <c r="D76" s="138"/>
-      <c r="E76" s="138"/>
-      <c r="F76" s="138"/>
-      <c r="G76" s="138"/>
-      <c r="H76" s="138"/>
-      <c r="I76" s="138"/>
-      <c r="J76" s="138"/>
-      <c r="K76" s="139"/>
-      <c r="L76" s="143"/>
-      <c r="M76" s="143"/>
-      <c r="N76" s="143"/>
-      <c r="O76" s="173"/>
-      <c r="P76" s="173"/>
-      <c r="Q76" s="173"/>
-    </row>
-    <row r="77" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B77" s="137"/>
-      <c r="C77" s="138"/>
-      <c r="D77" s="138"/>
-      <c r="E77" s="138"/>
-      <c r="F77" s="138"/>
-      <c r="G77" s="138"/>
-      <c r="H77" s="138"/>
-      <c r="I77" s="138"/>
-      <c r="J77" s="138"/>
-      <c r="K77" s="139"/>
-      <c r="L77" s="143"/>
-      <c r="M77" s="143"/>
-      <c r="N77" s="143"/>
-      <c r="O77" s="173"/>
-      <c r="P77" s="173"/>
-      <c r="Q77" s="173"/>
-    </row>
-    <row r="78" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B78" s="137"/>
-      <c r="C78" s="138"/>
-      <c r="D78" s="138"/>
-      <c r="E78" s="138"/>
-      <c r="F78" s="138"/>
-      <c r="G78" s="138"/>
-      <c r="H78" s="138"/>
-      <c r="I78" s="138"/>
-      <c r="J78" s="138"/>
-      <c r="K78" s="139"/>
-      <c r="L78" s="143"/>
-      <c r="M78" s="143"/>
-      <c r="N78" s="143"/>
-      <c r="O78" s="173"/>
-      <c r="P78" s="173"/>
-      <c r="Q78" s="173"/>
-    </row>
-    <row r="79" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B79" s="137"/>
-      <c r="C79" s="138"/>
-      <c r="D79" s="138"/>
-      <c r="E79" s="138"/>
-      <c r="F79" s="138"/>
-      <c r="G79" s="138"/>
-      <c r="H79" s="138"/>
-      <c r="I79" s="138"/>
-      <c r="J79" s="138"/>
-      <c r="K79" s="139"/>
-      <c r="L79" s="143"/>
-      <c r="M79" s="143"/>
-      <c r="N79" s="143"/>
-      <c r="O79" s="173"/>
-      <c r="P79" s="173"/>
-      <c r="Q79" s="173"/>
-    </row>
-    <row r="80" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B80" s="137"/>
-      <c r="C80" s="138"/>
-      <c r="D80" s="138"/>
-      <c r="E80" s="138"/>
-      <c r="F80" s="138"/>
-      <c r="G80" s="138"/>
-      <c r="H80" s="138"/>
-      <c r="I80" s="138"/>
-      <c r="J80" s="138"/>
-      <c r="K80" s="139"/>
-      <c r="L80" s="143">
-        <v>2</v>
-      </c>
-      <c r="M80" s="143" t="s">
-        <v>212</v>
-      </c>
-      <c r="N80" s="143"/>
-      <c r="O80" s="173" t="s">
-        <v>213</v>
-      </c>
-      <c r="P80" s="173"/>
-      <c r="Q80" s="173"/>
-    </row>
-    <row r="81" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B81" s="137"/>
-      <c r="C81" s="138"/>
-      <c r="D81" s="138"/>
-      <c r="E81" s="138"/>
-      <c r="F81" s="138"/>
-      <c r="G81" s="138"/>
-      <c r="H81" s="138"/>
-      <c r="I81" s="138"/>
-      <c r="J81" s="138"/>
-      <c r="K81" s="139"/>
-      <c r="L81" s="143"/>
-      <c r="M81" s="143"/>
-      <c r="N81" s="143"/>
-      <c r="O81" s="173"/>
-      <c r="P81" s="173"/>
-      <c r="Q81" s="173"/>
-    </row>
-    <row r="82" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B82" s="137"/>
-      <c r="C82" s="138"/>
-      <c r="D82" s="138"/>
-      <c r="E82" s="138"/>
-      <c r="F82" s="138"/>
-      <c r="G82" s="138"/>
-      <c r="H82" s="138"/>
-      <c r="I82" s="138"/>
-      <c r="J82" s="138"/>
-      <c r="K82" s="139"/>
-      <c r="L82" s="143"/>
-      <c r="M82" s="143"/>
-      <c r="N82" s="143"/>
-      <c r="O82" s="173"/>
-      <c r="P82" s="173"/>
-      <c r="Q82" s="173"/>
-    </row>
-    <row r="83" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B83" s="137"/>
-      <c r="C83" s="138"/>
-      <c r="D83" s="138"/>
-      <c r="E83" s="138"/>
-      <c r="F83" s="138"/>
-      <c r="G83" s="138"/>
-      <c r="H83" s="138"/>
-      <c r="I83" s="138"/>
-      <c r="J83" s="138"/>
-      <c r="K83" s="139"/>
-      <c r="L83" s="143"/>
-      <c r="M83" s="143"/>
-      <c r="N83" s="143"/>
-      <c r="O83" s="173"/>
-      <c r="P83" s="173"/>
-      <c r="Q83" s="173"/>
-    </row>
-    <row r="84" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B84" s="137"/>
-      <c r="C84" s="138"/>
-      <c r="D84" s="138"/>
-      <c r="E84" s="138"/>
-      <c r="F84" s="138"/>
-      <c r="G84" s="138"/>
-      <c r="H84" s="138"/>
-      <c r="I84" s="138"/>
-      <c r="J84" s="138"/>
-      <c r="K84" s="139"/>
-      <c r="L84" s="143"/>
-      <c r="M84" s="143"/>
-      <c r="N84" s="143"/>
-      <c r="O84" s="173"/>
-      <c r="P84" s="173"/>
-      <c r="Q84" s="173"/>
-    </row>
-    <row r="85" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B85" s="137"/>
-      <c r="C85" s="138"/>
-      <c r="D85" s="138"/>
-      <c r="E85" s="138"/>
-      <c r="F85" s="138"/>
-      <c r="G85" s="138"/>
-      <c r="H85" s="138"/>
-      <c r="I85" s="138"/>
-      <c r="J85" s="138"/>
-      <c r="K85" s="139"/>
-      <c r="L85" s="143"/>
-      <c r="M85" s="143"/>
-      <c r="N85" s="143"/>
-      <c r="O85" s="173"/>
-      <c r="P85" s="173"/>
-      <c r="Q85" s="173"/>
-    </row>
-    <row r="86" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B86" s="137"/>
-      <c r="C86" s="138"/>
-      <c r="D86" s="138"/>
-      <c r="E86" s="138"/>
-      <c r="F86" s="138"/>
-      <c r="G86" s="138"/>
-      <c r="H86" s="138"/>
-      <c r="I86" s="138"/>
-      <c r="J86" s="138"/>
-      <c r="K86" s="139"/>
-      <c r="L86" s="143">
-        <v>3</v>
-      </c>
-      <c r="M86" s="143" t="s">
-        <v>194</v>
-      </c>
-      <c r="N86" s="143"/>
-      <c r="O86" s="173" t="s">
-        <v>220</v>
-      </c>
-      <c r="P86" s="173"/>
-      <c r="Q86" s="173"/>
+      <c r="N86" s="127"/>
+      <c r="O86" s="126" t="s">
+        <v>219</v>
+      </c>
+      <c r="P86" s="126"/>
+      <c r="Q86" s="126"/>
     </row>
     <row r="87" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B87" s="137"/>
-      <c r="C87" s="138"/>
-      <c r="D87" s="138"/>
-      <c r="E87" s="138"/>
-      <c r="F87" s="138"/>
-      <c r="G87" s="138"/>
-      <c r="H87" s="138"/>
-      <c r="I87" s="138"/>
-      <c r="J87" s="138"/>
-      <c r="K87" s="139"/>
-      <c r="L87" s="143"/>
-      <c r="M87" s="143"/>
-      <c r="N87" s="143"/>
-      <c r="O87" s="173"/>
-      <c r="P87" s="173"/>
-      <c r="Q87" s="173"/>
+      <c r="B87" s="144"/>
+      <c r="C87" s="145"/>
+      <c r="D87" s="145"/>
+      <c r="E87" s="145"/>
+      <c r="F87" s="145"/>
+      <c r="G87" s="145"/>
+      <c r="H87" s="145"/>
+      <c r="I87" s="145"/>
+      <c r="J87" s="145"/>
+      <c r="K87" s="146"/>
+      <c r="L87" s="127"/>
+      <c r="M87" s="127"/>
+      <c r="N87" s="127"/>
+      <c r="O87" s="126"/>
+      <c r="P87" s="126"/>
+      <c r="Q87" s="126"/>
     </row>
     <row r="88" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B88" s="137"/>
-      <c r="C88" s="138"/>
-      <c r="D88" s="138"/>
-      <c r="E88" s="138"/>
-      <c r="F88" s="138"/>
-      <c r="G88" s="138"/>
-      <c r="H88" s="138"/>
-      <c r="I88" s="138"/>
-      <c r="J88" s="138"/>
-      <c r="K88" s="139"/>
-      <c r="L88" s="143"/>
-      <c r="M88" s="143"/>
-      <c r="N88" s="143"/>
-      <c r="O88" s="173"/>
-      <c r="P88" s="173"/>
-      <c r="Q88" s="173"/>
+      <c r="B88" s="144"/>
+      <c r="C88" s="145"/>
+      <c r="D88" s="145"/>
+      <c r="E88" s="145"/>
+      <c r="F88" s="145"/>
+      <c r="G88" s="145"/>
+      <c r="H88" s="145"/>
+      <c r="I88" s="145"/>
+      <c r="J88" s="145"/>
+      <c r="K88" s="146"/>
+      <c r="L88" s="127"/>
+      <c r="M88" s="127"/>
+      <c r="N88" s="127"/>
+      <c r="O88" s="126"/>
+      <c r="P88" s="126"/>
+      <c r="Q88" s="126"/>
     </row>
     <row r="89" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B89" s="137"/>
-      <c r="C89" s="138"/>
-      <c r="D89" s="138"/>
-      <c r="E89" s="138"/>
-      <c r="F89" s="138"/>
-      <c r="G89" s="138"/>
-      <c r="H89" s="138"/>
-      <c r="I89" s="138"/>
-      <c r="J89" s="138"/>
-      <c r="K89" s="139"/>
-      <c r="L89" s="143"/>
-      <c r="M89" s="143"/>
-      <c r="N89" s="143"/>
-      <c r="O89" s="173"/>
-      <c r="P89" s="173"/>
-      <c r="Q89" s="173"/>
+      <c r="B89" s="144"/>
+      <c r="C89" s="145"/>
+      <c r="D89" s="145"/>
+      <c r="E89" s="145"/>
+      <c r="F89" s="145"/>
+      <c r="G89" s="145"/>
+      <c r="H89" s="145"/>
+      <c r="I89" s="145"/>
+      <c r="J89" s="145"/>
+      <c r="K89" s="146"/>
+      <c r="L89" s="127"/>
+      <c r="M89" s="127"/>
+      <c r="N89" s="127"/>
+      <c r="O89" s="126"/>
+      <c r="P89" s="126"/>
+      <c r="Q89" s="126"/>
     </row>
     <row r="90" spans="2:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B90" s="140"/>
-      <c r="C90" s="141"/>
-      <c r="D90" s="141"/>
-      <c r="E90" s="141"/>
-      <c r="F90" s="141"/>
-      <c r="G90" s="141"/>
-      <c r="H90" s="141"/>
-      <c r="I90" s="141"/>
-      <c r="J90" s="141"/>
-      <c r="K90" s="142"/>
-      <c r="L90" s="143"/>
-      <c r="M90" s="143"/>
-      <c r="N90" s="143"/>
-      <c r="O90" s="173"/>
-      <c r="P90" s="173"/>
-      <c r="Q90" s="173"/>
+      <c r="B90" s="147"/>
+      <c r="C90" s="148"/>
+      <c r="D90" s="148"/>
+      <c r="E90" s="148"/>
+      <c r="F90" s="148"/>
+      <c r="G90" s="148"/>
+      <c r="H90" s="148"/>
+      <c r="I90" s="148"/>
+      <c r="J90" s="148"/>
+      <c r="K90" s="149"/>
+      <c r="L90" s="127"/>
+      <c r="M90" s="127"/>
+      <c r="N90" s="127"/>
+      <c r="O90" s="126"/>
+      <c r="P90" s="126"/>
+      <c r="Q90" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="O75:Q79"/>
-    <mergeCell ref="O80:Q85"/>
-    <mergeCell ref="O86:Q90"/>
-    <mergeCell ref="M86:N90"/>
-    <mergeCell ref="M75:N79"/>
-    <mergeCell ref="M80:N85"/>
-    <mergeCell ref="L86:L90"/>
-    <mergeCell ref="L80:L85"/>
-    <mergeCell ref="L75:L79"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="G74:K74"/>
+    <mergeCell ref="M74:N74"/>
+    <mergeCell ref="O74:Q74"/>
+    <mergeCell ref="B75:K90"/>
+    <mergeCell ref="M39:N40"/>
+    <mergeCell ref="M56:N56"/>
+    <mergeCell ref="M57:N58"/>
+    <mergeCell ref="M59:N60"/>
+    <mergeCell ref="M61:N62"/>
+    <mergeCell ref="M63:N64"/>
+    <mergeCell ref="M29:N32"/>
+    <mergeCell ref="M25:N28"/>
+    <mergeCell ref="M21:N24"/>
+    <mergeCell ref="M53:N54"/>
+    <mergeCell ref="M51:N52"/>
+    <mergeCell ref="M49:N50"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="G56:K56"/>
+    <mergeCell ref="O56:Q56"/>
+    <mergeCell ref="B57:K72"/>
+    <mergeCell ref="L57:L58"/>
+    <mergeCell ref="O57:Q58"/>
+    <mergeCell ref="L59:L60"/>
+    <mergeCell ref="O59:Q60"/>
+    <mergeCell ref="L61:L62"/>
+    <mergeCell ref="L67:L69"/>
+    <mergeCell ref="L70:L72"/>
+    <mergeCell ref="O67:Q69"/>
+    <mergeCell ref="O70:Q72"/>
+    <mergeCell ref="M70:N72"/>
+    <mergeCell ref="M67:N69"/>
+    <mergeCell ref="O61:Q62"/>
+    <mergeCell ref="L63:L64"/>
+    <mergeCell ref="O63:Q64"/>
+    <mergeCell ref="L65:L66"/>
+    <mergeCell ref="O65:Q66"/>
+    <mergeCell ref="M65:N66"/>
+    <mergeCell ref="B39:K54"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="O3:Q4"/>
+    <mergeCell ref="O5:Q6"/>
+    <mergeCell ref="O7:Q8"/>
+    <mergeCell ref="O9:Q10"/>
+    <mergeCell ref="O11:Q12"/>
+    <mergeCell ref="O16:Q18"/>
+    <mergeCell ref="O13:Q15"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="M47:N48"/>
+    <mergeCell ref="M45:N46"/>
+    <mergeCell ref="M43:N44"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M16:N18"/>
+    <mergeCell ref="M13:N15"/>
+    <mergeCell ref="M11:N12"/>
+    <mergeCell ref="M9:N10"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="O53:Q54"/>
+    <mergeCell ref="O51:Q52"/>
+    <mergeCell ref="O49:Q50"/>
+    <mergeCell ref="O47:Q48"/>
+    <mergeCell ref="O45:Q46"/>
+    <mergeCell ref="O43:Q44"/>
+    <mergeCell ref="O41:Q42"/>
+    <mergeCell ref="O39:Q40"/>
+    <mergeCell ref="M41:N42"/>
+    <mergeCell ref="L53:L54"/>
+    <mergeCell ref="L51:L52"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="L43:L44"/>
     <mergeCell ref="O38:Q38"/>
     <mergeCell ref="B38:F38"/>
     <mergeCell ref="G38:K38"/>
@@ -10524,85 +10618,15 @@
     <mergeCell ref="O29:Q32"/>
     <mergeCell ref="O25:Q28"/>
     <mergeCell ref="O21:Q24"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="O53:Q54"/>
-    <mergeCell ref="O51:Q52"/>
-    <mergeCell ref="O49:Q50"/>
-    <mergeCell ref="O47:Q48"/>
-    <mergeCell ref="O45:Q46"/>
-    <mergeCell ref="O43:Q44"/>
-    <mergeCell ref="O41:Q42"/>
-    <mergeCell ref="O39:Q40"/>
-    <mergeCell ref="M41:N42"/>
-    <mergeCell ref="L53:L54"/>
-    <mergeCell ref="L51:L52"/>
-    <mergeCell ref="L49:L50"/>
-    <mergeCell ref="L47:L48"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="B39:K54"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="O3:Q4"/>
-    <mergeCell ref="O5:Q6"/>
-    <mergeCell ref="O7:Q8"/>
-    <mergeCell ref="O9:Q10"/>
-    <mergeCell ref="O11:Q12"/>
-    <mergeCell ref="O16:Q18"/>
-    <mergeCell ref="O13:Q15"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="M47:N48"/>
-    <mergeCell ref="M45:N46"/>
-    <mergeCell ref="M43:N44"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M16:N18"/>
-    <mergeCell ref="M13:N15"/>
-    <mergeCell ref="M11:N12"/>
-    <mergeCell ref="M9:N10"/>
-    <mergeCell ref="L59:L60"/>
-    <mergeCell ref="O59:Q60"/>
-    <mergeCell ref="L61:L62"/>
-    <mergeCell ref="L67:L69"/>
-    <mergeCell ref="L70:L72"/>
-    <mergeCell ref="O67:Q69"/>
-    <mergeCell ref="O70:Q72"/>
-    <mergeCell ref="M70:N72"/>
-    <mergeCell ref="M67:N69"/>
-    <mergeCell ref="O61:Q62"/>
-    <mergeCell ref="L63:L64"/>
-    <mergeCell ref="O63:Q64"/>
-    <mergeCell ref="L65:L66"/>
-    <mergeCell ref="O65:Q66"/>
-    <mergeCell ref="M65:N66"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="G74:K74"/>
-    <mergeCell ref="M74:N74"/>
-    <mergeCell ref="O74:Q74"/>
-    <mergeCell ref="B75:K90"/>
-    <mergeCell ref="M39:N40"/>
-    <mergeCell ref="M56:N56"/>
-    <mergeCell ref="M57:N58"/>
-    <mergeCell ref="M59:N60"/>
-    <mergeCell ref="M61:N62"/>
-    <mergeCell ref="M63:N64"/>
-    <mergeCell ref="M29:N32"/>
-    <mergeCell ref="M25:N28"/>
-    <mergeCell ref="M21:N24"/>
-    <mergeCell ref="M53:N54"/>
-    <mergeCell ref="M51:N52"/>
-    <mergeCell ref="M49:N50"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="G56:K56"/>
-    <mergeCell ref="O56:Q56"/>
-    <mergeCell ref="B57:K72"/>
-    <mergeCell ref="L57:L58"/>
-    <mergeCell ref="O57:Q58"/>
+    <mergeCell ref="O75:Q79"/>
+    <mergeCell ref="O80:Q85"/>
+    <mergeCell ref="O86:Q90"/>
+    <mergeCell ref="M86:N90"/>
+    <mergeCell ref="M75:N79"/>
+    <mergeCell ref="M80:N85"/>
+    <mergeCell ref="L86:L90"/>
+    <mergeCell ref="L80:L85"/>
+    <mergeCell ref="L75:L79"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>